<commit_message>
Arbeitsjournal geführt und Zeitplan geführt.
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="498" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1753D605-81FC-4568-8BEA-C75AFA157C64}"/>
+  <xr:revisionPtr revIDLastSave="593" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65BC3B4B-0AB8-4589-8B16-79013385A77A}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="45" windowWidth="26760" windowHeight="15420" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Aufwand (h)</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Steuerelemente relalisieren (Add,Delete,Alter,Open…)</t>
-  </si>
-  <si>
-    <t>Klassen PUCalc und PUCalcItem Realisieren nach UML</t>
   </si>
   <si>
     <t>Form für Einstellungen erstellen und Realisieren</t>
@@ -273,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -702,19 +699,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -955,14 +939,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
@@ -970,7 +1009,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -982,39 +1021,47 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1045,6 +1092,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1054,7 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1075,6 +1134,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1084,17 +1155,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1105,49 +1197,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1156,9 +1221,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1192,34 +1254,34 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1546,7 +1608,7 @@
   <dimension ref="A1:BN62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:C35"/>
+      <selection activeCell="D24" sqref="D24:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,171 +1620,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="101" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="104" t="s">
+      <c r="A1" s="114" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="105"/>
-      <c r="F1" s="106" t="s">
+      <c r="E1" s="118"/>
+      <c r="F1" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="98" t="s">
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="98" t="s">
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="98" t="s">
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="100"/>
-      <c r="Z1" s="98" t="s">
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="99"/>
-      <c r="AB1" s="99"/>
-      <c r="AC1" s="99"/>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="98" t="s">
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="113"/>
+      <c r="AE1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="99"/>
-      <c r="AG1" s="99"/>
-      <c r="AH1" s="99"/>
-      <c r="AI1" s="100"/>
-      <c r="AJ1" s="98" t="s">
+      <c r="AF1" s="112"/>
+      <c r="AG1" s="112"/>
+      <c r="AH1" s="112"/>
+      <c r="AI1" s="113"/>
+      <c r="AJ1" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="99"/>
-      <c r="AL1" s="99"/>
-      <c r="AM1" s="99"/>
-      <c r="AN1" s="100"/>
-      <c r="AO1" s="98" t="s">
+      <c r="AK1" s="112"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="112"/>
+      <c r="AN1" s="113"/>
+      <c r="AO1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="99"/>
-      <c r="AQ1" s="99"/>
-      <c r="AR1" s="99"/>
-      <c r="AS1" s="100"/>
-      <c r="AT1" s="98" t="s">
+      <c r="AP1" s="112"/>
+      <c r="AQ1" s="112"/>
+      <c r="AR1" s="112"/>
+      <c r="AS1" s="113"/>
+      <c r="AT1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="99"/>
-      <c r="AV1" s="99"/>
-      <c r="AW1" s="99"/>
-      <c r="AX1" s="100"/>
-      <c r="AY1" s="98" t="s">
+      <c r="AU1" s="112"/>
+      <c r="AV1" s="112"/>
+      <c r="AW1" s="112"/>
+      <c r="AX1" s="113"/>
+      <c r="AY1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="99"/>
-      <c r="BA1" s="99"/>
-      <c r="BB1" s="99"/>
-      <c r="BC1" s="100"/>
-      <c r="BD1" s="62" t="s">
+      <c r="AZ1" s="112"/>
+      <c r="BA1" s="112"/>
+      <c r="BB1" s="112"/>
+      <c r="BC1" s="113"/>
+      <c r="BD1" s="70" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="102"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="109">
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="122">
         <v>44957</v>
       </c>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="95">
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="108">
         <v>44958</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="95">
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="108">
         <v>44959</v>
       </c>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="95">
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="108">
         <v>44960</v>
       </c>
-      <c r="V2" s="96"/>
-      <c r="W2" s="96"/>
-      <c r="X2" s="96"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="95">
+      <c r="V2" s="109"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="110"/>
+      <c r="Z2" s="108">
         <v>44964</v>
       </c>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="96"/>
-      <c r="AC2" s="96"/>
-      <c r="AD2" s="97"/>
-      <c r="AE2" s="95">
+      <c r="AA2" s="109"/>
+      <c r="AB2" s="109"/>
+      <c r="AC2" s="109"/>
+      <c r="AD2" s="110"/>
+      <c r="AE2" s="108">
         <v>44965</v>
       </c>
-      <c r="AF2" s="96"/>
-      <c r="AG2" s="96"/>
-      <c r="AH2" s="96"/>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="95">
+      <c r="AF2" s="109"/>
+      <c r="AG2" s="109"/>
+      <c r="AH2" s="109"/>
+      <c r="AI2" s="110"/>
+      <c r="AJ2" s="108">
         <v>44966</v>
       </c>
-      <c r="AK2" s="96"/>
-      <c r="AL2" s="96"/>
-      <c r="AM2" s="96"/>
-      <c r="AN2" s="97"/>
-      <c r="AO2" s="95">
+      <c r="AK2" s="109"/>
+      <c r="AL2" s="109"/>
+      <c r="AM2" s="109"/>
+      <c r="AN2" s="110"/>
+      <c r="AO2" s="108">
         <v>44967</v>
       </c>
-      <c r="AP2" s="96"/>
-      <c r="AQ2" s="96"/>
-      <c r="AR2" s="96"/>
-      <c r="AS2" s="97"/>
-      <c r="AT2" s="95">
+      <c r="AP2" s="109"/>
+      <c r="AQ2" s="109"/>
+      <c r="AR2" s="109"/>
+      <c r="AS2" s="110"/>
+      <c r="AT2" s="108">
         <v>44971</v>
       </c>
-      <c r="AU2" s="96"/>
-      <c r="AV2" s="96"/>
-      <c r="AW2" s="96"/>
-      <c r="AX2" s="97"/>
-      <c r="AY2" s="95">
+      <c r="AU2" s="109"/>
+      <c r="AV2" s="109"/>
+      <c r="AW2" s="109"/>
+      <c r="AX2" s="110"/>
+      <c r="AY2" s="108">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="96"/>
-      <c r="BA2" s="96"/>
-      <c r="BB2" s="96"/>
-      <c r="BC2" s="97"/>
-      <c r="BD2" s="62"/>
+      <c r="AZ2" s="109"/>
+      <c r="BA2" s="109"/>
+      <c r="BB2" s="109"/>
+      <c r="BC2" s="110"/>
+      <c r="BD2" s="70"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="103"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1879,18 +1941,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="59"/>
+      <c r="BD3" s="67"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="53">
+      <c r="B4" s="104"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="61">
         <v>30</v>
       </c>
-      <c r="E4" s="91"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1901,7 +1963,7 @@
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="50"/>
+      <c r="P4" s="46"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
@@ -1939,33 +2001,33 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="87" t="s">
+      <c r="BB4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="59"/>
+      <c r="BC4" s="100"/>
+      <c r="BD4" s="67"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="4"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="4"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="47"/>
       <c r="U5" s="8"/>
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
@@ -1999,24 +2061,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="87"/>
-      <c r="BC5" s="88"/>
-      <c r="BD5" s="59"/>
-      <c r="BF5" s="112" t="s">
-        <v>41</v>
-      </c>
-      <c r="BG5" s="116"/>
+      <c r="BB5" s="99"/>
+      <c r="BC5" s="100"/>
+      <c r="BD5" s="67"/>
+      <c r="BF5" s="125" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG5" s="129"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="57">
+      <c r="B6" s="80"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="65">
         <v>1</v>
       </c>
-      <c r="E6" s="93">
+      <c r="E6" s="106">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2026,9 +2088,9 @@
       <c r="J6" s="4"/>
       <c r="K6" s="8"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="48"/>
+      <c r="M6" s="44"/>
       <c r="N6" s="23"/>
-      <c r="O6" s="49"/>
+      <c r="O6" s="45"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
@@ -2067,18 +2129,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="87"/>
-      <c r="BC6" s="88"/>
-      <c r="BD6" s="59"/>
-      <c r="BF6" s="113"/>
-      <c r="BG6" s="117"/>
+      <c r="BB6" s="99"/>
+      <c r="BC6" s="100"/>
+      <c r="BD6" s="67"/>
+      <c r="BF6" s="126"/>
+      <c r="BG6" s="130"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="94"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="107"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2086,7 +2148,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="41"/>
+      <c r="M7" s="38"/>
       <c r="N7" s="11"/>
       <c r="O7" s="12"/>
       <c r="P7" s="10"/>
@@ -2127,25 +2189,25 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="87"/>
-      <c r="BC7" s="88"/>
-      <c r="BD7" s="59"/>
-      <c r="BF7" s="112" t="s">
-        <v>42</v>
-      </c>
-      <c r="BG7" s="118"/>
+      <c r="BB7" s="99"/>
+      <c r="BC7" s="100"/>
+      <c r="BD7" s="67"/>
+      <c r="BF7" s="125" t="s">
+        <v>41</v>
+      </c>
+      <c r="BG7" s="131"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="53">
+      <c r="B8" s="104"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="61">
         <v>1.5</v>
       </c>
-      <c r="E8" s="55">
-        <v>0.5</v>
+      <c r="E8" s="63">
+        <v>0.8</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="6"/>
@@ -2195,31 +2257,31 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="87"/>
-      <c r="BC8" s="88"/>
-      <c r="BD8" s="62" t="s">
+      <c r="BB8" s="99"/>
+      <c r="BC8" s="100"/>
+      <c r="BD8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="113"/>
-      <c r="BG8" s="119"/>
+      <c r="BF8" s="126"/>
+      <c r="BG8" s="132"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="70"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="29"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="39"/>
+      <c r="K9" s="36"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="8"/>
+      <c r="P9" s="36"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
@@ -2257,25 +2319,25 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="87"/>
-      <c r="BC9" s="88"/>
-      <c r="BD9" s="62"/>
-      <c r="BF9" s="114" t="s">
+      <c r="BB9" s="99"/>
+      <c r="BC9" s="100"/>
+      <c r="BD9" s="70"/>
+      <c r="BF9" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="120"/>
+      <c r="BG9" s="133"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="57">
+      <c r="B10" s="80"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="65">
         <v>1.5</v>
       </c>
-      <c r="E10" s="58">
-        <v>0.5</v>
+      <c r="E10" s="66">
+        <v>0.8</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
@@ -2325,29 +2387,29 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="87"/>
-      <c r="BC10" s="88"/>
-      <c r="BD10" s="62"/>
-      <c r="BF10" s="115"/>
-      <c r="BG10" s="121"/>
+      <c r="BB10" s="99"/>
+      <c r="BC10" s="100"/>
+      <c r="BD10" s="70"/>
+      <c r="BF10" s="128"/>
+      <c r="BG10" s="134"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="30"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
-      <c r="K11" s="40"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="10"/>
+      <c r="P11" s="37"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
@@ -2385,20 +2447,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="87"/>
-      <c r="BC11" s="88"/>
-      <c r="BD11" s="62"/>
+      <c r="BB11" s="99"/>
+      <c r="BC11" s="100"/>
+      <c r="BD11" s="70"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="53">
+      <c r="B12" s="104"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="61">
         <v>1</v>
       </c>
-      <c r="E12" s="55">
+      <c r="E12" s="63">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2449,9 +2511,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="87"/>
-      <c r="BC12" s="88"/>
-      <c r="BD12" s="62" t="s">
+      <c r="BB12" s="99"/>
+      <c r="BC12" s="100"/>
+      <c r="BD12" s="70" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2465,13 +2527,13 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="21"/>
@@ -2518,9 +2580,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="87"/>
-      <c r="BC13" s="88"/>
-      <c r="BD13" s="62"/>
+      <c r="BB13" s="99"/>
+      <c r="BC13" s="100"/>
+      <c r="BD13" s="70"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2532,15 +2594,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="57">
+      <c r="A14" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="80"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="65">
         <v>2</v>
       </c>
-      <c r="E14" s="58">
+      <c r="E14" s="66">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2554,9 +2616,9 @@
       <c r="N14" s="9"/>
       <c r="O14" s="4"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="52"/>
+      <c r="Q14" s="48"/>
       <c r="R14" s="9"/>
-      <c r="S14" s="47"/>
+      <c r="S14" s="43"/>
       <c r="T14" s="4"/>
       <c r="U14" s="8"/>
       <c r="V14" s="9"/>
@@ -2591,19 +2653,19 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="87"/>
-      <c r="BC14" s="88"/>
-      <c r="BD14" s="62"/>
+      <c r="BB14" s="99"/>
+      <c r="BC14" s="100"/>
+      <c r="BD14" s="70"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="70"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="9"/>
       <c r="J15" s="21"/>
       <c r="K15" s="8"/>
@@ -2649,20 +2711,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="87"/>
-      <c r="BC15" s="88"/>
-      <c r="BD15" s="62"/>
+      <c r="BB15" s="99"/>
+      <c r="BC15" s="100"/>
+      <c r="BD15" s="70"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="57">
+      <c r="B16" s="80"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="65">
         <v>1</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="66">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2713,22 +2775,22 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="87"/>
-      <c r="BC16" s="88"/>
-      <c r="BD16" s="62"/>
+      <c r="BB16" s="99"/>
+      <c r="BC16" s="100"/>
+      <c r="BD16" s="70"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="70"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="33"/>
+      <c r="H17" s="30"/>
       <c r="I17" s="24"/>
       <c r="J17" s="21"/>
-      <c r="K17" s="39"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -2771,23 +2833,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="87"/>
-      <c r="BC17" s="88"/>
-      <c r="BD17" s="62"/>
+      <c r="BB17" s="99"/>
+      <c r="BC17" s="100"/>
+      <c r="BD17" s="70"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="57">
+      <c r="B18" s="80"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="65">
         <v>2</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E18" s="66">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2838,20 +2900,20 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="87"/>
-      <c r="BC18" s="88"/>
-      <c r="BD18" s="62"/>
+      <c r="BB18" s="99"/>
+      <c r="BC18" s="100"/>
+      <c r="BD18" s="70"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="70"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="61"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="4"/>
       <c r="K19" s="8"/>
       <c r="L19" s="9"/>
@@ -2896,20 +2958,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="87"/>
-      <c r="BC19" s="88"/>
-      <c r="BD19" s="62"/>
+      <c r="BB19" s="99"/>
+      <c r="BC19" s="100"/>
+      <c r="BD19" s="70"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="57">
+      <c r="B20" s="80"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="65">
         <v>1</v>
       </c>
-      <c r="E20" s="58">
+      <c r="E20" s="66">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -2960,23 +3022,23 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="87"/>
-      <c r="BC20" s="88"/>
-      <c r="BD20" s="62"/>
+      <c r="BB20" s="99"/>
+      <c r="BC20" s="100"/>
+      <c r="BD20" s="70"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="73"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="56"/>
+      <c r="A21" s="89"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="43"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="40"/>
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
       <c r="O21" s="12"/>
@@ -3018,29 +3080,29 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="87"/>
-      <c r="BC21" s="88"/>
-      <c r="BD21" s="62"/>
+      <c r="BB21" s="99"/>
+      <c r="BC21" s="100"/>
+      <c r="BD21" s="70"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="53">
+      <c r="B22" s="104"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="61">
         <v>0.5</v>
       </c>
-      <c r="E22" s="55">
+      <c r="E22" s="63">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="7"/>
@@ -3082,25 +3144,25 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="87"/>
-      <c r="BC22" s="88"/>
-      <c r="BD22" s="62" t="s">
+      <c r="BB22" s="99"/>
+      <c r="BC22" s="100"/>
+      <c r="BD22" s="70" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="73"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="56"/>
+      <c r="A23" s="89"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="64"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="41"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
       <c r="O23" s="12"/>
@@ -3142,20 +3204,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="87"/>
-      <c r="BC23" s="88"/>
-      <c r="BD23" s="62"/>
+      <c r="BB23" s="99"/>
+      <c r="BC23" s="100"/>
+      <c r="BD23" s="70"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80" t="s">
+      <c r="A24" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="53">
+      <c r="B24" s="104"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="61">
         <v>2</v>
       </c>
-      <c r="E24" s="55">
+      <c r="E24" s="63">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3206,25 +3268,25 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="87"/>
-      <c r="BC24" s="88"/>
-      <c r="BD24" s="62" t="s">
+      <c r="BB24" s="99"/>
+      <c r="BC24" s="100"/>
+      <c r="BD24" s="70" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="4"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="33"/>
+      <c r="L25" s="30"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="4"/>
@@ -3266,20 +3328,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="87"/>
-      <c r="BC25" s="88"/>
-      <c r="BD25" s="62"/>
+      <c r="BB25" s="99"/>
+      <c r="BC25" s="100"/>
+      <c r="BD25" s="70"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="57">
+      <c r="A26" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="80"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="58">
+      <c r="E26" s="66">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3330,23 +3392,23 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="87"/>
-      <c r="BC26" s="88"/>
-      <c r="BD26" s="62"/>
+      <c r="BB26" s="99"/>
+      <c r="BC26" s="100"/>
+      <c r="BD26" s="70"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="70"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="4"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="33"/>
+      <c r="L27" s="30"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
       <c r="O27" s="4"/>
@@ -3388,20 +3450,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="87"/>
-      <c r="BC27" s="88"/>
-      <c r="BD27" s="62"/>
+      <c r="BB27" s="99"/>
+      <c r="BC27" s="100"/>
+      <c r="BD27" s="70"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="57">
+      <c r="A28" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="80"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="65">
         <v>2</v>
       </c>
-      <c r="E28" s="58">
+      <c r="E28" s="66">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3452,16 +3514,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="87"/>
-      <c r="BC28" s="88"/>
-      <c r="BD28" s="62"/>
+      <c r="BB28" s="99"/>
+      <c r="BC28" s="100"/>
+      <c r="BD28" s="70"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="70"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="61"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3469,8 +3531,8 @@
       <c r="J29" s="4"/>
       <c r="K29" s="8"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
       <c r="O29" s="4"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="9"/>
@@ -3510,20 +3572,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="87"/>
-      <c r="BC29" s="88"/>
-      <c r="BD29" s="62"/>
+      <c r="BB29" s="99"/>
+      <c r="BC29" s="100"/>
+      <c r="BD29" s="70"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="57">
+      <c r="A30" s="79" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="80"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="65">
         <v>2</v>
       </c>
-      <c r="E30" s="58">
+      <c r="E30" s="66">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3535,7 +3597,7 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="18"/>
-      <c r="O30" s="35"/>
+      <c r="O30" s="32"/>
       <c r="P30" s="25"/>
       <c r="Q30" s="24"/>
       <c r="R30" s="9"/>
@@ -3574,16 +3636,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="87"/>
-      <c r="BC30" s="88"/>
-      <c r="BD30" s="62"/>
+      <c r="BB30" s="99"/>
+      <c r="BC30" s="100"/>
+      <c r="BD30" s="70"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="70"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="61"/>
+      <c r="A31" s="82"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3592,9 +3654,9 @@
       <c r="K31" s="8"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="33"/>
+      <c r="N31" s="30"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="39"/>
+      <c r="P31" s="36"/>
       <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
@@ -3632,20 +3694,22 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="87"/>
-      <c r="BC31" s="88"/>
-      <c r="BD31" s="62"/>
+      <c r="BB31" s="99"/>
+      <c r="BC31" s="100"/>
+      <c r="BD31" s="70"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="68"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="57">
+      <c r="B32" s="80"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="65">
         <v>4</v>
       </c>
-      <c r="E32" s="58"/>
+      <c r="E32" s="66">
+        <v>4</v>
+      </c>
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -3694,16 +3758,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="87"/>
-      <c r="BC32" s="88"/>
-      <c r="BD32" s="62"/>
+      <c r="BB32" s="99"/>
+      <c r="BC32" s="100"/>
+      <c r="BD32" s="70"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="61"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3715,8 +3779,8 @@
       <c r="N33" s="9"/>
       <c r="O33" s="4"/>
       <c r="P33" s="8"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
       <c r="S33" s="9"/>
       <c r="T33" s="4"/>
       <c r="U33" s="8"/>
@@ -3752,20 +3816,22 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="87"/>
-      <c r="BC33" s="88"/>
-      <c r="BD33" s="62"/>
+      <c r="BB33" s="99"/>
+      <c r="BC33" s="100"/>
+      <c r="BD33" s="70"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="57">
+      <c r="B34" s="80"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="65">
         <v>3</v>
       </c>
-      <c r="E34" s="58"/>
+      <c r="E34" s="66">
+        <v>2</v>
+      </c>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -3814,16 +3880,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="87"/>
-      <c r="BC34" s="88"/>
-      <c r="BD34" s="62"/>
+      <c r="BB34" s="99"/>
+      <c r="BC34" s="100"/>
+      <c r="BD34" s="70"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="70"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="61"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="69"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3837,8 +3903,8 @@
       <c r="P35" s="8"/>
       <c r="Q35" s="9"/>
       <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="4"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="32"/>
       <c r="U35" s="8"/>
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
@@ -3872,20 +3938,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="87"/>
-      <c r="BC35" s="88"/>
-      <c r="BD35" s="62"/>
+      <c r="BB35" s="99"/>
+      <c r="BC35" s="100"/>
+      <c r="BD35" s="70"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="68"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="57">
+      <c r="A36" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="65">
         <v>4</v>
       </c>
-      <c r="E36" s="58"/>
+      <c r="E36" s="66"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -3900,8 +3966,8 @@
       <c r="Q36" s="9"/>
       <c r="R36" s="9"/>
       <c r="S36" s="24"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="36"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="33"/>
       <c r="V36" s="18"/>
       <c r="W36" s="18"/>
       <c r="Y36" s="4"/>
@@ -3933,16 +3999,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="87"/>
-      <c r="BC36" s="88"/>
-      <c r="BD36" s="62"/>
+      <c r="BB36" s="99"/>
+      <c r="BC36" s="100"/>
+      <c r="BD36" s="70"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="70"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="61"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="69"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -3991,20 +4057,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="87"/>
-      <c r="BC37" s="88"/>
-      <c r="BD37" s="62"/>
+      <c r="BB37" s="99"/>
+      <c r="BC37" s="100"/>
+      <c r="BD37" s="70"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="68"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="57">
+      <c r="B38" s="80"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="65">
         <v>1</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="66"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -4052,16 +4118,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="87"/>
-      <c r="BC38" s="88"/>
-      <c r="BD38" s="62"/>
+      <c r="BB38" s="99"/>
+      <c r="BC38" s="100"/>
+      <c r="BD38" s="70"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="70"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
+      <c r="A39" s="82"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4110,20 +4176,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="87"/>
-      <c r="BC39" s="88"/>
-      <c r="BD39" s="62"/>
+      <c r="BB39" s="99"/>
+      <c r="BC39" s="100"/>
+      <c r="BD39" s="70"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="68"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="57">
+      <c r="B40" s="80"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="65">
         <v>1</v>
       </c>
-      <c r="E40" s="58"/>
+      <c r="E40" s="66"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -4144,7 +4210,7 @@
       <c r="W40" s="9"/>
       <c r="X40" s="18"/>
       <c r="Y40" s="4"/>
-      <c r="AA40" s="44"/>
+      <c r="AA40" s="41"/>
       <c r="AB40" s="9" t="s">
         <v>18</v>
       </c>
@@ -4173,16 +4239,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="87"/>
-      <c r="BC40" s="88"/>
-      <c r="BD40" s="62"/>
+      <c r="BB40" s="99"/>
+      <c r="BC40" s="100"/>
+      <c r="BD40" s="70"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="70"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
+      <c r="A41" s="82"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4231,20 +4297,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="87"/>
-      <c r="BC41" s="88"/>
-      <c r="BD41" s="62"/>
+      <c r="BB41" s="99"/>
+      <c r="BC41" s="100"/>
+      <c r="BD41" s="70"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="68"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="57">
+      <c r="B42" s="80"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="65">
         <v>2</v>
       </c>
-      <c r="E42" s="58"/>
+      <c r="E42" s="66"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -4267,6 +4333,7 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="18"/>
       <c r="AA42" s="18"/>
+      <c r="AB42" s="18"/>
       <c r="AC42" s="9"/>
       <c r="AD42" s="4"/>
       <c r="AE42" s="8"/>
@@ -4292,16 +4359,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="87"/>
-      <c r="BC42" s="88"/>
-      <c r="BD42" s="62"/>
+      <c r="BB42" s="99"/>
+      <c r="BC42" s="100"/>
+      <c r="BD42" s="70"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="70"/>
-      <c r="B43" s="71"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
+      <c r="A43" s="82"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4350,20 +4417,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="87"/>
-      <c r="BC43" s="88"/>
-      <c r="BD43" s="62"/>
+      <c r="BB43" s="99"/>
+      <c r="BC43" s="100"/>
+      <c r="BD43" s="70"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="57">
+      <c r="B44" s="80"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="65">
         <v>2</v>
       </c>
-      <c r="E44" s="58"/>
+      <c r="E44" s="66"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4385,8 +4452,9 @@
       <c r="X44" s="24"/>
       <c r="Y44" s="4"/>
       <c r="Z44" s="8"/>
-      <c r="AA44" s="18"/>
+      <c r="AA44" s="42"/>
       <c r="AB44" s="18"/>
+      <c r="AC44" s="54"/>
       <c r="AD44" s="4"/>
       <c r="AE44" s="8"/>
       <c r="AF44" s="9"/>
@@ -4411,737 +4479,730 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="87"/>
-      <c r="BC44" s="88"/>
-      <c r="BD44" s="62"/>
+      <c r="BB44" s="99"/>
+      <c r="BC44" s="100"/>
+      <c r="BD44" s="70"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="70"/>
-      <c r="B45" s="71"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="9"/>
-      <c r="W45" s="9"/>
-      <c r="X45" s="9"/>
-      <c r="Y45" s="4"/>
-      <c r="Z45" s="8"/>
-      <c r="AA45" s="9"/>
-      <c r="AB45" s="9"/>
-      <c r="AC45" s="9"/>
-      <c r="AD45" s="4"/>
-      <c r="AE45" s="8"/>
-      <c r="AF45" s="9"/>
-      <c r="AG45" s="9"/>
-      <c r="AH45" s="9"/>
-      <c r="AI45" s="4"/>
-      <c r="AJ45" s="8"/>
-      <c r="AK45" s="9"/>
-      <c r="AL45" s="9"/>
-      <c r="AM45" s="9"/>
-      <c r="AN45" s="4"/>
-      <c r="AO45" s="8"/>
-      <c r="AP45" s="9"/>
-      <c r="AQ45" s="9"/>
-      <c r="AR45" s="9"/>
-      <c r="AS45" s="4"/>
-      <c r="AT45" s="8"/>
-      <c r="AU45" s="9"/>
-      <c r="AV45" s="9"/>
-      <c r="AW45" s="9"/>
-      <c r="AX45" s="4"/>
-      <c r="AY45" s="8"/>
-      <c r="AZ45" s="9"/>
-      <c r="BA45" s="9"/>
-      <c r="BB45" s="87"/>
-      <c r="BC45" s="88"/>
-      <c r="BD45" s="62"/>
+      <c r="A45" s="89"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="11"/>
+      <c r="AC45" s="11"/>
+      <c r="AD45" s="12"/>
+      <c r="AE45" s="10"/>
+      <c r="AF45" s="11"/>
+      <c r="AG45" s="11"/>
+      <c r="AH45" s="11"/>
+      <c r="AI45" s="12"/>
+      <c r="AJ45" s="10"/>
+      <c r="AK45" s="11"/>
+      <c r="AL45" s="11"/>
+      <c r="AM45" s="11"/>
+      <c r="AN45" s="12"/>
+      <c r="AO45" s="10"/>
+      <c r="AP45" s="11"/>
+      <c r="AQ45" s="11"/>
+      <c r="AR45" s="11"/>
+      <c r="AS45" s="12"/>
+      <c r="AT45" s="10"/>
+      <c r="AU45" s="11"/>
+      <c r="AV45" s="11"/>
+      <c r="AW45" s="11"/>
+      <c r="AX45" s="12"/>
+      <c r="AY45" s="10"/>
+      <c r="AZ45" s="11"/>
+      <c r="BA45" s="11"/>
+      <c r="BB45" s="99"/>
+      <c r="BC45" s="100"/>
+      <c r="BD45" s="70"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="67" t="s">
+      <c r="A46" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="68"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="57">
+      <c r="B46" s="93"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="71">
+        <v>1</v>
+      </c>
+      <c r="E46" s="72"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="45"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="23"/>
+      <c r="S46" s="23"/>
+      <c r="T46" s="45"/>
+      <c r="U46" s="50"/>
+      <c r="V46" s="23"/>
+      <c r="W46" s="23"/>
+      <c r="X46" s="23"/>
+      <c r="Y46" s="52"/>
+      <c r="Z46" s="53"/>
+      <c r="AA46" s="23"/>
+      <c r="AB46" s="51"/>
+      <c r="AC46" s="56"/>
+      <c r="AD46" s="7"/>
+      <c r="AE46" s="44"/>
+      <c r="AG46" s="23"/>
+      <c r="AH46" s="23"/>
+      <c r="AI46" s="45"/>
+      <c r="AJ46" s="50"/>
+      <c r="AK46" s="23"/>
+      <c r="AL46" s="23"/>
+      <c r="AM46" s="23"/>
+      <c r="AN46" s="45"/>
+      <c r="AO46" s="50"/>
+      <c r="AP46" s="23"/>
+      <c r="AQ46" s="23"/>
+      <c r="AR46" s="23"/>
+      <c r="AS46" s="45"/>
+      <c r="AT46" s="50"/>
+      <c r="AU46" s="23"/>
+      <c r="AV46" s="23"/>
+      <c r="AW46" s="23"/>
+      <c r="AX46" s="45"/>
+      <c r="AY46" s="50"/>
+      <c r="AZ46" s="23"/>
+      <c r="BA46" s="23"/>
+      <c r="BB46" s="99"/>
+      <c r="BC46" s="100"/>
+      <c r="BD46" s="70"/>
+    </row>
+    <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="82"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="43"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="9"/>
+      <c r="AC47" s="43"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="43"/>
+      <c r="AF47" s="9"/>
+      <c r="AG47" s="9"/>
+      <c r="AH47" s="9"/>
+      <c r="AI47" s="4"/>
+      <c r="AJ47" s="8"/>
+      <c r="AK47" s="9"/>
+      <c r="AL47" s="9"/>
+      <c r="AM47" s="9"/>
+      <c r="AN47" s="4"/>
+      <c r="AO47" s="8"/>
+      <c r="AP47" s="9"/>
+      <c r="AQ47" s="9"/>
+      <c r="AR47" s="9"/>
+      <c r="AS47" s="4"/>
+      <c r="AT47" s="8"/>
+      <c r="AU47" s="9"/>
+      <c r="AV47" s="9"/>
+      <c r="AW47" s="9"/>
+      <c r="AX47" s="4"/>
+      <c r="AY47" s="8"/>
+      <c r="AZ47" s="9"/>
+      <c r="BA47" s="9"/>
+      <c r="BB47" s="99"/>
+      <c r="BC47" s="100"/>
+      <c r="BD47" s="70"/>
+    </row>
+    <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="80"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="65">
         <v>2</v>
       </c>
-      <c r="E46" s="58"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="4"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="35"/>
-      <c r="Z46" s="36"/>
-      <c r="AA46" s="9"/>
-      <c r="AB46" s="24"/>
-      <c r="AC46" s="28"/>
-      <c r="AD46" s="21"/>
-      <c r="AE46" s="45"/>
-      <c r="AG46" s="9"/>
-      <c r="AH46" s="9"/>
-      <c r="AI46" s="4"/>
-      <c r="AJ46" s="8"/>
-      <c r="AK46" s="9"/>
-      <c r="AL46" s="9"/>
-      <c r="AM46" s="9"/>
-      <c r="AN46" s="4"/>
-      <c r="AO46" s="8"/>
-      <c r="AP46" s="9"/>
-      <c r="AQ46" s="9"/>
-      <c r="AR46" s="9"/>
-      <c r="AS46" s="4"/>
-      <c r="AT46" s="8"/>
-      <c r="AU46" s="9"/>
-      <c r="AV46" s="9"/>
-      <c r="AW46" s="9"/>
-      <c r="AX46" s="4"/>
-      <c r="AY46" s="8"/>
-      <c r="AZ46" s="9"/>
-      <c r="BA46" s="9"/>
-      <c r="BB46" s="87"/>
-      <c r="BC46" s="88"/>
-      <c r="BD46" s="62"/>
-    </row>
-    <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="73"/>
-      <c r="B47" s="74"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="12"/>
-      <c r="U47" s="10"/>
-      <c r="V47" s="11"/>
-      <c r="W47" s="11"/>
-      <c r="X47" s="11"/>
-      <c r="Y47" s="12"/>
-      <c r="Z47" s="26"/>
-      <c r="AA47" s="11"/>
-      <c r="AB47" s="11"/>
-      <c r="AC47" s="26"/>
-      <c r="AD47" s="12"/>
-      <c r="AE47" s="10"/>
-      <c r="AF47" s="11"/>
-      <c r="AG47" s="11"/>
-      <c r="AH47" s="11"/>
-      <c r="AI47" s="12"/>
-      <c r="AJ47" s="10"/>
-      <c r="AK47" s="11"/>
-      <c r="AL47" s="11"/>
-      <c r="AM47" s="11"/>
-      <c r="AN47" s="12"/>
-      <c r="AO47" s="10"/>
-      <c r="AP47" s="11"/>
-      <c r="AQ47" s="11"/>
-      <c r="AR47" s="11"/>
-      <c r="AS47" s="12"/>
-      <c r="AT47" s="10"/>
-      <c r="AU47" s="11"/>
-      <c r="AV47" s="11"/>
-      <c r="AW47" s="11"/>
-      <c r="AX47" s="12"/>
-      <c r="AY47" s="10"/>
-      <c r="AZ47" s="11"/>
-      <c r="BA47" s="11"/>
-      <c r="BB47" s="87"/>
-      <c r="BC47" s="88"/>
-      <c r="BD47" s="62"/>
-    </row>
-    <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="80" t="s">
+      <c r="E48" s="66"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="45"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="23"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="45"/>
+      <c r="U48" s="50"/>
+      <c r="V48" s="23"/>
+      <c r="W48" s="23"/>
+      <c r="X48" s="23"/>
+      <c r="Y48" s="45"/>
+      <c r="Z48" s="50"/>
+      <c r="AA48" s="51"/>
+      <c r="AB48" s="23"/>
+      <c r="AC48" s="51"/>
+      <c r="AD48" s="45"/>
+      <c r="AE48" s="44"/>
+      <c r="AF48" s="55"/>
+      <c r="AG48" s="23"/>
+      <c r="AH48" s="23"/>
+      <c r="AI48" s="45"/>
+      <c r="AJ48" s="50"/>
+      <c r="AK48" s="23"/>
+      <c r="AL48" s="23"/>
+      <c r="AM48" s="23"/>
+      <c r="AN48" s="45"/>
+      <c r="AO48" s="50"/>
+      <c r="AP48" s="23"/>
+      <c r="AQ48" s="23"/>
+      <c r="AR48" s="23"/>
+      <c r="AS48" s="45"/>
+      <c r="AT48" s="50"/>
+      <c r="AU48" s="23"/>
+      <c r="AV48" s="23"/>
+      <c r="AW48" s="23"/>
+      <c r="AX48" s="45"/>
+      <c r="AY48" s="50"/>
+      <c r="AZ48" s="23"/>
+      <c r="BA48" s="23"/>
+      <c r="BB48" s="99"/>
+      <c r="BC48" s="100"/>
+      <c r="BD48" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="53">
-        <v>1</v>
-      </c>
-      <c r="E48" s="55"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="6"/>
-      <c r="T48" s="7"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="6"/>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6"/>
-      <c r="Y48" s="7"/>
-      <c r="Z48" s="5"/>
-      <c r="AA48" s="24"/>
-      <c r="AB48" s="6"/>
-      <c r="AC48" s="24"/>
-      <c r="AD48" s="7"/>
-      <c r="AE48" s="18"/>
-      <c r="AG48" s="6"/>
-      <c r="AH48" s="6"/>
-      <c r="AI48" s="7"/>
-      <c r="AJ48" s="5"/>
-      <c r="AK48" s="6"/>
-      <c r="AL48" s="6"/>
-      <c r="AM48" s="6"/>
-      <c r="AN48" s="7"/>
-      <c r="AO48" s="5"/>
-      <c r="AP48" s="6"/>
-      <c r="AQ48" s="6"/>
-      <c r="AR48" s="6"/>
-      <c r="AS48" s="7"/>
-      <c r="AT48" s="5"/>
-      <c r="AU48" s="6"/>
-      <c r="AV48" s="6"/>
-      <c r="AW48" s="6"/>
-      <c r="AX48" s="7"/>
-      <c r="AY48" s="5"/>
-      <c r="AZ48" s="6"/>
-      <c r="BA48" s="6"/>
-      <c r="BB48" s="87"/>
-      <c r="BC48" s="88"/>
-      <c r="BD48" s="62" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="70"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
-      <c r="X49" s="9"/>
-      <c r="Y49" s="4"/>
-      <c r="Z49" s="8"/>
-      <c r="AA49" s="9"/>
-      <c r="AB49" s="9"/>
-      <c r="AC49" s="9"/>
-      <c r="AD49" s="4"/>
-      <c r="AE49" s="8"/>
-      <c r="AF49" s="9"/>
-      <c r="AG49" s="9"/>
-      <c r="AH49" s="9"/>
-      <c r="AI49" s="4"/>
-      <c r="AJ49" s="8"/>
-      <c r="AK49" s="9"/>
-      <c r="AL49" s="9"/>
-      <c r="AM49" s="9"/>
-      <c r="AN49" s="4"/>
-      <c r="AO49" s="8"/>
-      <c r="AP49" s="9"/>
-      <c r="AQ49" s="9"/>
-      <c r="AR49" s="9"/>
-      <c r="AS49" s="4"/>
-      <c r="AT49" s="8"/>
-      <c r="AU49" s="9"/>
-      <c r="AV49" s="9"/>
-      <c r="AW49" s="9"/>
-      <c r="AX49" s="4"/>
-      <c r="AY49" s="8"/>
-      <c r="AZ49" s="9"/>
-      <c r="BA49" s="9"/>
-      <c r="BB49" s="87"/>
-      <c r="BC49" s="88"/>
-      <c r="BD49" s="62"/>
+      <c r="A49" s="89"/>
+      <c r="B49" s="90"/>
+      <c r="C49" s="91"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="10"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="12"/>
+      <c r="Z49" s="10"/>
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="11"/>
+      <c r="AC49" s="11"/>
+      <c r="AD49" s="12"/>
+      <c r="AE49" s="10"/>
+      <c r="AF49" s="11"/>
+      <c r="AG49" s="11"/>
+      <c r="AH49" s="11"/>
+      <c r="AI49" s="12"/>
+      <c r="AJ49" s="10"/>
+      <c r="AK49" s="11"/>
+      <c r="AL49" s="11"/>
+      <c r="AM49" s="11"/>
+      <c r="AN49" s="12"/>
+      <c r="AO49" s="10"/>
+      <c r="AP49" s="11"/>
+      <c r="AQ49" s="11"/>
+      <c r="AR49" s="11"/>
+      <c r="AS49" s="12"/>
+      <c r="AT49" s="10"/>
+      <c r="AU49" s="11"/>
+      <c r="AV49" s="11"/>
+      <c r="AW49" s="11"/>
+      <c r="AX49" s="12"/>
+      <c r="AY49" s="10"/>
+      <c r="AZ49" s="11"/>
+      <c r="BA49" s="11"/>
+      <c r="BB49" s="99"/>
+      <c r="BC49" s="100"/>
+      <c r="BD49" s="70"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="67" t="s">
+      <c r="A50" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="68"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="57">
+      <c r="B50" s="86"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="71">
+        <v>5</v>
+      </c>
+      <c r="E50" s="74"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="44"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="50"/>
+      <c r="V50" s="23"/>
+      <c r="W50" s="23"/>
+      <c r="X50" s="44"/>
+      <c r="Y50" s="45"/>
+      <c r="Z50" s="50"/>
+      <c r="AA50" s="23"/>
+      <c r="AB50" s="23"/>
+      <c r="AC50" s="44"/>
+      <c r="AD50" s="45"/>
+      <c r="AE50" s="50"/>
+      <c r="AF50" s="23"/>
+      <c r="AG50" s="23"/>
+      <c r="AH50" s="44"/>
+      <c r="AI50" s="45"/>
+      <c r="AJ50" s="50"/>
+      <c r="AK50" s="23"/>
+      <c r="AL50" s="23"/>
+      <c r="AM50" s="44"/>
+      <c r="AN50" s="45"/>
+      <c r="AO50" s="50"/>
+      <c r="AP50" s="23"/>
+      <c r="AQ50" s="23"/>
+      <c r="AR50" s="44"/>
+      <c r="AS50" s="45"/>
+      <c r="AT50" s="50"/>
+      <c r="AU50" s="23"/>
+      <c r="AV50" s="23"/>
+      <c r="AW50" s="44"/>
+      <c r="AX50" s="45"/>
+      <c r="AY50" s="50"/>
+      <c r="AZ50" s="23"/>
+      <c r="BA50" s="44"/>
+      <c r="BB50" s="99"/>
+      <c r="BC50" s="100"/>
+      <c r="BD50" s="70"/>
+    </row>
+    <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="87"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="48"/>
+      <c r="S51" s="30"/>
+      <c r="T51" s="21"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="48"/>
+      <c r="X51" s="42"/>
+      <c r="Y51" s="21"/>
+      <c r="Z51" s="8"/>
+      <c r="AA51" s="9"/>
+      <c r="AB51" s="48"/>
+      <c r="AC51" s="42"/>
+      <c r="AD51" s="21"/>
+      <c r="AE51" s="8"/>
+      <c r="AF51" s="9"/>
+      <c r="AG51" s="48"/>
+      <c r="AH51" s="42"/>
+      <c r="AI51" s="21"/>
+      <c r="AJ51" s="8"/>
+      <c r="AK51" s="9"/>
+      <c r="AL51" s="48"/>
+      <c r="AM51" s="42"/>
+      <c r="AN51" s="21"/>
+      <c r="AO51" s="8"/>
+      <c r="AP51" s="9"/>
+      <c r="AQ51" s="48"/>
+      <c r="AR51" s="42"/>
+      <c r="AS51" s="21"/>
+      <c r="AT51" s="8"/>
+      <c r="AU51" s="9"/>
+      <c r="AV51" s="48"/>
+      <c r="AW51" s="42"/>
+      <c r="AX51" s="21"/>
+      <c r="AY51" s="8"/>
+      <c r="AZ51" s="9"/>
+      <c r="BA51" s="48"/>
+      <c r="BB51" s="99"/>
+      <c r="BC51" s="100"/>
+      <c r="BD51" s="70"/>
+    </row>
+    <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="80"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E50" s="58"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="4"/>
-      <c r="Z50" s="8"/>
-      <c r="AA50" s="24"/>
-      <c r="AB50" s="36"/>
-      <c r="AC50" s="9"/>
-      <c r="AD50" s="4"/>
-      <c r="AE50" s="18"/>
-      <c r="AF50" s="27"/>
-      <c r="AH50" s="46"/>
-      <c r="AI50" s="4"/>
-      <c r="AJ50" s="8"/>
-      <c r="AK50" s="9"/>
-      <c r="AL50" s="9"/>
-      <c r="AM50" s="9"/>
-      <c r="AN50" s="4"/>
-      <c r="AO50" s="8"/>
-      <c r="AP50" s="9"/>
-      <c r="AQ50" s="9"/>
-      <c r="AR50" s="9"/>
-      <c r="AS50" s="4"/>
-      <c r="AT50" s="8"/>
-      <c r="AU50" s="9"/>
-      <c r="AV50" s="9"/>
-      <c r="AW50" s="9"/>
-      <c r="AX50" s="4"/>
-      <c r="AY50" s="8"/>
-      <c r="AZ50" s="9"/>
-      <c r="BA50" s="9"/>
-      <c r="BB50" s="87"/>
-      <c r="BC50" s="88"/>
-      <c r="BD50" s="62"/>
-    </row>
-    <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="73"/>
-      <c r="B51" s="74"/>
-      <c r="C51" s="75"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="12"/>
-      <c r="U51" s="10"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
-      <c r="X51" s="11"/>
-      <c r="Y51" s="12"/>
-      <c r="Z51" s="10"/>
-      <c r="AA51" s="11"/>
-      <c r="AB51" s="11"/>
-      <c r="AC51" s="11"/>
-      <c r="AD51" s="12"/>
-      <c r="AE51" s="10"/>
-      <c r="AF51" s="11"/>
-      <c r="AG51" s="11"/>
-      <c r="AH51" s="11"/>
-      <c r="AI51" s="12"/>
-      <c r="AJ51" s="10"/>
-      <c r="AK51" s="11"/>
-      <c r="AL51" s="11"/>
-      <c r="AM51" s="11"/>
-      <c r="AN51" s="12"/>
-      <c r="AO51" s="10"/>
-      <c r="AP51" s="11"/>
-      <c r="AQ51" s="11"/>
-      <c r="AR51" s="11"/>
-      <c r="AS51" s="12"/>
-      <c r="AT51" s="10"/>
-      <c r="AU51" s="11"/>
-      <c r="AV51" s="11"/>
-      <c r="AW51" s="11"/>
-      <c r="AX51" s="12"/>
-      <c r="AY51" s="10"/>
-      <c r="AZ51" s="11"/>
-      <c r="BA51" s="11"/>
-      <c r="BB51" s="87"/>
-      <c r="BC51" s="88"/>
-      <c r="BD51" s="62"/>
-    </row>
-    <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="76" t="s">
+      <c r="E52" s="66"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="23"/>
+      <c r="M52" s="23"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="23"/>
+      <c r="R52" s="23"/>
+      <c r="T52" s="51"/>
+      <c r="U52" s="50"/>
+      <c r="V52" s="23"/>
+      <c r="W52" s="23"/>
+      <c r="Y52" s="51"/>
+      <c r="Z52" s="50"/>
+      <c r="AA52" s="23"/>
+      <c r="AB52" s="23"/>
+      <c r="AD52" s="51"/>
+      <c r="AE52" s="50"/>
+      <c r="AF52" s="23"/>
+      <c r="AG52" s="23"/>
+      <c r="AI52" s="51"/>
+      <c r="AJ52" s="50"/>
+      <c r="AK52" s="23"/>
+      <c r="AL52" s="23"/>
+      <c r="AN52" s="51"/>
+      <c r="AO52" s="50"/>
+      <c r="AP52" s="23"/>
+      <c r="AQ52" s="23"/>
+      <c r="AS52" s="51"/>
+      <c r="AT52" s="50"/>
+      <c r="AU52" s="23"/>
+      <c r="AV52" s="23"/>
+      <c r="AX52" s="51"/>
+      <c r="AY52" s="50"/>
+      <c r="AZ52" s="23"/>
+      <c r="BA52" s="23"/>
+      <c r="BB52" s="99"/>
+      <c r="BC52" s="100"/>
+      <c r="BD52" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="77"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="53">
-        <v>5</v>
-      </c>
-      <c r="E52" s="55"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="24"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="6"/>
-      <c r="W52" s="6"/>
-      <c r="X52" s="18"/>
-      <c r="Y52" s="24"/>
-      <c r="Z52" s="5"/>
-      <c r="AA52" s="6"/>
-      <c r="AB52" s="6"/>
-      <c r="AC52" s="18"/>
-      <c r="AD52" s="24"/>
-      <c r="AE52" s="5"/>
-      <c r="AF52" s="6"/>
-      <c r="AG52" s="6"/>
-      <c r="AH52" s="18"/>
-      <c r="AI52" s="24"/>
-      <c r="AJ52" s="5"/>
-      <c r="AK52" s="6"/>
-      <c r="AL52" s="6"/>
-      <c r="AM52" s="18"/>
-      <c r="AN52" s="24"/>
-      <c r="AO52" s="5"/>
-      <c r="AP52" s="6"/>
-      <c r="AQ52" s="6"/>
-      <c r="AR52" s="18"/>
-      <c r="AS52" s="24"/>
-      <c r="AT52" s="5"/>
-      <c r="AU52" s="6"/>
-      <c r="AV52" s="6"/>
-      <c r="AW52" s="18"/>
-      <c r="AX52" s="24"/>
-      <c r="AY52" s="5"/>
-      <c r="AZ52" s="6"/>
-      <c r="BA52" s="18"/>
-      <c r="BB52" s="87"/>
-      <c r="BC52" s="88"/>
-      <c r="BD52" s="62" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="78"/>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
-      <c r="N53" s="9"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="9"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="9"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="8"/>
-      <c r="V53" s="9"/>
-      <c r="W53" s="9"/>
-      <c r="X53" s="9"/>
-      <c r="Y53" s="4"/>
-      <c r="Z53" s="8"/>
-      <c r="AA53" s="9"/>
-      <c r="AB53" s="9"/>
-      <c r="AC53" s="9"/>
-      <c r="AD53" s="4"/>
-      <c r="AE53" s="8"/>
-      <c r="AF53" s="9"/>
-      <c r="AG53" s="9"/>
-      <c r="AH53" s="9"/>
-      <c r="AI53" s="4"/>
-      <c r="AJ53" s="8"/>
-      <c r="AK53" s="9"/>
-      <c r="AL53" s="9"/>
-      <c r="AM53" s="9"/>
-      <c r="AN53" s="4"/>
-      <c r="AO53" s="8"/>
-      <c r="AP53" s="9"/>
-      <c r="AQ53" s="9"/>
-      <c r="AR53" s="9"/>
-      <c r="AS53" s="4"/>
-      <c r="AT53" s="8"/>
-      <c r="AU53" s="9"/>
-      <c r="AV53" s="9"/>
-      <c r="AW53" s="9"/>
-      <c r="AX53" s="4"/>
-      <c r="AY53" s="8"/>
-      <c r="AZ53" s="9"/>
-      <c r="BA53" s="9"/>
-      <c r="BB53" s="87"/>
-      <c r="BC53" s="88"/>
-      <c r="BD53" s="62"/>
+      <c r="A53" s="89"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="12"/>
+      <c r="U53" s="10"/>
+      <c r="V53" s="11"/>
+      <c r="W53" s="11"/>
+      <c r="X53" s="11"/>
+      <c r="Y53" s="12"/>
+      <c r="Z53" s="10"/>
+      <c r="AA53" s="11"/>
+      <c r="AB53" s="11"/>
+      <c r="AC53" s="11"/>
+      <c r="AD53" s="12"/>
+      <c r="AE53" s="10"/>
+      <c r="AF53" s="11"/>
+      <c r="AG53" s="11"/>
+      <c r="AH53" s="11"/>
+      <c r="AI53" s="12"/>
+      <c r="AJ53" s="10"/>
+      <c r="AK53" s="11"/>
+      <c r="AL53" s="11"/>
+      <c r="AM53" s="11"/>
+      <c r="AN53" s="12"/>
+      <c r="AO53" s="10"/>
+      <c r="AP53" s="11"/>
+      <c r="AQ53" s="11"/>
+      <c r="AR53" s="11"/>
+      <c r="AS53" s="12"/>
+      <c r="AT53" s="10"/>
+      <c r="AU53" s="11"/>
+      <c r="AV53" s="11"/>
+      <c r="AW53" s="11"/>
+      <c r="AX53" s="12"/>
+      <c r="AY53" s="10"/>
+      <c r="AZ53" s="11"/>
+      <c r="BA53" s="11"/>
+      <c r="BB53" s="99"/>
+      <c r="BC53" s="100"/>
+      <c r="BD53" s="70"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="67" t="s">
+      <c r="A54" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="68"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="57">
-        <v>2</v>
-      </c>
-      <c r="E54" s="58"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="9"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="4"/>
-      <c r="U54" s="8"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="4"/>
-      <c r="Z54" s="8"/>
-      <c r="AA54" s="9"/>
-      <c r="AB54" s="9"/>
-      <c r="AC54" s="9"/>
-      <c r="AD54" s="4"/>
-      <c r="AE54" s="8"/>
-      <c r="AF54" s="9"/>
-      <c r="AG54" s="9"/>
-      <c r="AH54" s="9"/>
-      <c r="AI54" s="4"/>
-      <c r="AJ54" s="8"/>
-      <c r="AK54" s="9"/>
-      <c r="AL54" s="9"/>
-      <c r="AM54" s="9"/>
-      <c r="AN54" s="4"/>
-      <c r="AO54" s="8"/>
-      <c r="AP54" s="9"/>
-      <c r="AQ54" s="9"/>
-      <c r="AR54" s="9"/>
-      <c r="AS54" s="4"/>
-      <c r="AT54" s="8"/>
-      <c r="AU54" s="9"/>
-      <c r="AV54" s="9"/>
-      <c r="AW54" s="9"/>
-      <c r="AX54" s="4"/>
-      <c r="AY54" s="8"/>
-      <c r="AZ54" s="9"/>
-      <c r="BA54" s="28"/>
-      <c r="BB54" s="87"/>
-      <c r="BC54" s="88"/>
-      <c r="BD54" s="62"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="71">
+        <v>4.5</v>
+      </c>
+      <c r="E54" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="F54" s="50"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="23"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="45"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="23"/>
+      <c r="R54" s="23"/>
+      <c r="S54" s="23"/>
+      <c r="U54" s="50"/>
+      <c r="V54" s="23"/>
+      <c r="W54" s="23"/>
+      <c r="X54" s="23"/>
+      <c r="Y54" s="45"/>
+      <c r="Z54" s="50"/>
+      <c r="AA54" s="23"/>
+      <c r="AB54" s="23"/>
+      <c r="AC54" s="23"/>
+      <c r="AD54" s="45"/>
+      <c r="AE54" s="50"/>
+      <c r="AF54" s="23"/>
+      <c r="AG54" s="23"/>
+      <c r="AH54" s="23"/>
+      <c r="AI54" s="45"/>
+      <c r="AJ54" s="50"/>
+      <c r="AK54" s="23"/>
+      <c r="AL54" s="23"/>
+      <c r="AM54" s="23"/>
+      <c r="AN54" s="45"/>
+      <c r="AO54" s="50"/>
+      <c r="AP54" s="23"/>
+      <c r="AQ54" s="23"/>
+      <c r="AR54" s="23"/>
+      <c r="AS54" s="45"/>
+      <c r="AT54" s="50"/>
+      <c r="AU54" s="23"/>
+      <c r="AV54" s="23"/>
+      <c r="AW54" s="23"/>
+      <c r="AX54" s="45"/>
+      <c r="AY54" s="50"/>
+      <c r="AZ54" s="23"/>
+      <c r="BA54" s="54"/>
+      <c r="BB54" s="99"/>
+      <c r="BC54" s="100"/>
+      <c r="BD54" s="70"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="73"/>
-      <c r="B55" s="74"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="10"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="10"/>
-      <c r="V55" s="11"/>
-      <c r="W55" s="11"/>
-      <c r="X55" s="11"/>
-      <c r="Y55" s="12"/>
-      <c r="Z55" s="10"/>
-      <c r="AA55" s="11"/>
-      <c r="AB55" s="11"/>
-      <c r="AC55" s="11"/>
-      <c r="AD55" s="12"/>
-      <c r="AE55" s="10"/>
-      <c r="AF55" s="11"/>
-      <c r="AG55" s="11"/>
-      <c r="AH55" s="11"/>
-      <c r="AI55" s="12"/>
-      <c r="AJ55" s="10"/>
-      <c r="AK55" s="11"/>
-      <c r="AL55" s="11"/>
-      <c r="AM55" s="11"/>
-      <c r="AN55" s="12"/>
-      <c r="AO55" s="10"/>
-      <c r="AP55" s="11"/>
-      <c r="AQ55" s="11"/>
-      <c r="AR55" s="11"/>
-      <c r="AS55" s="12"/>
-      <c r="AT55" s="10"/>
-      <c r="AU55" s="11"/>
-      <c r="AV55" s="11"/>
-      <c r="AW55" s="11"/>
-      <c r="AX55" s="12"/>
-      <c r="AY55" s="10"/>
-      <c r="AZ55" s="11"/>
-      <c r="BA55" s="11"/>
-      <c r="BB55" s="87"/>
-      <c r="BC55" s="88"/>
-      <c r="BD55" s="62"/>
+      <c r="A55" s="82"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="49"/>
+      <c r="U55" s="43"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="9"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="4"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="9"/>
+      <c r="AG55" s="9"/>
+      <c r="AH55" s="9"/>
+      <c r="AI55" s="4"/>
+      <c r="AJ55" s="8"/>
+      <c r="AK55" s="9"/>
+      <c r="AL55" s="9"/>
+      <c r="AM55" s="9"/>
+      <c r="AN55" s="4"/>
+      <c r="AO55" s="8"/>
+      <c r="AP55" s="9"/>
+      <c r="AQ55" s="9"/>
+      <c r="AR55" s="9"/>
+      <c r="AS55" s="4"/>
+      <c r="AT55" s="8"/>
+      <c r="AU55" s="9"/>
+      <c r="AV55" s="9"/>
+      <c r="AW55" s="9"/>
+      <c r="AX55" s="4"/>
+      <c r="AY55" s="8"/>
+      <c r="AZ55" s="9"/>
+      <c r="BA55" s="9"/>
+      <c r="BB55" s="99"/>
+      <c r="BC55" s="100"/>
+      <c r="BD55" s="70"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56" s="81"/>
-      <c r="C56" s="82"/>
-      <c r="D56" s="53">
-        <v>2.5</v>
-      </c>
-      <c r="E56" s="55"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
-      <c r="S56" s="6"/>
-      <c r="T56" s="7"/>
-      <c r="U56" s="5"/>
-      <c r="V56" s="6"/>
-      <c r="W56" s="6"/>
-      <c r="X56" s="6"/>
-      <c r="Y56" s="7"/>
-      <c r="Z56" s="5"/>
-      <c r="AA56" s="6"/>
-      <c r="AB56" s="6"/>
-      <c r="AC56" s="6"/>
-      <c r="AD56" s="7"/>
-      <c r="AE56" s="5"/>
-      <c r="AF56" s="6"/>
-      <c r="AG56" s="6"/>
-      <c r="AH56" s="6"/>
-      <c r="AI56" s="7"/>
-      <c r="AJ56" s="5"/>
-      <c r="AK56" s="6"/>
-      <c r="AL56" s="6"/>
-      <c r="AM56" s="6"/>
-      <c r="AN56" s="7"/>
-      <c r="AO56" s="5"/>
-      <c r="AP56" s="6"/>
-      <c r="AQ56" s="6"/>
-      <c r="AR56" s="6"/>
-      <c r="AS56" s="7"/>
-      <c r="AT56" s="5"/>
-      <c r="AU56" s="6"/>
-      <c r="AV56" s="6"/>
-      <c r="AW56" s="6"/>
-      <c r="AX56" s="7"/>
-      <c r="AY56" s="5"/>
-      <c r="AZ56" s="6"/>
-      <c r="BA56" s="6"/>
-      <c r="BB56" s="87"/>
-      <c r="BC56" s="88"/>
-      <c r="BD56" s="62"/>
+      <c r="A56" s="92" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="93"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="23"/>
+      <c r="M56" s="23"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="45"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="23"/>
+      <c r="R56" s="23"/>
+      <c r="S56" s="23"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="60"/>
+      <c r="V56" s="23"/>
+      <c r="W56" s="23"/>
+      <c r="X56" s="23"/>
+      <c r="Y56" s="45"/>
+      <c r="Z56" s="50"/>
+      <c r="AA56" s="23"/>
+      <c r="AB56" s="23"/>
+      <c r="AC56" s="23"/>
+      <c r="AD56" s="45"/>
+      <c r="AE56" s="50"/>
+      <c r="AF56" s="23"/>
+      <c r="AG56" s="23"/>
+      <c r="AH56" s="23"/>
+      <c r="AI56" s="45"/>
+      <c r="AJ56" s="50"/>
+      <c r="AK56" s="23"/>
+      <c r="AL56" s="23"/>
+      <c r="AM56" s="23"/>
+      <c r="AN56" s="45"/>
+      <c r="AO56" s="50"/>
+      <c r="AP56" s="23"/>
+      <c r="AQ56" s="23"/>
+      <c r="AR56" s="23"/>
+      <c r="AS56" s="45"/>
+      <c r="AT56" s="50"/>
+      <c r="AU56" s="23"/>
+      <c r="AV56" s="23"/>
+      <c r="AW56" s="23"/>
+      <c r="AX56" s="45"/>
+      <c r="AY56" s="50"/>
+      <c r="AZ56" s="23"/>
+      <c r="BA56" s="23"/>
+      <c r="BB56" s="99"/>
+      <c r="BC56" s="100"/>
+      <c r="BD56" s="70"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="70"/>
-      <c r="B57" s="71"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61"/>
+      <c r="A57" s="82"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5156,8 +5217,8 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="2"/>
+      <c r="T57" s="32"/>
+      <c r="U57" s="14"/>
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
@@ -5190,16 +5251,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="87"/>
-      <c r="BC57" s="88"/>
-      <c r="BD57" s="62"/>
+      <c r="BB57" s="99"/>
+      <c r="BC57" s="100"/>
+      <c r="BD57" s="70"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="67"/>
-      <c r="B58" s="68"/>
-      <c r="C58" s="69"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="58"/>
+      <c r="A58" s="79"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="81"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="66"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5248,16 +5309,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="87"/>
-      <c r="BC58" s="88"/>
-      <c r="BD58" s="62"/>
+      <c r="BB58" s="99"/>
+      <c r="BC58" s="100"/>
+      <c r="BD58" s="70"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="73"/>
-      <c r="B59" s="74"/>
-      <c r="C59" s="75"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="56"/>
+      <c r="A59" s="89"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="91"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="64"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5306,31 +5367,31 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="89"/>
-      <c r="BC59" s="90"/>
-      <c r="BD59" s="62"/>
+      <c r="BB59" s="101"/>
+      <c r="BC59" s="102"/>
+      <c r="BD59" s="70"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84"/>
-      <c r="D60" s="63">
+      <c r="A60" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="96"/>
+      <c r="C60" s="96"/>
+      <c r="D60" s="75">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="65">
+      <c r="E60" s="77">
         <f>SUM(E4:E59)</f>
-        <v>16.2</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="85"/>
-      <c r="B61" s="86"/>
-      <c r="C61" s="86"/>
-      <c r="D61" s="64"/>
-      <c r="E61" s="66"/>
+      <c r="A61" s="97"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="98"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="78"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -5410,9 +5471,9 @@
     <mergeCell ref="A60:C61"/>
     <mergeCell ref="A40:C41"/>
     <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A44:C45"/>
     <mergeCell ref="A46:C47"/>
     <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="E54:E55"/>
     <mergeCell ref="D52:D53"/>

</xml_diff>

<commit_message>
boSL und boGrid fertig
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="593" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65BC3B4B-0AB8-4589-8B16-79013385A77A}"/>
+  <xr:revisionPtr revIDLastSave="615" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2B3F617-BFE9-45E2-95FC-A402E50A73C0}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Aufwand (h)</t>
   </si>
@@ -270,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -994,11 +994,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1062,227 +1073,239 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1594,7 +1617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1607,8 +1630,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,171 +1643,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="117" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="119" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="111" t="s">
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="111" t="s">
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="111" t="s">
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="111" t="s">
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="113"/>
-      <c r="AE1" s="111" t="s">
+      <c r="AA1" s="87"/>
+      <c r="AB1" s="87"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="88"/>
+      <c r="AE1" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="112"/>
-      <c r="AG1" s="112"/>
-      <c r="AH1" s="112"/>
-      <c r="AI1" s="113"/>
-      <c r="AJ1" s="111" t="s">
+      <c r="AF1" s="87"/>
+      <c r="AG1" s="87"/>
+      <c r="AH1" s="87"/>
+      <c r="AI1" s="88"/>
+      <c r="AJ1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="112"/>
-      <c r="AL1" s="112"/>
-      <c r="AM1" s="112"/>
-      <c r="AN1" s="113"/>
-      <c r="AO1" s="111" t="s">
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="87"/>
+      <c r="AM1" s="87"/>
+      <c r="AN1" s="88"/>
+      <c r="AO1" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="112"/>
-      <c r="AQ1" s="112"/>
-      <c r="AR1" s="112"/>
-      <c r="AS1" s="113"/>
-      <c r="AT1" s="111" t="s">
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="87"/>
+      <c r="AR1" s="87"/>
+      <c r="AS1" s="88"/>
+      <c r="AT1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="112"/>
-      <c r="AV1" s="112"/>
-      <c r="AW1" s="112"/>
-      <c r="AX1" s="113"/>
-      <c r="AY1" s="111" t="s">
+      <c r="AU1" s="87"/>
+      <c r="AV1" s="87"/>
+      <c r="AW1" s="87"/>
+      <c r="AX1" s="88"/>
+      <c r="AY1" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="112"/>
-      <c r="BA1" s="112"/>
-      <c r="BB1" s="112"/>
-      <c r="BC1" s="113"/>
-      <c r="BD1" s="70" t="s">
+      <c r="AZ1" s="87"/>
+      <c r="BA1" s="87"/>
+      <c r="BB1" s="87"/>
+      <c r="BC1" s="88"/>
+      <c r="BD1" s="61" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="122">
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="83">
         <v>44957</v>
       </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="108">
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="72">
         <v>44958</v>
       </c>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="108">
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="72">
         <v>44959</v>
       </c>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="109"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="108">
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="72">
         <v>44960</v>
       </c>
-      <c r="V2" s="109"/>
-      <c r="W2" s="109"/>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="108">
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="72">
         <v>44964</v>
       </c>
-      <c r="AA2" s="109"/>
-      <c r="AB2" s="109"/>
-      <c r="AC2" s="109"/>
-      <c r="AD2" s="110"/>
-      <c r="AE2" s="108">
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="72">
         <v>44965</v>
       </c>
-      <c r="AF2" s="109"/>
-      <c r="AG2" s="109"/>
-      <c r="AH2" s="109"/>
-      <c r="AI2" s="110"/>
-      <c r="AJ2" s="108">
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="72">
         <v>44966</v>
       </c>
-      <c r="AK2" s="109"/>
-      <c r="AL2" s="109"/>
-      <c r="AM2" s="109"/>
-      <c r="AN2" s="110"/>
-      <c r="AO2" s="108">
+      <c r="AK2" s="73"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="73"/>
+      <c r="AN2" s="74"/>
+      <c r="AO2" s="72">
         <v>44967</v>
       </c>
-      <c r="AP2" s="109"/>
-      <c r="AQ2" s="109"/>
-      <c r="AR2" s="109"/>
-      <c r="AS2" s="110"/>
-      <c r="AT2" s="108">
+      <c r="AP2" s="73"/>
+      <c r="AQ2" s="73"/>
+      <c r="AR2" s="73"/>
+      <c r="AS2" s="74"/>
+      <c r="AT2" s="72">
         <v>44971</v>
       </c>
-      <c r="AU2" s="109"/>
-      <c r="AV2" s="109"/>
-      <c r="AW2" s="109"/>
-      <c r="AX2" s="110"/>
-      <c r="AY2" s="108">
+      <c r="AU2" s="73"/>
+      <c r="AV2" s="73"/>
+      <c r="AW2" s="73"/>
+      <c r="AX2" s="74"/>
+      <c r="AY2" s="72">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="109"/>
-      <c r="BA2" s="109"/>
-      <c r="BB2" s="109"/>
-      <c r="BC2" s="110"/>
-      <c r="BD2" s="70"/>
+      <c r="AZ2" s="73"/>
+      <c r="BA2" s="73"/>
+      <c r="BB2" s="73"/>
+      <c r="BC2" s="74"/>
+      <c r="BD2" s="61"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="116"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1935,24 +1958,24 @@
       <c r="BA3" s="1">
         <v>13</v>
       </c>
-      <c r="BB3" s="1">
+      <c r="BB3" s="11">
         <v>15</v>
       </c>
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="67"/>
+      <c r="BD3" s="134"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="61">
+      <c r="B4" s="102"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="107">
         <v>30</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="109"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -2001,18 +2024,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="99" t="s">
+      <c r="BB4" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="100"/>
-      <c r="BD4" s="67"/>
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="134"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="82"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="73"/>
+      <c r="A5" s="104"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2061,24 +2084,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="99"/>
-      <c r="BC5" s="100"/>
-      <c r="BD5" s="67"/>
-      <c r="BF5" s="125" t="s">
+      <c r="BB5" s="113"/>
+      <c r="BC5" s="114"/>
+      <c r="BD5" s="134"/>
+      <c r="BF5" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="129"/>
+      <c r="BG5" s="66"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="65">
+      <c r="B6" s="92"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="97">
         <v>1</v>
       </c>
-      <c r="E6" s="106">
+      <c r="E6" s="111">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2129,18 +2152,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="99"/>
-      <c r="BC6" s="100"/>
-      <c r="BD6" s="67"/>
-      <c r="BF6" s="126"/>
-      <c r="BG6" s="130"/>
+      <c r="BB6" s="113"/>
+      <c r="BC6" s="114"/>
+      <c r="BD6" s="134"/>
+      <c r="BF6" s="63"/>
+      <c r="BG6" s="67"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="107"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="112"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2189,24 +2212,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="99"/>
-      <c r="BC7" s="100"/>
-      <c r="BD7" s="67"/>
-      <c r="BF7" s="125" t="s">
+      <c r="BB7" s="113"/>
+      <c r="BC7" s="114"/>
+      <c r="BD7" s="134"/>
+      <c r="BF7" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="131"/>
+      <c r="BG7" s="68"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="104"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="61">
+      <c r="B8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="107">
         <v>1.5</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="89">
         <v>0.8</v>
       </c>
       <c r="F8" s="17"/>
@@ -2257,20 +2280,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="99"/>
-      <c r="BC8" s="100"/>
-      <c r="BD8" s="70" t="s">
+      <c r="BB8" s="113"/>
+      <c r="BC8" s="114"/>
+      <c r="BD8" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="126"/>
-      <c r="BG8" s="132"/>
+      <c r="BF8" s="63"/>
+      <c r="BG8" s="69"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="82"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="69"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="90"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2286,7 +2309,7 @@
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
       <c r="T9" s="4"/>
-      <c r="U9" s="8"/>
+      <c r="U9" s="36"/>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
@@ -2319,24 +2342,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="99"/>
-      <c r="BC9" s="100"/>
-      <c r="BD9" s="70"/>
-      <c r="BF9" s="127" t="s">
+      <c r="BB9" s="113"/>
+      <c r="BC9" s="114"/>
+      <c r="BD9" s="61"/>
+      <c r="BF9" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="133"/>
+      <c r="BG9" s="70"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="65">
+      <c r="B10" s="92"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="97">
         <v>1.5</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="99">
         <v>0.8</v>
       </c>
       <c r="F10" s="19"/>
@@ -2387,18 +2410,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="99"/>
-      <c r="BC10" s="100"/>
-      <c r="BD10" s="70"/>
-      <c r="BF10" s="128"/>
-      <c r="BG10" s="134"/>
+      <c r="BB10" s="113"/>
+      <c r="BC10" s="114"/>
+      <c r="BD10" s="61"/>
+      <c r="BF10" s="65"/>
+      <c r="BG10" s="71"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="64"/>
+      <c r="A11" s="94"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="100"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2414,7 +2437,7 @@
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="12"/>
-      <c r="U11" s="10"/>
+      <c r="U11" s="37"/>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11"/>
@@ -2447,20 +2470,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="99"/>
-      <c r="BC11" s="100"/>
-      <c r="BD11" s="70"/>
+      <c r="BB11" s="113"/>
+      <c r="BC11" s="114"/>
+      <c r="BD11" s="61"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="61">
+      <c r="B12" s="102"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="107">
         <v>1</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="89">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2511,9 +2534,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="99"/>
-      <c r="BC12" s="100"/>
-      <c r="BD12" s="70" t="s">
+      <c r="BB12" s="113"/>
+      <c r="BC12" s="114"/>
+      <c r="BD12" s="61" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2527,11 +2550,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="69"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="90"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2580,9 +2603,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="99"/>
-      <c r="BC13" s="100"/>
-      <c r="BD13" s="70"/>
+      <c r="BB13" s="113"/>
+      <c r="BC13" s="114"/>
+      <c r="BD13" s="61"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2594,15 +2617,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="65">
+      <c r="B14" s="92"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="97">
         <v>2</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="99">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2653,16 +2676,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="99"/>
-      <c r="BC14" s="100"/>
-      <c r="BD14" s="70"/>
+      <c r="BB14" s="113"/>
+      <c r="BC14" s="114"/>
+      <c r="BD14" s="61"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2711,20 +2734,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="99"/>
-      <c r="BC15" s="100"/>
-      <c r="BD15" s="70"/>
+      <c r="BB15" s="113"/>
+      <c r="BC15" s="114"/>
+      <c r="BD15" s="61"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="65">
+      <c r="B16" s="92"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="97">
         <v>1</v>
       </c>
-      <c r="E16" s="66">
+      <c r="E16" s="99">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2775,16 +2798,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="99"/>
-      <c r="BC16" s="100"/>
-      <c r="BD16" s="70"/>
+      <c r="BB16" s="113"/>
+      <c r="BC16" s="114"/>
+      <c r="BD16" s="61"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="82"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="69"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2833,23 +2856,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="99"/>
-      <c r="BC17" s="100"/>
-      <c r="BD17" s="70"/>
+      <c r="BB17" s="113"/>
+      <c r="BC17" s="114"/>
+      <c r="BD17" s="61"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="65">
+      <c r="B18" s="92"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="97">
         <v>2</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="99">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2900,16 +2923,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="99"/>
-      <c r="BC18" s="100"/>
-      <c r="BD18" s="70"/>
+      <c r="BB18" s="113"/>
+      <c r="BC18" s="114"/>
+      <c r="BD18" s="61"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="82"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="69"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="90"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -2958,20 +2981,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="99"/>
-      <c r="BC19" s="100"/>
-      <c r="BD19" s="70"/>
+      <c r="BB19" s="113"/>
+      <c r="BC19" s="114"/>
+      <c r="BD19" s="61"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="65">
+      <c r="B20" s="92"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="97">
         <v>1</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="99">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3022,16 +3045,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="99"/>
-      <c r="BC20" s="100"/>
-      <c r="BD20" s="70"/>
+      <c r="BB20" s="113"/>
+      <c r="BC20" s="114"/>
+      <c r="BD20" s="61"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="89"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="64"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="100"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3080,20 +3103,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="99"/>
-      <c r="BC21" s="100"/>
-      <c r="BD21" s="70"/>
+      <c r="BB21" s="113"/>
+      <c r="BC21" s="114"/>
+      <c r="BD21" s="61"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="104"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="61">
+      <c r="B22" s="102"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="107">
         <v>0.5</v>
       </c>
-      <c r="E22" s="63">
+      <c r="E22" s="89">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3144,18 +3167,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="99"/>
-      <c r="BC22" s="100"/>
-      <c r="BD22" s="70" t="s">
+      <c r="BB22" s="113"/>
+      <c r="BC22" s="114"/>
+      <c r="BD22" s="61" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="64"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="100"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3204,20 +3227,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="99"/>
-      <c r="BC23" s="100"/>
-      <c r="BD23" s="70"/>
-    </row>
-    <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="103" t="s">
+      <c r="BB23" s="113"/>
+      <c r="BC23" s="114"/>
+      <c r="BD23" s="61"/>
+    </row>
+    <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="104"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="61">
+      <c r="B24" s="102"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="107">
         <v>2</v>
       </c>
-      <c r="E24" s="63">
+      <c r="E24" s="89">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3268,18 +3291,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="99"/>
-      <c r="BC24" s="100"/>
-      <c r="BD24" s="70" t="s">
+      <c r="BB24" s="113"/>
+      <c r="BC24" s="114"/>
+      <c r="BD24" s="136" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="82"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="69"/>
+    <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="104"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="90"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3328,20 +3351,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="99"/>
-      <c r="BC25" s="100"/>
-      <c r="BD25" s="70"/>
-    </row>
-    <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="79" t="s">
+      <c r="BB25" s="113"/>
+      <c r="BC25" s="114"/>
+      <c r="BD25" s="137"/>
+    </row>
+    <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="65">
+      <c r="B26" s="92"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="97">
         <v>1</v>
       </c>
-      <c r="E26" s="66">
+      <c r="E26" s="99">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3392,16 +3415,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="99"/>
-      <c r="BC26" s="100"/>
-      <c r="BD26" s="70"/>
-    </row>
-    <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="82"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
+      <c r="BB26" s="113"/>
+      <c r="BC26" s="114"/>
+      <c r="BD26" s="137"/>
+    </row>
+    <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="104"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="90"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3450,20 +3473,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="99"/>
-      <c r="BC27" s="100"/>
-      <c r="BD27" s="70"/>
-    </row>
-    <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="79" t="s">
+      <c r="BB27" s="113"/>
+      <c r="BC27" s="114"/>
+      <c r="BD27" s="137"/>
+    </row>
+    <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="80"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="65">
+      <c r="B28" s="92"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="97">
         <v>2</v>
       </c>
-      <c r="E28" s="66">
+      <c r="E28" s="99">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3514,16 +3537,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="99"/>
-      <c r="BC28" s="100"/>
-      <c r="BD28" s="70"/>
-    </row>
-    <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="82"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
+      <c r="BB28" s="113"/>
+      <c r="BC28" s="114"/>
+      <c r="BD28" s="137"/>
+    </row>
+    <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="104"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="90"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3572,20 +3595,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="99"/>
-      <c r="BC29" s="100"/>
-      <c r="BD29" s="70"/>
-    </row>
-    <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="79" t="s">
+      <c r="BB29" s="113"/>
+      <c r="BC29" s="114"/>
+      <c r="BD29" s="137"/>
+    </row>
+    <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="65">
+      <c r="B30" s="92"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="97">
         <v>2</v>
       </c>
-      <c r="E30" s="66">
+      <c r="E30" s="99">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3636,16 +3659,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="99"/>
-      <c r="BC30" s="100"/>
-      <c r="BD30" s="70"/>
-    </row>
-    <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="82"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="69"/>
+      <c r="BB30" s="113"/>
+      <c r="BC30" s="114"/>
+      <c r="BD30" s="137"/>
+    </row>
+    <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="104"/>
+      <c r="B31" s="105"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="90"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3694,20 +3717,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="99"/>
-      <c r="BC31" s="100"/>
-      <c r="BD31" s="70"/>
-    </row>
-    <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="79" t="s">
+      <c r="BB31" s="113"/>
+      <c r="BC31" s="114"/>
+      <c r="BD31" s="137"/>
+    </row>
+    <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="65">
+      <c r="B32" s="92"/>
+      <c r="C32" s="93"/>
+      <c r="D32" s="97">
         <v>4</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="99">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3758,16 +3781,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="99"/>
-      <c r="BC32" s="100"/>
-      <c r="BD32" s="70"/>
-    </row>
-    <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="82"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="69"/>
+      <c r="BB32" s="113"/>
+      <c r="BC32" s="114"/>
+      <c r="BD32" s="137"/>
+    </row>
+    <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="104"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="90"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3816,21 +3839,21 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="99"/>
-      <c r="BC33" s="100"/>
-      <c r="BD33" s="70"/>
-    </row>
-    <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="79" t="s">
+      <c r="BB33" s="113"/>
+      <c r="BC33" s="114"/>
+      <c r="BD33" s="137"/>
+    </row>
+    <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="80"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="65">
+      <c r="B34" s="92"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="97">
         <v>3</v>
       </c>
-      <c r="E34" s="66">
-        <v>2</v>
+      <c r="E34" s="99">
+        <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
@@ -3880,16 +3903,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="99"/>
-      <c r="BC34" s="100"/>
-      <c r="BD34" s="70"/>
-    </row>
-    <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="82"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="69"/>
+      <c r="BB34" s="113"/>
+      <c r="BC34" s="114"/>
+      <c r="BD34" s="137"/>
+    </row>
+    <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="104"/>
+      <c r="B35" s="105"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="90"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3905,7 +3928,7 @@
       <c r="R35" s="9"/>
       <c r="S35" s="30"/>
       <c r="T35" s="32"/>
-      <c r="U35" s="8"/>
+      <c r="U35" s="36"/>
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
       <c r="X35" s="9"/>
@@ -3938,20 +3961,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="99"/>
-      <c r="BC35" s="100"/>
-      <c r="BD35" s="70"/>
-    </row>
-    <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="79" t="s">
+      <c r="BB35" s="113"/>
+      <c r="BC35" s="114"/>
+      <c r="BD35" s="137"/>
+    </row>
+    <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="80"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="65">
+      <c r="B36" s="92"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="97">
         <v>4</v>
       </c>
-      <c r="E36" s="66"/>
+      <c r="E36" s="99"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -3999,16 +4022,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="99"/>
-      <c r="BC36" s="100"/>
-      <c r="BD36" s="70"/>
-    </row>
-    <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="69"/>
+      <c r="BB36" s="113"/>
+      <c r="BC36" s="114"/>
+      <c r="BD36" s="137"/>
+    </row>
+    <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="104"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="90"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4057,20 +4080,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="99"/>
-      <c r="BC37" s="100"/>
-      <c r="BD37" s="70"/>
-    </row>
-    <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="79" t="s">
+      <c r="BB37" s="113"/>
+      <c r="BC37" s="114"/>
+      <c r="BD37" s="137"/>
+    </row>
+    <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="65">
+      <c r="B38" s="92"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="97">
         <v>1</v>
       </c>
-      <c r="E38" s="66"/>
+      <c r="E38" s="99"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -4118,16 +4141,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="99"/>
-      <c r="BC38" s="100"/>
-      <c r="BD38" s="70"/>
-    </row>
-    <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="82"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="69"/>
+      <c r="BB38" s="113"/>
+      <c r="BC38" s="114"/>
+      <c r="BD38" s="137"/>
+    </row>
+    <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="104"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="108"/>
+      <c r="E39" s="90"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4176,20 +4199,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="99"/>
-      <c r="BC39" s="100"/>
-      <c r="BD39" s="70"/>
-    </row>
-    <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="79" t="s">
+      <c r="BB39" s="113"/>
+      <c r="BC39" s="114"/>
+      <c r="BD39" s="137"/>
+    </row>
+    <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="80"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="65">
+      <c r="B40" s="92"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="97">
         <v>1</v>
       </c>
-      <c r="E40" s="66"/>
+      <c r="E40" s="99"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -4239,16 +4262,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="99"/>
-      <c r="BC40" s="100"/>
-      <c r="BD40" s="70"/>
-    </row>
-    <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="82"/>
-      <c r="B41" s="83"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="69"/>
+      <c r="BB40" s="113"/>
+      <c r="BC40" s="114"/>
+      <c r="BD40" s="137"/>
+    </row>
+    <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="104"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="108"/>
+      <c r="E41" s="90"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4297,20 +4320,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="99"/>
-      <c r="BC41" s="100"/>
-      <c r="BD41" s="70"/>
-    </row>
-    <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="79" t="s">
+      <c r="BB41" s="113"/>
+      <c r="BC41" s="114"/>
+      <c r="BD41" s="137"/>
+    </row>
+    <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="65">
+      <c r="B42" s="92"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="97">
         <v>2</v>
       </c>
-      <c r="E42" s="66"/>
+      <c r="E42" s="99"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -4359,16 +4382,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="99"/>
-      <c r="BC42" s="100"/>
-      <c r="BD42" s="70"/>
-    </row>
-    <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="82"/>
-      <c r="B43" s="83"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="69"/>
+      <c r="BB42" s="113"/>
+      <c r="BC42" s="114"/>
+      <c r="BD42" s="137"/>
+    </row>
+    <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="104"/>
+      <c r="B43" s="105"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="90"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4417,20 +4440,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="99"/>
-      <c r="BC43" s="100"/>
-      <c r="BD43" s="70"/>
-    </row>
-    <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="79" t="s">
+      <c r="BB43" s="113"/>
+      <c r="BC43" s="114"/>
+      <c r="BD43" s="137"/>
+    </row>
+    <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="80"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="65">
+      <c r="B44" s="92"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="97">
         <v>2</v>
       </c>
-      <c r="E44" s="66"/>
+      <c r="E44" s="99"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4479,16 +4502,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="99"/>
-      <c r="BC44" s="100"/>
-      <c r="BD44" s="70"/>
+      <c r="BB44" s="113"/>
+      <c r="BC44" s="114"/>
+      <c r="BD44" s="137"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="89"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="91"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="64"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="98"/>
+      <c r="E45" s="100"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4537,20 +4560,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="99"/>
-      <c r="BC45" s="100"/>
-      <c r="BD45" s="70"/>
+      <c r="BB45" s="113"/>
+      <c r="BC45" s="114"/>
+      <c r="BD45" s="138"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="92" t="s">
+      <c r="A46" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="93"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="71">
+      <c r="B46" s="122"/>
+      <c r="C46" s="123"/>
+      <c r="D46" s="128">
         <v>1</v>
       </c>
-      <c r="E46" s="72"/>
+      <c r="E46" s="109"/>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4598,16 +4621,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="99"/>
-      <c r="BC46" s="100"/>
-      <c r="BD46" s="70"/>
+      <c r="BB46" s="113"/>
+      <c r="BC46" s="114"/>
+      <c r="BD46" s="61" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="82"/>
-      <c r="B47" s="83"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="73"/>
+      <c r="A47" s="104"/>
+      <c r="B47" s="105"/>
+      <c r="C47" s="106"/>
+      <c r="D47" s="108"/>
+      <c r="E47" s="110"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4656,20 +4681,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="99"/>
-      <c r="BC47" s="100"/>
-      <c r="BD47" s="70"/>
+      <c r="BB47" s="113"/>
+      <c r="BC47" s="114"/>
+      <c r="BD47" s="61"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="79" t="s">
+      <c r="A48" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="80"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="65">
+      <c r="B48" s="92"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="97">
         <v>2</v>
       </c>
-      <c r="E48" s="66"/>
+      <c r="E48" s="99"/>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4718,18 +4743,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="99"/>
-      <c r="BC48" s="100"/>
-      <c r="BD48" s="70" t="s">
-        <v>32</v>
-      </c>
+      <c r="BB48" s="113"/>
+      <c r="BC48" s="114"/>
+      <c r="BD48" s="61"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="89"/>
-      <c r="B49" s="90"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="64"/>
+      <c r="A49" s="94"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="98"/>
+      <c r="E49" s="100"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4778,20 +4801,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="99"/>
-      <c r="BC49" s="100"/>
-      <c r="BD49" s="70"/>
+      <c r="BB49" s="113"/>
+      <c r="BC49" s="114"/>
+      <c r="BD49" s="61"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="85" t="s">
+      <c r="A50" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="86"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="71">
+      <c r="B50" s="118"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="128">
         <v>5</v>
       </c>
-      <c r="E50" s="74"/>
+      <c r="E50" s="129"/>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4839,17 +4862,19 @@
       <c r="AX50" s="45"/>
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
-      <c r="BA50" s="44"/>
-      <c r="BB50" s="99"/>
-      <c r="BC50" s="100"/>
-      <c r="BD50" s="70"/>
+      <c r="BA50" s="54"/>
+      <c r="BB50" s="113"/>
+      <c r="BC50" s="114"/>
+      <c r="BD50" s="61" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="87"/>
-      <c r="B51" s="88"/>
-      <c r="C51" s="88"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="69"/>
+      <c r="A51" s="119"/>
+      <c r="B51" s="120"/>
+      <c r="C51" s="120"/>
+      <c r="D51" s="108"/>
+      <c r="E51" s="90"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4898,20 +4923,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="99"/>
-      <c r="BC51" s="100"/>
-      <c r="BD51" s="70"/>
+      <c r="BB51" s="113"/>
+      <c r="BC51" s="114"/>
+      <c r="BD51" s="61"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="79" t="s">
+      <c r="A52" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="80"/>
-      <c r="C52" s="81"/>
-      <c r="D52" s="65">
+      <c r="B52" s="92"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="97">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
+      <c r="E52" s="99"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -4952,18 +4977,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="23"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="99"/>
-      <c r="BC52" s="100"/>
-      <c r="BD52" s="70" t="s">
-        <v>35</v>
-      </c>
+      <c r="BB52" s="113"/>
+      <c r="BC52" s="114"/>
+      <c r="BD52" s="61"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="89"/>
-      <c r="B53" s="90"/>
-      <c r="C53" s="91"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="64"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="96"/>
+      <c r="D53" s="98"/>
+      <c r="E53" s="100"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5012,21 +5035,21 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="99"/>
-      <c r="BC53" s="100"/>
-      <c r="BD53" s="70"/>
+      <c r="BB53" s="113"/>
+      <c r="BC53" s="114"/>
+      <c r="BD53" s="61"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="92" t="s">
+      <c r="A54" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="93"/>
-      <c r="C54" s="94"/>
-      <c r="D54" s="71">
+      <c r="B54" s="122"/>
+      <c r="C54" s="123"/>
+      <c r="D54" s="128">
         <v>4.5</v>
       </c>
-      <c r="E54" s="74">
-        <v>0.5</v>
+      <c r="E54" s="129">
+        <v>1</v>
       </c>
       <c r="F54" s="50"/>
       <c r="G54" s="23"/>
@@ -5074,17 +5097,17 @@
       <c r="AX54" s="45"/>
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
-      <c r="BA54" s="54"/>
-      <c r="BB54" s="99"/>
-      <c r="BC54" s="100"/>
-      <c r="BD54" s="70"/>
+      <c r="BA54" s="51"/>
+      <c r="BB54" s="113"/>
+      <c r="BC54" s="114"/>
+      <c r="BD54" s="135"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="82"/>
-      <c r="B55" s="83"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="69"/>
+      <c r="A55" s="104"/>
+      <c r="B55" s="105"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="108"/>
+      <c r="E55" s="90"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5133,18 +5156,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="99"/>
-      <c r="BC55" s="100"/>
-      <c r="BD55" s="70"/>
+      <c r="BB55" s="113"/>
+      <c r="BC55" s="114"/>
+      <c r="BD55" s="135"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="93"/>
-      <c r="C56" s="94"/>
-      <c r="D56" s="71"/>
-      <c r="E56" s="74"/>
+      <c r="A56" s="121"/>
+      <c r="B56" s="122"/>
+      <c r="C56" s="123"/>
+      <c r="D56" s="128"/>
+      <c r="E56" s="129"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5193,16 +5214,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="99"/>
-      <c r="BC56" s="100"/>
-      <c r="BD56" s="70"/>
+      <c r="BB56" s="113"/>
+      <c r="BC56" s="114"/>
+      <c r="BD56" s="135"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="82"/>
-      <c r="B57" s="83"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="69"/>
+      <c r="A57" s="104"/>
+      <c r="B57" s="105"/>
+      <c r="C57" s="106"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="90"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5251,16 +5272,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="99"/>
-      <c r="BC57" s="100"/>
-      <c r="BD57" s="70"/>
+      <c r="BB57" s="113"/>
+      <c r="BC57" s="114"/>
+      <c r="BD57" s="135"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="79"/>
-      <c r="B58" s="80"/>
-      <c r="C58" s="81"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="66"/>
+      <c r="A58" s="91"/>
+      <c r="B58" s="92"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="99"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5309,16 +5330,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="99"/>
-      <c r="BC58" s="100"/>
-      <c r="BD58" s="70"/>
+      <c r="BB58" s="113"/>
+      <c r="BC58" s="114"/>
+      <c r="BD58" s="135"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="89"/>
-      <c r="B59" s="90"/>
-      <c r="C59" s="91"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="64"/>
+      <c r="A59" s="94"/>
+      <c r="B59" s="95"/>
+      <c r="C59" s="96"/>
+      <c r="D59" s="98"/>
+      <c r="E59" s="100"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5367,53 +5388,117 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="101"/>
-      <c r="BC59" s="102"/>
-      <c r="BD59" s="70"/>
+      <c r="BB59" s="115"/>
+      <c r="BC59" s="116"/>
+      <c r="BD59" s="135"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="95" t="s">
+      <c r="A60" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="96"/>
-      <c r="C60" s="96"/>
-      <c r="D60" s="75">
+      <c r="B60" s="125"/>
+      <c r="C60" s="125"/>
+      <c r="D60" s="130">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="77">
+      <c r="E60" s="132">
         <f>SUM(E4:E59)</f>
-        <v>23.3</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="97"/>
-      <c r="B61" s="98"/>
-      <c r="C61" s="98"/>
-      <c r="D61" s="76"/>
-      <c r="E61" s="78"/>
+      <c r="A61" s="126"/>
+      <c r="B61" s="127"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="131"/>
+      <c r="E61" s="133"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="125">
-    <mergeCell ref="BD48:BD51"/>
-    <mergeCell ref="BD52:BD55"/>
-    <mergeCell ref="BD56:BD59"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
+  <mergeCells count="124">
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="BD8:BD11"/>
+    <mergeCell ref="BD12:BD21"/>
+    <mergeCell ref="BD22:BD23"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="BB4:BC59"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="A10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -5438,89 +5523,24 @@
     <mergeCell ref="Z1:AD1"/>
     <mergeCell ref="AE1:AI1"/>
     <mergeCell ref="P2:T2"/>
-    <mergeCell ref="BB4:BC59"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="BD3:BD7"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="BD8:BD11"/>
-    <mergeCell ref="BD12:BD21"/>
-    <mergeCell ref="BD22:BD23"/>
-    <mergeCell ref="BD24:BD47"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD50:BD53"/>
+    <mergeCell ref="BD46:BD49"/>
+    <mergeCell ref="BD24:BD45"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Klasse PU mit allen Buttons Realisiert
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="615" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2B3F617-BFE9-45E2-95FC-A402E50A73C0}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E448FC1-0AE1-4A74-A945-2F3A1E959DD1}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
@@ -1074,7 +1074,199 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1105,198 +1297,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1630,8 +1630,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:E37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB38" sqref="AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,171 +1643,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="78" t="s">
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="80" t="s">
+      <c r="E1" s="119"/>
+      <c r="F1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="86" t="s">
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="86" t="s">
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="86" t="s">
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="114"/>
+      <c r="Z1" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="86" t="s">
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="113"/>
+      <c r="AC1" s="113"/>
+      <c r="AD1" s="114"/>
+      <c r="AE1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="87"/>
-      <c r="AG1" s="87"/>
-      <c r="AH1" s="87"/>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="86" t="s">
+      <c r="AF1" s="113"/>
+      <c r="AG1" s="113"/>
+      <c r="AH1" s="113"/>
+      <c r="AI1" s="114"/>
+      <c r="AJ1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="87"/>
-      <c r="AL1" s="87"/>
-      <c r="AM1" s="87"/>
-      <c r="AN1" s="88"/>
-      <c r="AO1" s="86" t="s">
+      <c r="AK1" s="113"/>
+      <c r="AL1" s="113"/>
+      <c r="AM1" s="113"/>
+      <c r="AN1" s="114"/>
+      <c r="AO1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="87"/>
-      <c r="AQ1" s="87"/>
-      <c r="AR1" s="87"/>
-      <c r="AS1" s="88"/>
-      <c r="AT1" s="86" t="s">
+      <c r="AP1" s="113"/>
+      <c r="AQ1" s="113"/>
+      <c r="AR1" s="113"/>
+      <c r="AS1" s="114"/>
+      <c r="AT1" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="87"/>
-      <c r="AV1" s="87"/>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="88"/>
-      <c r="AY1" s="86" t="s">
+      <c r="AU1" s="113"/>
+      <c r="AV1" s="113"/>
+      <c r="AW1" s="113"/>
+      <c r="AX1" s="114"/>
+      <c r="AY1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="87"/>
-      <c r="BA1" s="87"/>
-      <c r="BB1" s="87"/>
-      <c r="BC1" s="88"/>
-      <c r="BD1" s="61" t="s">
+      <c r="AZ1" s="113"/>
+      <c r="BA1" s="113"/>
+      <c r="BB1" s="113"/>
+      <c r="BC1" s="114"/>
+      <c r="BD1" s="71" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="83">
+      <c r="A2" s="116"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="123">
         <v>44957</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="72">
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="109">
         <v>44958</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="72">
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="109">
         <v>44959</v>
       </c>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="72">
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="109">
         <v>44960</v>
       </c>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="72">
+      <c r="V2" s="110"/>
+      <c r="W2" s="110"/>
+      <c r="X2" s="110"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="109">
         <v>44964</v>
       </c>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="74"/>
-      <c r="AE2" s="72">
+      <c r="AA2" s="110"/>
+      <c r="AB2" s="110"/>
+      <c r="AC2" s="110"/>
+      <c r="AD2" s="111"/>
+      <c r="AE2" s="109">
         <v>44965</v>
       </c>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="72">
+      <c r="AF2" s="110"/>
+      <c r="AG2" s="110"/>
+      <c r="AH2" s="110"/>
+      <c r="AI2" s="111"/>
+      <c r="AJ2" s="109">
         <v>44966</v>
       </c>
-      <c r="AK2" s="73"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="73"/>
-      <c r="AN2" s="74"/>
-      <c r="AO2" s="72">
+      <c r="AK2" s="110"/>
+      <c r="AL2" s="110"/>
+      <c r="AM2" s="110"/>
+      <c r="AN2" s="111"/>
+      <c r="AO2" s="109">
         <v>44967</v>
       </c>
-      <c r="AP2" s="73"/>
-      <c r="AQ2" s="73"/>
-      <c r="AR2" s="73"/>
-      <c r="AS2" s="74"/>
-      <c r="AT2" s="72">
+      <c r="AP2" s="110"/>
+      <c r="AQ2" s="110"/>
+      <c r="AR2" s="110"/>
+      <c r="AS2" s="111"/>
+      <c r="AT2" s="109">
         <v>44971</v>
       </c>
-      <c r="AU2" s="73"/>
-      <c r="AV2" s="73"/>
-      <c r="AW2" s="73"/>
-      <c r="AX2" s="74"/>
-      <c r="AY2" s="72">
+      <c r="AU2" s="110"/>
+      <c r="AV2" s="110"/>
+      <c r="AW2" s="110"/>
+      <c r="AX2" s="111"/>
+      <c r="AY2" s="109">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="73"/>
-      <c r="BA2" s="73"/>
-      <c r="BB2" s="73"/>
-      <c r="BC2" s="74"/>
-      <c r="BD2" s="61"/>
+      <c r="AZ2" s="110"/>
+      <c r="BA2" s="110"/>
+      <c r="BB2" s="110"/>
+      <c r="BC2" s="111"/>
+      <c r="BD2" s="71"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
+      <c r="A3" s="117"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1964,18 +1964,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="134"/>
+      <c r="BD3" s="68"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="107">
+      <c r="B4" s="105"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="62">
         <v>30</v>
       </c>
-      <c r="E4" s="109"/>
+      <c r="E4" s="73"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -2024,18 +2024,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="113" t="s">
+      <c r="BB4" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="134"/>
+      <c r="BC4" s="101"/>
+      <c r="BD4" s="68"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="104"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="110"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="74"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2084,24 +2084,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="113"/>
-      <c r="BC5" s="114"/>
-      <c r="BD5" s="134"/>
-      <c r="BF5" s="62" t="s">
+      <c r="BB5" s="100"/>
+      <c r="BC5" s="101"/>
+      <c r="BD5" s="68"/>
+      <c r="BF5" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="66"/>
+      <c r="BG5" s="130"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="97">
+      <c r="B6" s="81"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="66">
         <v>1</v>
       </c>
-      <c r="E6" s="111">
+      <c r="E6" s="107">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2152,18 +2152,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="113"/>
-      <c r="BC6" s="114"/>
-      <c r="BD6" s="134"/>
-      <c r="BF6" s="63"/>
-      <c r="BG6" s="67"/>
+      <c r="BB6" s="100"/>
+      <c r="BC6" s="101"/>
+      <c r="BD6" s="68"/>
+      <c r="BF6" s="127"/>
+      <c r="BG6" s="131"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="94"/>
-      <c r="B7" s="95"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="112"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="108"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2212,24 +2212,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="113"/>
-      <c r="BC7" s="114"/>
-      <c r="BD7" s="134"/>
-      <c r="BF7" s="62" t="s">
+      <c r="BB7" s="100"/>
+      <c r="BC7" s="101"/>
+      <c r="BD7" s="68"/>
+      <c r="BF7" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="68"/>
+      <c r="BG7" s="132"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="101" t="s">
+      <c r="A8" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="102"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="107">
+      <c r="B8" s="105"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="62">
         <v>1.5</v>
       </c>
-      <c r="E8" s="89">
+      <c r="E8" s="64">
         <v>0.8</v>
       </c>
       <c r="F8" s="17"/>
@@ -2280,20 +2280,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="113"/>
-      <c r="BC8" s="114"/>
-      <c r="BD8" s="61" t="s">
+      <c r="BB8" s="100"/>
+      <c r="BC8" s="101"/>
+      <c r="BD8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="63"/>
-      <c r="BG8" s="69"/>
+      <c r="BF8" s="127"/>
+      <c r="BG8" s="133"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="90"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="70"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2342,24 +2342,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="113"/>
-      <c r="BC9" s="114"/>
-      <c r="BD9" s="61"/>
-      <c r="BF9" s="64" t="s">
+      <c r="BB9" s="100"/>
+      <c r="BC9" s="101"/>
+      <c r="BD9" s="71"/>
+      <c r="BF9" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="70"/>
+      <c r="BG9" s="134"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="97">
+      <c r="B10" s="81"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="66">
         <v>1.5</v>
       </c>
-      <c r="E10" s="99">
+      <c r="E10" s="67">
         <v>0.8</v>
       </c>
       <c r="F10" s="19"/>
@@ -2410,18 +2410,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="113"/>
-      <c r="BC10" s="114"/>
-      <c r="BD10" s="61"/>
-      <c r="BF10" s="65"/>
-      <c r="BG10" s="71"/>
+      <c r="BB10" s="100"/>
+      <c r="BC10" s="101"/>
+      <c r="BD10" s="71"/>
+      <c r="BF10" s="129"/>
+      <c r="BG10" s="135"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="94"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="100"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="65"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2470,20 +2470,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="113"/>
-      <c r="BC11" s="114"/>
-      <c r="BD11" s="61"/>
+      <c r="BB11" s="100"/>
+      <c r="BC11" s="101"/>
+      <c r="BD11" s="71"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="102"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="107">
+      <c r="B12" s="105"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="62">
         <v>1</v>
       </c>
-      <c r="E12" s="89">
+      <c r="E12" s="64">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2534,9 +2534,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="113"/>
-      <c r="BC12" s="114"/>
-      <c r="BD12" s="61" t="s">
+      <c r="BB12" s="100"/>
+      <c r="BC12" s="101"/>
+      <c r="BD12" s="71" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2550,11 +2550,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="104"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="108"/>
-      <c r="E13" s="90"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2603,9 +2603,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="113"/>
-      <c r="BC13" s="114"/>
-      <c r="BD13" s="61"/>
+      <c r="BB13" s="100"/>
+      <c r="BC13" s="101"/>
+      <c r="BD13" s="71"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2617,15 +2617,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="97">
+      <c r="B14" s="81"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="66">
         <v>2</v>
       </c>
-      <c r="E14" s="99">
+      <c r="E14" s="67">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2676,16 +2676,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="113"/>
-      <c r="BC14" s="114"/>
-      <c r="BD14" s="61"/>
+      <c r="BB14" s="100"/>
+      <c r="BC14" s="101"/>
+      <c r="BD14" s="71"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104"/>
-      <c r="B15" s="105"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="90"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2734,20 +2734,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="113"/>
-      <c r="BC15" s="114"/>
-      <c r="BD15" s="61"/>
+      <c r="BB15" s="100"/>
+      <c r="BC15" s="101"/>
+      <c r="BD15" s="71"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="97">
+      <c r="B16" s="81"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="66">
         <v>1</v>
       </c>
-      <c r="E16" s="99">
+      <c r="E16" s="67">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2798,16 +2798,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="113"/>
-      <c r="BC16" s="114"/>
-      <c r="BD16" s="61"/>
+      <c r="BB16" s="100"/>
+      <c r="BC16" s="101"/>
+      <c r="BD16" s="71"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="104"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="90"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2856,23 +2856,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="113"/>
-      <c r="BC17" s="114"/>
-      <c r="BD17" s="61"/>
+      <c r="BB17" s="100"/>
+      <c r="BC17" s="101"/>
+      <c r="BD17" s="71"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="91" t="s">
+      <c r="A18" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="97">
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="66">
         <v>2</v>
       </c>
-      <c r="E18" s="99">
+      <c r="E18" s="67">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2923,16 +2923,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="113"/>
-      <c r="BC18" s="114"/>
-      <c r="BD18" s="61"/>
+      <c r="BB18" s="100"/>
+      <c r="BC18" s="101"/>
+      <c r="BD18" s="71"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="104"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="106"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="90"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -2981,20 +2981,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="113"/>
-      <c r="BC19" s="114"/>
-      <c r="BD19" s="61"/>
+      <c r="BB19" s="100"/>
+      <c r="BC19" s="101"/>
+      <c r="BD19" s="71"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="97">
+      <c r="B20" s="81"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="66">
         <v>1</v>
       </c>
-      <c r="E20" s="99">
+      <c r="E20" s="67">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3045,16 +3045,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="113"/>
-      <c r="BC20" s="114"/>
-      <c r="BD20" s="61"/>
+      <c r="BB20" s="100"/>
+      <c r="BC20" s="101"/>
+      <c r="BD20" s="71"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="94"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="100"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="65"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3103,20 +3103,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="113"/>
-      <c r="BC21" s="114"/>
-      <c r="BD21" s="61"/>
+      <c r="BB21" s="100"/>
+      <c r="BC21" s="101"/>
+      <c r="BD21" s="71"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="102"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="107">
+      <c r="B22" s="105"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="62">
         <v>0.5</v>
       </c>
-      <c r="E22" s="89">
+      <c r="E22" s="64">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3167,18 +3167,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="113"/>
-      <c r="BC22" s="114"/>
-      <c r="BD22" s="61" t="s">
+      <c r="BB22" s="100"/>
+      <c r="BC22" s="101"/>
+      <c r="BD22" s="71" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="94"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="100"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3227,20 +3227,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="113"/>
-      <c r="BC23" s="114"/>
-      <c r="BD23" s="61"/>
+      <c r="BB23" s="100"/>
+      <c r="BC23" s="101"/>
+      <c r="BD23" s="71"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="102"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="107">
+      <c r="B24" s="105"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="62">
         <v>2</v>
       </c>
-      <c r="E24" s="89">
+      <c r="E24" s="64">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3291,18 +3291,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="113"/>
-      <c r="BC24" s="114"/>
+      <c r="BB24" s="100"/>
+      <c r="BC24" s="101"/>
       <c r="BD24" s="136" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="104"/>
-      <c r="B25" s="105"/>
-      <c r="C25" s="106"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="90"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="70"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3351,20 +3351,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="113"/>
-      <c r="BC25" s="114"/>
+      <c r="BB25" s="100"/>
+      <c r="BC25" s="101"/>
       <c r="BD25" s="137"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="92"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="97">
+      <c r="B26" s="81"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="66">
         <v>1</v>
       </c>
-      <c r="E26" s="99">
+      <c r="E26" s="67">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3415,16 +3415,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="113"/>
-      <c r="BC26" s="114"/>
+      <c r="BB26" s="100"/>
+      <c r="BC26" s="101"/>
       <c r="BD26" s="137"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="104"/>
-      <c r="B27" s="105"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="90"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="70"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3473,20 +3473,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="113"/>
-      <c r="BC27" s="114"/>
+      <c r="BB27" s="100"/>
+      <c r="BC27" s="101"/>
       <c r="BD27" s="137"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="91" t="s">
+      <c r="A28" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="92"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="97">
+      <c r="B28" s="81"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="66">
         <v>2</v>
       </c>
-      <c r="E28" s="99">
+      <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3537,16 +3537,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="113"/>
-      <c r="BC28" s="114"/>
+      <c r="BB28" s="100"/>
+      <c r="BC28" s="101"/>
       <c r="BD28" s="137"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="104"/>
-      <c r="B29" s="105"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="90"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="70"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3595,20 +3595,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="113"/>
-      <c r="BC29" s="114"/>
+      <c r="BB29" s="100"/>
+      <c r="BC29" s="101"/>
       <c r="BD29" s="137"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="97">
+      <c r="B30" s="81"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="66">
         <v>2</v>
       </c>
-      <c r="E30" s="99">
+      <c r="E30" s="67">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3659,16 +3659,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="113"/>
-      <c r="BC30" s="114"/>
+      <c r="BB30" s="100"/>
+      <c r="BC30" s="101"/>
       <c r="BD30" s="137"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="104"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="106"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="90"/>
+      <c r="A31" s="83"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="70"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3717,20 +3717,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="113"/>
-      <c r="BC31" s="114"/>
+      <c r="BB31" s="100"/>
+      <c r="BC31" s="101"/>
       <c r="BD31" s="137"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="93"/>
-      <c r="D32" s="97">
+      <c r="B32" s="81"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="66">
         <v>4</v>
       </c>
-      <c r="E32" s="99">
+      <c r="E32" s="67">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3781,16 +3781,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="113"/>
-      <c r="BC32" s="114"/>
+      <c r="BB32" s="100"/>
+      <c r="BC32" s="101"/>
       <c r="BD32" s="137"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="104"/>
-      <c r="B33" s="105"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="90"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="70"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3839,20 +3839,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="113"/>
-      <c r="BC33" s="114"/>
+      <c r="BB33" s="100"/>
+      <c r="BC33" s="101"/>
       <c r="BD33" s="137"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="91" t="s">
+      <c r="A34" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="92"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="97">
+      <c r="B34" s="81"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="66">
         <v>3</v>
       </c>
-      <c r="E34" s="99">
+      <c r="E34" s="67">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3903,16 +3903,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="113"/>
-      <c r="BC34" s="114"/>
+      <c r="BB34" s="100"/>
+      <c r="BC34" s="101"/>
       <c r="BD34" s="137"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="104"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="90"/>
+      <c r="A35" s="83"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="70"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3961,20 +3961,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="113"/>
-      <c r="BC35" s="114"/>
+      <c r="BB35" s="100"/>
+      <c r="BC35" s="101"/>
       <c r="BD35" s="137"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="91" t="s">
+      <c r="A36" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="92"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="97">
+      <c r="B36" s="81"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="66">
         <v>4</v>
       </c>
-      <c r="E36" s="99"/>
+      <c r="E36" s="67"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -4022,16 +4022,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="113"/>
-      <c r="BC36" s="114"/>
+      <c r="BB36" s="100"/>
+      <c r="BC36" s="101"/>
       <c r="BD36" s="137"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="104"/>
-      <c r="B37" s="105"/>
-      <c r="C37" s="106"/>
-      <c r="D37" s="108"/>
-      <c r="E37" s="90"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="70"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4080,20 +4080,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="113"/>
-      <c r="BC37" s="114"/>
+      <c r="BB37" s="100"/>
+      <c r="BC37" s="101"/>
       <c r="BD37" s="137"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="92"/>
-      <c r="C38" s="93"/>
-      <c r="D38" s="97">
+      <c r="B38" s="81"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="66">
         <v>1</v>
       </c>
-      <c r="E38" s="99"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -4111,8 +4111,7 @@
       <c r="T38" s="4"/>
       <c r="U38" s="8"/>
       <c r="V38" s="24"/>
-      <c r="W38" s="24"/>
-      <c r="X38" s="18"/>
+      <c r="W38" s="18"/>
       <c r="Y38" s="4"/>
       <c r="AA38" s="9"/>
       <c r="AB38" s="9"/>
@@ -4141,16 +4140,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="113"/>
-      <c r="BC38" s="114"/>
+      <c r="BB38" s="100"/>
+      <c r="BC38" s="101"/>
       <c r="BD38" s="137"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="104"/>
-      <c r="B39" s="105"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="108"/>
-      <c r="E39" s="90"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4199,20 +4198,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="113"/>
-      <c r="BC39" s="114"/>
+      <c r="BB39" s="100"/>
+      <c r="BC39" s="101"/>
       <c r="BD39" s="137"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="92"/>
-      <c r="C40" s="93"/>
-      <c r="D40" s="97">
+      <c r="B40" s="81"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="66">
         <v>1</v>
       </c>
-      <c r="E40" s="99"/>
+      <c r="E40" s="67"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -4262,16 +4261,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="113"/>
-      <c r="BC40" s="114"/>
+      <c r="BB40" s="100"/>
+      <c r="BC40" s="101"/>
       <c r="BD40" s="137"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="104"/>
-      <c r="B41" s="105"/>
-      <c r="C41" s="106"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="90"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4320,20 +4319,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="113"/>
-      <c r="BC41" s="114"/>
+      <c r="BB41" s="100"/>
+      <c r="BC41" s="101"/>
       <c r="BD41" s="137"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="92"/>
-      <c r="C42" s="93"/>
-      <c r="D42" s="97">
+      <c r="B42" s="81"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="66">
         <v>2</v>
       </c>
-      <c r="E42" s="99"/>
+      <c r="E42" s="67"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -4382,16 +4381,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="113"/>
-      <c r="BC42" s="114"/>
+      <c r="BB42" s="100"/>
+      <c r="BC42" s="101"/>
       <c r="BD42" s="137"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="104"/>
-      <c r="B43" s="105"/>
-      <c r="C43" s="106"/>
-      <c r="D43" s="108"/>
-      <c r="E43" s="90"/>
+      <c r="A43" s="83"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="70"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4440,20 +4439,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="113"/>
-      <c r="BC43" s="114"/>
+      <c r="BB43" s="100"/>
+      <c r="BC43" s="101"/>
       <c r="BD43" s="137"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="91" t="s">
+      <c r="A44" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="92"/>
-      <c r="C44" s="93"/>
-      <c r="D44" s="97">
+      <c r="B44" s="81"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="66">
         <v>2</v>
       </c>
-      <c r="E44" s="99"/>
+      <c r="E44" s="67"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4502,16 +4501,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="113"/>
-      <c r="BC44" s="114"/>
+      <c r="BB44" s="100"/>
+      <c r="BC44" s="101"/>
       <c r="BD44" s="137"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="94"/>
-      <c r="B45" s="95"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="98"/>
-      <c r="E45" s="100"/>
+      <c r="A45" s="90"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="65"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4560,20 +4559,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="113"/>
-      <c r="BC45" s="114"/>
+      <c r="BB45" s="100"/>
+      <c r="BC45" s="101"/>
       <c r="BD45" s="138"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="121" t="s">
+      <c r="A46" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="122"/>
-      <c r="C46" s="123"/>
-      <c r="D46" s="128">
+      <c r="B46" s="94"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="72">
         <v>1</v>
       </c>
-      <c r="E46" s="109"/>
+      <c r="E46" s="73"/>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4621,18 +4620,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="113"/>
-      <c r="BC46" s="114"/>
-      <c r="BD46" s="61" t="s">
+      <c r="BB46" s="100"/>
+      <c r="BC46" s="101"/>
+      <c r="BD46" s="71" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="104"/>
-      <c r="B47" s="105"/>
-      <c r="C47" s="106"/>
-      <c r="D47" s="108"/>
-      <c r="E47" s="110"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="85"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="74"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4681,20 +4680,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="113"/>
-      <c r="BC47" s="114"/>
-      <c r="BD47" s="61"/>
+      <c r="BB47" s="100"/>
+      <c r="BC47" s="101"/>
+      <c r="BD47" s="71"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="91" t="s">
+      <c r="A48" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="92"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="97">
+      <c r="B48" s="81"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="66">
         <v>2</v>
       </c>
-      <c r="E48" s="99"/>
+      <c r="E48" s="67"/>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4743,16 +4742,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="113"/>
-      <c r="BC48" s="114"/>
-      <c r="BD48" s="61"/>
+      <c r="BB48" s="100"/>
+      <c r="BC48" s="101"/>
+      <c r="BD48" s="71"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="94"/>
-      <c r="B49" s="95"/>
-      <c r="C49" s="96"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="100"/>
+      <c r="A49" s="90"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="65"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4801,20 +4800,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="113"/>
-      <c r="BC49" s="114"/>
-      <c r="BD49" s="61"/>
+      <c r="BB49" s="100"/>
+      <c r="BC49" s="101"/>
+      <c r="BD49" s="71"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="117" t="s">
+      <c r="A50" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="118"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="128">
+      <c r="B50" s="87"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="72">
         <v>5</v>
       </c>
-      <c r="E50" s="129"/>
+      <c r="E50" s="75"/>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4863,18 +4862,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="113"/>
-      <c r="BC50" s="114"/>
-      <c r="BD50" s="61" t="s">
+      <c r="BB50" s="100"/>
+      <c r="BC50" s="101"/>
+      <c r="BD50" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="119"/>
-      <c r="B51" s="120"/>
-      <c r="C51" s="120"/>
-      <c r="D51" s="108"/>
-      <c r="E51" s="90"/>
+      <c r="A51" s="88"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="70"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4923,20 +4922,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="113"/>
-      <c r="BC51" s="114"/>
-      <c r="BD51" s="61"/>
+      <c r="BB51" s="100"/>
+      <c r="BC51" s="101"/>
+      <c r="BD51" s="71"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="91" t="s">
+      <c r="A52" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="92"/>
-      <c r="C52" s="93"/>
-      <c r="D52" s="97">
+      <c r="B52" s="81"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="66">
         <v>2</v>
       </c>
-      <c r="E52" s="99"/>
+      <c r="E52" s="67"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -4977,16 +4976,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="23"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="113"/>
-      <c r="BC52" s="114"/>
-      <c r="BD52" s="61"/>
+      <c r="BB52" s="100"/>
+      <c r="BC52" s="101"/>
+      <c r="BD52" s="71"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="94"/>
-      <c r="B53" s="95"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="98"/>
-      <c r="E53" s="100"/>
+      <c r="A53" s="90"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="92"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="65"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5035,20 +5034,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="113"/>
-      <c r="BC53" s="114"/>
-      <c r="BD53" s="61"/>
+      <c r="BB53" s="100"/>
+      <c r="BC53" s="101"/>
+      <c r="BD53" s="71"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="121" t="s">
+      <c r="A54" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="122"/>
-      <c r="C54" s="123"/>
-      <c r="D54" s="128">
+      <c r="B54" s="94"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="72">
         <v>4.5</v>
       </c>
-      <c r="E54" s="129">
+      <c r="E54" s="75">
         <v>1</v>
       </c>
       <c r="F54" s="50"/>
@@ -5098,16 +5097,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="113"/>
-      <c r="BC54" s="114"/>
-      <c r="BD54" s="135"/>
+      <c r="BB54" s="100"/>
+      <c r="BC54" s="101"/>
+      <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="104"/>
-      <c r="B55" s="105"/>
-      <c r="C55" s="106"/>
-      <c r="D55" s="108"/>
-      <c r="E55" s="90"/>
+      <c r="A55" s="83"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="70"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5156,16 +5155,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="113"/>
-      <c r="BC55" s="114"/>
-      <c r="BD55" s="135"/>
+      <c r="BB55" s="100"/>
+      <c r="BC55" s="101"/>
+      <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="121"/>
-      <c r="B56" s="122"/>
-      <c r="C56" s="123"/>
-      <c r="D56" s="128"/>
-      <c r="E56" s="129"/>
+      <c r="A56" s="93"/>
+      <c r="B56" s="94"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="75"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5214,16 +5213,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="113"/>
-      <c r="BC56" s="114"/>
-      <c r="BD56" s="135"/>
+      <c r="BB56" s="100"/>
+      <c r="BC56" s="101"/>
+      <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="104"/>
-      <c r="B57" s="105"/>
-      <c r="C57" s="106"/>
-      <c r="D57" s="108"/>
-      <c r="E57" s="90"/>
+      <c r="A57" s="83"/>
+      <c r="B57" s="84"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="70"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5272,16 +5271,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="113"/>
-      <c r="BC57" s="114"/>
-      <c r="BD57" s="135"/>
+      <c r="BB57" s="100"/>
+      <c r="BC57" s="101"/>
+      <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="91"/>
-      <c r="B58" s="92"/>
-      <c r="C58" s="93"/>
-      <c r="D58" s="97"/>
-      <c r="E58" s="99"/>
+      <c r="A58" s="80"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="67"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5330,16 +5329,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="113"/>
-      <c r="BC58" s="114"/>
-      <c r="BD58" s="135"/>
+      <c r="BB58" s="100"/>
+      <c r="BC58" s="101"/>
+      <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="94"/>
-      <c r="B59" s="95"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="98"/>
-      <c r="E59" s="100"/>
+      <c r="A59" s="90"/>
+      <c r="B59" s="91"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="65"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5388,121 +5387,46 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="115"/>
-      <c r="BC59" s="116"/>
-      <c r="BD59" s="135"/>
+      <c r="BB59" s="102"/>
+      <c r="BC59" s="103"/>
+      <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="124" t="s">
+      <c r="A60" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="125"/>
-      <c r="C60" s="125"/>
-      <c r="D60" s="130">
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="76">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="132">
+      <c r="E60" s="78">
         <f>SUM(E4:E59)</f>
         <v>24.3</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="126"/>
-      <c r="B61" s="127"/>
-      <c r="C61" s="127"/>
-      <c r="D61" s="131"/>
-      <c r="E61" s="133"/>
+      <c r="A61" s="98"/>
+      <c r="B61" s="99"/>
+      <c r="C61" s="99"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="79"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="BD3:BD7"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="BD8:BD11"/>
-    <mergeCell ref="BD12:BD21"/>
-    <mergeCell ref="BD22:BD23"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="BB4:BC59"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
     <mergeCell ref="BD1:BD2"/>
     <mergeCell ref="A4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -5527,17 +5451,92 @@
     <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="AE2:AI2"/>
     <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="BD8:BD11"/>
+    <mergeCell ref="BD12:BD21"/>
+    <mergeCell ref="BD22:BD23"/>
+    <mergeCell ref="BB4:BC59"/>
     <mergeCell ref="BD50:BD53"/>
     <mergeCell ref="BD46:BD49"/>
     <mergeCell ref="BD24:BD45"/>

</xml_diff>

<commit_message>
PU,PUCalc,PUCalcItem Fertig gestellt und funktionieren auch miteinander. kurz angefangen mit From Settings
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="616" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E448FC1-0AE1-4A74-A945-2F3A1E959DD1}"/>
+  <xr:revisionPtr revIDLastSave="625" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86669F76-C564-4780-8851-1B8B5EE290A9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
+    <workbookView xWindow="29985" yWindow="45" windowWidth="26760" windowHeight="15420" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1076,120 +1076,216 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1201,102 +1297,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1631,7 +1631,7 @@
   <dimension ref="A1:BN62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
+      <selection activeCell="AE34" sqref="AE34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,171 +1643,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="118" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="119"/>
-      <c r="F1" s="120" t="s">
+      <c r="E1" s="63"/>
+      <c r="F1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="112" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="112" t="s">
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="112" t="s">
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="114"/>
-      <c r="Z1" s="112" t="s">
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="113"/>
-      <c r="AB1" s="113"/>
-      <c r="AC1" s="113"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="112" t="s">
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="113"/>
-      <c r="AG1" s="113"/>
-      <c r="AH1" s="113"/>
-      <c r="AI1" s="114"/>
-      <c r="AJ1" s="112" t="s">
+      <c r="AF1" s="74"/>
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="74"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="113"/>
-      <c r="AL1" s="113"/>
-      <c r="AM1" s="113"/>
-      <c r="AN1" s="114"/>
-      <c r="AO1" s="112" t="s">
+      <c r="AK1" s="74"/>
+      <c r="AL1" s="74"/>
+      <c r="AM1" s="74"/>
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="113"/>
-      <c r="AQ1" s="113"/>
-      <c r="AR1" s="113"/>
-      <c r="AS1" s="114"/>
-      <c r="AT1" s="112" t="s">
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="74"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="113"/>
-      <c r="AV1" s="113"/>
-      <c r="AW1" s="113"/>
-      <c r="AX1" s="114"/>
-      <c r="AY1" s="112" t="s">
+      <c r="AU1" s="74"/>
+      <c r="AV1" s="74"/>
+      <c r="AW1" s="74"/>
+      <c r="AX1" s="75"/>
+      <c r="AY1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="113"/>
-      <c r="BA1" s="113"/>
-      <c r="BB1" s="113"/>
-      <c r="BC1" s="114"/>
-      <c r="BD1" s="71" t="s">
+      <c r="AZ1" s="74"/>
+      <c r="BA1" s="74"/>
+      <c r="BB1" s="74"/>
+      <c r="BC1" s="75"/>
+      <c r="BD1" s="86" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="123">
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="67">
         <v>44957</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="109">
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70">
         <v>44958</v>
       </c>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="109">
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="70">
         <v>44959</v>
       </c>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="109">
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="70">
         <v>44960</v>
       </c>
-      <c r="V2" s="110"/>
-      <c r="W2" s="110"/>
-      <c r="X2" s="110"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="109">
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="70">
         <v>44964</v>
       </c>
-      <c r="AA2" s="110"/>
-      <c r="AB2" s="110"/>
-      <c r="AC2" s="110"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="109">
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="72"/>
+      <c r="AE2" s="70">
         <v>44965</v>
       </c>
-      <c r="AF2" s="110"/>
-      <c r="AG2" s="110"/>
-      <c r="AH2" s="110"/>
-      <c r="AI2" s="111"/>
-      <c r="AJ2" s="109">
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="72"/>
+      <c r="AJ2" s="70">
         <v>44966</v>
       </c>
-      <c r="AK2" s="110"/>
-      <c r="AL2" s="110"/>
-      <c r="AM2" s="110"/>
-      <c r="AN2" s="111"/>
-      <c r="AO2" s="109">
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="72"/>
+      <c r="AO2" s="70">
         <v>44967</v>
       </c>
-      <c r="AP2" s="110"/>
-      <c r="AQ2" s="110"/>
-      <c r="AR2" s="110"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="109">
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="72"/>
+      <c r="AT2" s="70">
         <v>44971</v>
       </c>
-      <c r="AU2" s="110"/>
-      <c r="AV2" s="110"/>
-      <c r="AW2" s="110"/>
-      <c r="AX2" s="111"/>
-      <c r="AY2" s="109">
+      <c r="AU2" s="71"/>
+      <c r="AV2" s="71"/>
+      <c r="AW2" s="71"/>
+      <c r="AX2" s="72"/>
+      <c r="AY2" s="70">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="110"/>
-      <c r="BA2" s="110"/>
-      <c r="BB2" s="110"/>
-      <c r="BC2" s="111"/>
-      <c r="BD2" s="71"/>
+      <c r="AZ2" s="71"/>
+      <c r="BA2" s="71"/>
+      <c r="BB2" s="71"/>
+      <c r="BC2" s="72"/>
+      <c r="BD2" s="86"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="117"/>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
+      <c r="A3" s="109"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1964,18 +1964,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="68"/>
+      <c r="BD3" s="131"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="62">
+      <c r="B4" s="88"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="93">
         <v>30</v>
       </c>
-      <c r="E4" s="73"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -2024,18 +2024,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="100" t="s">
+      <c r="BB4" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="101"/>
-      <c r="BD4" s="68"/>
+      <c r="BC4" s="133"/>
+      <c r="BD4" s="131"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="74"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="96"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2084,24 +2084,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="100"/>
-      <c r="BC5" s="101"/>
-      <c r="BD5" s="68"/>
-      <c r="BF5" s="126" t="s">
+      <c r="BB5" s="132"/>
+      <c r="BC5" s="133"/>
+      <c r="BD5" s="131"/>
+      <c r="BF5" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="130"/>
+      <c r="BG5" s="80"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="66">
+      <c r="B6" s="98"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="103">
         <v>1</v>
       </c>
-      <c r="E6" s="107">
+      <c r="E6" s="105">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2152,18 +2152,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="100"/>
-      <c r="BC6" s="101"/>
-      <c r="BD6" s="68"/>
-      <c r="BF6" s="127"/>
-      <c r="BG6" s="131"/>
+      <c r="BB6" s="132"/>
+      <c r="BC6" s="133"/>
+      <c r="BD6" s="131"/>
+      <c r="BF6" s="77"/>
+      <c r="BG6" s="81"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="108"/>
+      <c r="A7" s="100"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="106"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2212,24 +2212,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="100"/>
-      <c r="BC7" s="101"/>
-      <c r="BD7" s="68"/>
-      <c r="BF7" s="126" t="s">
+      <c r="BB7" s="132"/>
+      <c r="BC7" s="133"/>
+      <c r="BD7" s="131"/>
+      <c r="BF7" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="132"/>
+      <c r="BG7" s="82"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="62">
+      <c r="B8" s="88"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="93">
         <v>1.5</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="110">
         <v>0.8</v>
       </c>
       <c r="F8" s="17"/>
@@ -2280,20 +2280,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="100"/>
-      <c r="BC8" s="101"/>
-      <c r="BD8" s="71" t="s">
+      <c r="BB8" s="132"/>
+      <c r="BC8" s="133"/>
+      <c r="BD8" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="127"/>
-      <c r="BG8" s="133"/>
+      <c r="BF8" s="77"/>
+      <c r="BG8" s="83"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="111"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2342,24 +2342,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="100"/>
-      <c r="BC9" s="101"/>
-      <c r="BD9" s="71"/>
-      <c r="BF9" s="128" t="s">
+      <c r="BB9" s="132"/>
+      <c r="BC9" s="133"/>
+      <c r="BD9" s="86"/>
+      <c r="BF9" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="134"/>
+      <c r="BG9" s="84"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="66">
+      <c r="B10" s="98"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="103">
         <v>1.5</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="112">
         <v>0.8</v>
       </c>
       <c r="F10" s="19"/>
@@ -2410,18 +2410,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="100"/>
-      <c r="BC10" s="101"/>
-      <c r="BD10" s="71"/>
-      <c r="BF10" s="129"/>
-      <c r="BG10" s="135"/>
+      <c r="BB10" s="132"/>
+      <c r="BC10" s="133"/>
+      <c r="BD10" s="86"/>
+      <c r="BF10" s="79"/>
+      <c r="BG10" s="85"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90"/>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="65"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="113"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2470,20 +2470,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="100"/>
-      <c r="BC11" s="101"/>
-      <c r="BD11" s="71"/>
+      <c r="BB11" s="132"/>
+      <c r="BC11" s="133"/>
+      <c r="BD11" s="86"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="105"/>
-      <c r="C12" s="106"/>
-      <c r="D12" s="62">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="93">
         <v>1</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="110">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2534,9 +2534,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="100"/>
-      <c r="BC12" s="101"/>
-      <c r="BD12" s="71" t="s">
+      <c r="BB12" s="132"/>
+      <c r="BC12" s="133"/>
+      <c r="BD12" s="86" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2550,11 +2550,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="70"/>
+      <c r="A13" s="90"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="111"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2603,9 +2603,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="100"/>
-      <c r="BC13" s="101"/>
-      <c r="BD13" s="71"/>
+      <c r="BB13" s="132"/>
+      <c r="BC13" s="133"/>
+      <c r="BD13" s="86"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2617,15 +2617,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="81"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="66">
+      <c r="B14" s="98"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="103">
         <v>2</v>
       </c>
-      <c r="E14" s="67">
+      <c r="E14" s="112">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2676,16 +2676,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="100"/>
-      <c r="BC14" s="101"/>
-      <c r="BD14" s="71"/>
+      <c r="BB14" s="132"/>
+      <c r="BC14" s="133"/>
+      <c r="BD14" s="86"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="111"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2734,20 +2734,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="100"/>
-      <c r="BC15" s="101"/>
-      <c r="BD15" s="71"/>
+      <c r="BB15" s="132"/>
+      <c r="BC15" s="133"/>
+      <c r="BD15" s="86"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="66">
+      <c r="B16" s="98"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="103">
         <v>1</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="112">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2798,16 +2798,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="100"/>
-      <c r="BC16" s="101"/>
-      <c r="BD16" s="71"/>
+      <c r="BB16" s="132"/>
+      <c r="BC16" s="133"/>
+      <c r="BD16" s="86"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="83"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="70"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="111"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2856,23 +2856,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="100"/>
-      <c r="BC17" s="101"/>
-      <c r="BD17" s="71"/>
+      <c r="BB17" s="132"/>
+      <c r="BC17" s="133"/>
+      <c r="BD17" s="86"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="66">
+      <c r="B18" s="98"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="103">
         <v>2</v>
       </c>
-      <c r="E18" s="67">
+      <c r="E18" s="112">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2923,16 +2923,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="100"/>
-      <c r="BC18" s="101"/>
-      <c r="BD18" s="71"/>
+      <c r="BB18" s="132"/>
+      <c r="BC18" s="133"/>
+      <c r="BD18" s="86"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="83"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="70"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="111"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -2981,20 +2981,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="100"/>
-      <c r="BC19" s="101"/>
-      <c r="BD19" s="71"/>
+      <c r="BB19" s="132"/>
+      <c r="BC19" s="133"/>
+      <c r="BD19" s="86"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="66">
+      <c r="B20" s="98"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="103">
         <v>1</v>
       </c>
-      <c r="E20" s="67">
+      <c r="E20" s="112">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3045,16 +3045,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="100"/>
-      <c r="BC20" s="101"/>
-      <c r="BD20" s="71"/>
+      <c r="BB20" s="132"/>
+      <c r="BC20" s="133"/>
+      <c r="BD20" s="86"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="65"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="113"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3103,20 +3103,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="100"/>
-      <c r="BC21" s="101"/>
-      <c r="BD21" s="71"/>
+      <c r="BB21" s="132"/>
+      <c r="BC21" s="133"/>
+      <c r="BD21" s="86"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="62">
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="93">
         <v>0.5</v>
       </c>
-      <c r="E22" s="64">
+      <c r="E22" s="110">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3167,18 +3167,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="100"/>
-      <c r="BC22" s="101"/>
-      <c r="BD22" s="71" t="s">
+      <c r="BB22" s="132"/>
+      <c r="BC22" s="133"/>
+      <c r="BD22" s="86" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="90"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="65"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="113"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3227,20 +3227,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="100"/>
-      <c r="BC23" s="101"/>
-      <c r="BD23" s="71"/>
+      <c r="BB23" s="132"/>
+      <c r="BC23" s="133"/>
+      <c r="BD23" s="86"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="104" t="s">
+      <c r="A24" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="106"/>
-      <c r="D24" s="62">
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="93">
         <v>2</v>
       </c>
-      <c r="E24" s="64">
+      <c r="E24" s="110">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3291,18 +3291,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="100"/>
-      <c r="BC24" s="101"/>
+      <c r="BB24" s="132"/>
+      <c r="BC24" s="133"/>
       <c r="BD24" s="136" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="111"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3351,20 +3351,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="100"/>
-      <c r="BC25" s="101"/>
+      <c r="BB25" s="132"/>
+      <c r="BC25" s="133"/>
       <c r="BD25" s="137"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="66">
+      <c r="B26" s="98"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="103">
         <v>1</v>
       </c>
-      <c r="E26" s="67">
+      <c r="E26" s="112">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3415,16 +3415,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="100"/>
-      <c r="BC26" s="101"/>
+      <c r="BB26" s="132"/>
+      <c r="BC26" s="133"/>
       <c r="BD26" s="137"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="85"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="70"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="111"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3473,20 +3473,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="100"/>
-      <c r="BC27" s="101"/>
+      <c r="BB27" s="132"/>
+      <c r="BC27" s="133"/>
       <c r="BD27" s="137"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="80" t="s">
+      <c r="A28" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="66">
+      <c r="B28" s="98"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="103">
         <v>2</v>
       </c>
-      <c r="E28" s="67">
+      <c r="E28" s="112">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3537,16 +3537,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="100"/>
-      <c r="BC28" s="101"/>
+      <c r="BB28" s="132"/>
+      <c r="BC28" s="133"/>
       <c r="BD28" s="137"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="70"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="111"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3595,20 +3595,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="100"/>
-      <c r="BC29" s="101"/>
+      <c r="BB29" s="132"/>
+      <c r="BC29" s="133"/>
       <c r="BD29" s="137"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="66">
+      <c r="B30" s="98"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="103">
         <v>2</v>
       </c>
-      <c r="E30" s="67">
+      <c r="E30" s="112">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3659,16 +3659,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="100"/>
-      <c r="BC30" s="101"/>
+      <c r="BB30" s="132"/>
+      <c r="BC30" s="133"/>
       <c r="BD30" s="137"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="70"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="111"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3717,20 +3717,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="100"/>
-      <c r="BC31" s="101"/>
+      <c r="BB31" s="132"/>
+      <c r="BC31" s="133"/>
       <c r="BD31" s="137"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="81"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="66">
+      <c r="B32" s="98"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="103">
         <v>4</v>
       </c>
-      <c r="E32" s="67">
+      <c r="E32" s="112">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3781,16 +3781,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="100"/>
-      <c r="BC32" s="101"/>
+      <c r="BB32" s="132"/>
+      <c r="BC32" s="133"/>
       <c r="BD32" s="137"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="70"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="111"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3839,20 +3839,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="100"/>
-      <c r="BC33" s="101"/>
+      <c r="BB33" s="132"/>
+      <c r="BC33" s="133"/>
       <c r="BD33" s="137"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80" t="s">
+      <c r="A34" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="66">
+      <c r="B34" s="98"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="103">
         <v>3</v>
       </c>
-      <c r="E34" s="67">
+      <c r="E34" s="112">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3903,16 +3903,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="100"/>
-      <c r="BC34" s="101"/>
+      <c r="BB34" s="132"/>
+      <c r="BC34" s="133"/>
       <c r="BD34" s="137"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
-      <c r="B35" s="84"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="70"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="111"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3961,20 +3961,22 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="100"/>
-      <c r="BC35" s="101"/>
+      <c r="BB35" s="132"/>
+      <c r="BC35" s="133"/>
       <c r="BD35" s="137"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="80" t="s">
+      <c r="A36" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="81"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="66">
+      <c r="B36" s="98"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="103">
         <v>4</v>
       </c>
-      <c r="E36" s="67"/>
+      <c r="E36" s="112">
+        <v>4</v>
+      </c>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -4022,16 +4024,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="100"/>
-      <c r="BC36" s="101"/>
+      <c r="BB36" s="132"/>
+      <c r="BC36" s="133"/>
       <c r="BD36" s="137"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
-      <c r="B37" s="84"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="70"/>
+      <c r="A37" s="90"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="92"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="111"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4048,8 +4050,8 @@
       <c r="S37" s="9"/>
       <c r="T37" s="4"/>
       <c r="U37" s="8"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="4"/>
       <c r="Z37" s="8"/>
@@ -4080,20 +4082,22 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="100"/>
-      <c r="BC37" s="101"/>
+      <c r="BB37" s="132"/>
+      <c r="BC37" s="133"/>
       <c r="BD37" s="137"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="81"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="66">
+      <c r="B38" s="98"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="103">
         <v>1</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="112">
+        <v>1</v>
+      </c>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -4140,16 +4144,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="100"/>
-      <c r="BC38" s="101"/>
+      <c r="BB38" s="132"/>
+      <c r="BC38" s="133"/>
       <c r="BD38" s="137"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="84"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="70"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="111"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4167,7 +4171,7 @@
       <c r="T39" s="4"/>
       <c r="U39" s="8"/>
       <c r="V39" s="24"/>
-      <c r="W39" s="9"/>
+      <c r="W39" s="30"/>
       <c r="X39" s="9"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="8"/>
@@ -4198,20 +4202,22 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="100"/>
-      <c r="BC39" s="101"/>
+      <c r="BB39" s="132"/>
+      <c r="BC39" s="133"/>
       <c r="BD39" s="137"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="80" t="s">
+      <c r="A40" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="81"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="66">
+      <c r="B40" s="98"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="103">
         <v>1</v>
       </c>
-      <c r="E40" s="67"/>
+      <c r="E40" s="112">
+        <v>1</v>
+      </c>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -4261,16 +4267,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="100"/>
-      <c r="BC40" s="101"/>
+      <c r="BB40" s="132"/>
+      <c r="BC40" s="133"/>
       <c r="BD40" s="137"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
-      <c r="B41" s="84"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="70"/>
+      <c r="A41" s="90"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="111"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4289,7 +4295,7 @@
       <c r="U41" s="8"/>
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
-      <c r="X41" s="9"/>
+      <c r="X41" s="30"/>
       <c r="Y41" s="4"/>
       <c r="Z41" s="8"/>
       <c r="AA41" s="9"/>
@@ -4319,20 +4325,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="100"/>
-      <c r="BC41" s="101"/>
+      <c r="BB41" s="132"/>
+      <c r="BC41" s="133"/>
       <c r="BD41" s="137"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="80" t="s">
+      <c r="A42" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="66">
+      <c r="B42" s="98"/>
+      <c r="C42" s="99"/>
+      <c r="D42" s="103">
         <v>2</v>
       </c>
-      <c r="E42" s="67"/>
+      <c r="E42" s="112"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -4381,16 +4387,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="100"/>
-      <c r="BC42" s="101"/>
+      <c r="BB42" s="132"/>
+      <c r="BC42" s="133"/>
       <c r="BD42" s="137"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="83"/>
-      <c r="B43" s="84"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="70"/>
+      <c r="A43" s="90"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="111"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4409,7 +4415,7 @@
       <c r="U43" s="8"/>
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
-      <c r="X43" s="9"/>
+      <c r="X43" s="30"/>
       <c r="Y43" s="4"/>
       <c r="Z43" s="8"/>
       <c r="AA43" s="9"/>
@@ -4439,20 +4445,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="100"/>
-      <c r="BC43" s="101"/>
+      <c r="BB43" s="132"/>
+      <c r="BC43" s="133"/>
       <c r="BD43" s="137"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="80" t="s">
+      <c r="A44" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="81"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="66">
+      <c r="B44" s="98"/>
+      <c r="C44" s="99"/>
+      <c r="D44" s="103">
         <v>2</v>
       </c>
-      <c r="E44" s="67"/>
+      <c r="E44" s="112"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4501,16 +4507,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="100"/>
-      <c r="BC44" s="101"/>
+      <c r="BB44" s="132"/>
+      <c r="BC44" s="133"/>
       <c r="BD44" s="137"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="90"/>
-      <c r="B45" s="91"/>
-      <c r="C45" s="92"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="65"/>
+      <c r="A45" s="100"/>
+      <c r="B45" s="101"/>
+      <c r="C45" s="102"/>
+      <c r="D45" s="104"/>
+      <c r="E45" s="113"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4559,20 +4565,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="100"/>
-      <c r="BC45" s="101"/>
+      <c r="BB45" s="132"/>
+      <c r="BC45" s="133"/>
       <c r="BD45" s="138"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="93" t="s">
+      <c r="A46" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="94"/>
-      <c r="C46" s="95"/>
-      <c r="D46" s="72">
+      <c r="B46" s="125"/>
+      <c r="C46" s="126"/>
+      <c r="D46" s="118">
         <v>1</v>
       </c>
-      <c r="E46" s="73"/>
+      <c r="E46" s="95"/>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4620,18 +4626,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="100"/>
-      <c r="BC46" s="101"/>
-      <c r="BD46" s="71" t="s">
+      <c r="BB46" s="132"/>
+      <c r="BC46" s="133"/>
+      <c r="BD46" s="86" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="83"/>
-      <c r="B47" s="84"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="74"/>
+      <c r="A47" s="90"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="94"/>
+      <c r="E47" s="96"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4680,20 +4686,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="100"/>
-      <c r="BC47" s="101"/>
-      <c r="BD47" s="71"/>
+      <c r="BB47" s="132"/>
+      <c r="BC47" s="133"/>
+      <c r="BD47" s="86"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="66">
+      <c r="B48" s="98"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="103">
         <v>2</v>
       </c>
-      <c r="E48" s="67"/>
+      <c r="E48" s="112"/>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4742,16 +4748,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="100"/>
-      <c r="BC48" s="101"/>
-      <c r="BD48" s="71"/>
+      <c r="BB48" s="132"/>
+      <c r="BC48" s="133"/>
+      <c r="BD48" s="86"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="90"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="92"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="65"/>
+      <c r="A49" s="100"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="102"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="113"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4800,20 +4806,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="100"/>
-      <c r="BC49" s="101"/>
-      <c r="BD49" s="71"/>
+      <c r="BB49" s="132"/>
+      <c r="BC49" s="133"/>
+      <c r="BD49" s="86"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="86" t="s">
+      <c r="A50" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="87"/>
-      <c r="C50" s="87"/>
-      <c r="D50" s="72">
+      <c r="B50" s="121"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="118">
         <v>5</v>
       </c>
-      <c r="E50" s="75"/>
+      <c r="E50" s="119"/>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4862,18 +4868,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="100"/>
-      <c r="BC50" s="101"/>
-      <c r="BD50" s="71" t="s">
+      <c r="BB50" s="132"/>
+      <c r="BC50" s="133"/>
+      <c r="BD50" s="86" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="88"/>
-      <c r="B51" s="89"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="70"/>
+      <c r="A51" s="122"/>
+      <c r="B51" s="123"/>
+      <c r="C51" s="123"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="111"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4922,20 +4928,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="100"/>
-      <c r="BC51" s="101"/>
-      <c r="BD51" s="71"/>
+      <c r="BB51" s="132"/>
+      <c r="BC51" s="133"/>
+      <c r="BD51" s="86"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="80" t="s">
+      <c r="A52" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="81"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="66">
+      <c r="B52" s="98"/>
+      <c r="C52" s="99"/>
+      <c r="D52" s="103">
         <v>2</v>
       </c>
-      <c r="E52" s="67"/>
+      <c r="E52" s="112"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -4976,16 +4982,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="23"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="100"/>
-      <c r="BC52" s="101"/>
-      <c r="BD52" s="71"/>
+      <c r="BB52" s="132"/>
+      <c r="BC52" s="133"/>
+      <c r="BD52" s="86"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="90"/>
-      <c r="B53" s="91"/>
-      <c r="C53" s="92"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="65"/>
+      <c r="A53" s="100"/>
+      <c r="B53" s="101"/>
+      <c r="C53" s="102"/>
+      <c r="D53" s="104"/>
+      <c r="E53" s="113"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5034,20 +5040,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="100"/>
-      <c r="BC53" s="101"/>
-      <c r="BD53" s="71"/>
+      <c r="BB53" s="132"/>
+      <c r="BC53" s="133"/>
+      <c r="BD53" s="86"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="93" t="s">
+      <c r="A54" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="94"/>
-      <c r="C54" s="95"/>
-      <c r="D54" s="72">
+      <c r="B54" s="125"/>
+      <c r="C54" s="126"/>
+      <c r="D54" s="118">
         <v>4.5</v>
       </c>
-      <c r="E54" s="75">
+      <c r="E54" s="119">
         <v>1</v>
       </c>
       <c r="F54" s="50"/>
@@ -5097,16 +5103,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="100"/>
-      <c r="BC54" s="101"/>
+      <c r="BB54" s="132"/>
+      <c r="BC54" s="133"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="83"/>
-      <c r="B55" s="84"/>
-      <c r="C55" s="85"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="70"/>
+      <c r="A55" s="90"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="111"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5155,16 +5161,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="100"/>
-      <c r="BC55" s="101"/>
+      <c r="BB55" s="132"/>
+      <c r="BC55" s="133"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="93"/>
-      <c r="B56" s="94"/>
-      <c r="C56" s="95"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="75"/>
+      <c r="A56" s="124"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="126"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="119"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5213,16 +5219,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="100"/>
-      <c r="BC56" s="101"/>
+      <c r="BB56" s="132"/>
+      <c r="BC56" s="133"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="83"/>
-      <c r="B57" s="84"/>
-      <c r="C57" s="85"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="70"/>
+      <c r="A57" s="90"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="94"/>
+      <c r="E57" s="111"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5271,16 +5277,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="100"/>
-      <c r="BC57" s="101"/>
+      <c r="BB57" s="132"/>
+      <c r="BC57" s="133"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="80"/>
-      <c r="B58" s="81"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="67"/>
+      <c r="A58" s="97"/>
+      <c r="B58" s="98"/>
+      <c r="C58" s="99"/>
+      <c r="D58" s="103"/>
+      <c r="E58" s="112"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5329,16 +5335,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="100"/>
-      <c r="BC58" s="101"/>
+      <c r="BB58" s="132"/>
+      <c r="BC58" s="133"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="90"/>
-      <c r="B59" s="91"/>
-      <c r="C59" s="92"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="65"/>
+      <c r="A59" s="100"/>
+      <c r="B59" s="101"/>
+      <c r="C59" s="102"/>
+      <c r="D59" s="104"/>
+      <c r="E59" s="113"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5387,93 +5393,76 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="102"/>
-      <c r="BC59" s="103"/>
+      <c r="BB59" s="134"/>
+      <c r="BC59" s="135"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="97"/>
-      <c r="C60" s="97"/>
-      <c r="D60" s="76">
+      <c r="B60" s="128"/>
+      <c r="C60" s="128"/>
+      <c r="D60" s="114">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="78">
+      <c r="E60" s="116">
         <f>SUM(E4:E59)</f>
-        <v>24.3</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="98"/>
-      <c r="B61" s="99"/>
-      <c r="C61" s="99"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="79"/>
+      <c r="A61" s="129"/>
+      <c r="B61" s="130"/>
+      <c r="C61" s="130"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="117"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="BD8:BD11"/>
+    <mergeCell ref="BD12:BD21"/>
+    <mergeCell ref="BD22:BD23"/>
+    <mergeCell ref="BB4:BC59"/>
+    <mergeCell ref="BD50:BD53"/>
+    <mergeCell ref="BD46:BD49"/>
+    <mergeCell ref="BD24:BD45"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
     <mergeCell ref="D60:D61"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="D58:D59"/>
@@ -5498,48 +5487,65 @@
     <mergeCell ref="A38:C39"/>
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="BD3:BD7"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="BD8:BD11"/>
-    <mergeCell ref="BD12:BD21"/>
-    <mergeCell ref="BD22:BD23"/>
-    <mergeCell ref="BB4:BC59"/>
-    <mergeCell ref="BD50:BD53"/>
-    <mergeCell ref="BD46:BD49"/>
-    <mergeCell ref="BD24:BD45"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Abspeicherung vor Feierabend. Dokumentation, Arbeitsjournal geschrieben
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="625" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86669F76-C564-4780-8851-1B8B5EE290A9}"/>
+  <xr:revisionPtr revIDLastSave="637" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9454EDA-DBA2-47F3-9216-6724D0D371AA}"/>
   <bookViews>
     <workbookView xWindow="29985" yWindow="45" windowWidth="26760" windowHeight="15420" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
@@ -1009,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1076,6 +1076,183 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1100,24 +1277,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1148,164 +1307,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1630,8 +1649,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE34" sqref="AE34"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,171 +1662,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="62" t="s">
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64" t="s">
+      <c r="E1" s="122"/>
+      <c r="F1" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="73" t="s">
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="73" t="s">
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="73" t="s">
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="73" t="s">
+      <c r="V1" s="116"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="116"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="73" t="s">
+      <c r="AA1" s="116"/>
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="74"/>
-      <c r="AG1" s="74"/>
-      <c r="AH1" s="74"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="73" t="s">
+      <c r="AF1" s="116"/>
+      <c r="AG1" s="116"/>
+      <c r="AH1" s="116"/>
+      <c r="AI1" s="117"/>
+      <c r="AJ1" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="74"/>
-      <c r="AL1" s="74"/>
-      <c r="AM1" s="74"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="73" t="s">
+      <c r="AK1" s="116"/>
+      <c r="AL1" s="116"/>
+      <c r="AM1" s="116"/>
+      <c r="AN1" s="117"/>
+      <c r="AO1" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="74"/>
-      <c r="AQ1" s="74"/>
-      <c r="AR1" s="74"/>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="73" t="s">
+      <c r="AP1" s="116"/>
+      <c r="AQ1" s="116"/>
+      <c r="AR1" s="116"/>
+      <c r="AS1" s="117"/>
+      <c r="AT1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="74"/>
-      <c r="AV1" s="74"/>
-      <c r="AW1" s="74"/>
-      <c r="AX1" s="75"/>
-      <c r="AY1" s="73" t="s">
+      <c r="AU1" s="116"/>
+      <c r="AV1" s="116"/>
+      <c r="AW1" s="116"/>
+      <c r="AX1" s="117"/>
+      <c r="AY1" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="74"/>
-      <c r="BA1" s="74"/>
-      <c r="BB1" s="74"/>
-      <c r="BC1" s="75"/>
-      <c r="BD1" s="86" t="s">
+      <c r="AZ1" s="116"/>
+      <c r="BA1" s="116"/>
+      <c r="BB1" s="116"/>
+      <c r="BC1" s="117"/>
+      <c r="BD1" s="71" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="67">
+      <c r="A2" s="119"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="126">
         <v>44957</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="70">
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="112">
         <v>44958</v>
       </c>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="70">
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="112">
         <v>44959</v>
       </c>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="70">
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="114"/>
+      <c r="U2" s="112">
         <v>44960</v>
       </c>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="70">
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="114"/>
+      <c r="Z2" s="112">
         <v>44964</v>
       </c>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="70">
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="114"/>
+      <c r="AE2" s="112">
         <v>44965</v>
       </c>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="71"/>
-      <c r="AI2" s="72"/>
-      <c r="AJ2" s="70">
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
+      <c r="AH2" s="113"/>
+      <c r="AI2" s="114"/>
+      <c r="AJ2" s="112">
         <v>44966</v>
       </c>
-      <c r="AK2" s="71"/>
-      <c r="AL2" s="71"/>
-      <c r="AM2" s="71"/>
-      <c r="AN2" s="72"/>
-      <c r="AO2" s="70">
+      <c r="AK2" s="113"/>
+      <c r="AL2" s="113"/>
+      <c r="AM2" s="113"/>
+      <c r="AN2" s="114"/>
+      <c r="AO2" s="112">
         <v>44967</v>
       </c>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="71"/>
-      <c r="AS2" s="72"/>
-      <c r="AT2" s="70">
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="113"/>
+      <c r="AR2" s="113"/>
+      <c r="AS2" s="114"/>
+      <c r="AT2" s="112">
         <v>44971</v>
       </c>
-      <c r="AU2" s="71"/>
-      <c r="AV2" s="71"/>
-      <c r="AW2" s="71"/>
-      <c r="AX2" s="72"/>
-      <c r="AY2" s="70">
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="114"/>
+      <c r="AY2" s="112">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="71"/>
-      <c r="BA2" s="71"/>
-      <c r="BB2" s="71"/>
-      <c r="BC2" s="72"/>
-      <c r="BD2" s="86"/>
+      <c r="AZ2" s="113"/>
+      <c r="BA2" s="113"/>
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="114"/>
+      <c r="BD2" s="71"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="109"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
+      <c r="A3" s="120"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1964,18 +1983,20 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="131"/>
+      <c r="BD3" s="67"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="93">
+      <c r="B4" s="108"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="70">
         <v>30</v>
       </c>
-      <c r="E4" s="95"/>
+      <c r="E4" s="80">
+        <v>30</v>
+      </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -2024,18 +2045,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="132" t="s">
+      <c r="BB4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="133"/>
-      <c r="BD4" s="131"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="67"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="90"/>
       <c r="B5" s="91"/>
       <c r="C5" s="92"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="96"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2051,10 +2072,10 @@
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
       <c r="T5" s="47"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
+      <c r="U5" s="142"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="9"/>
@@ -2084,24 +2105,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="132"/>
-      <c r="BC5" s="133"/>
-      <c r="BD5" s="131"/>
-      <c r="BF5" s="76" t="s">
+      <c r="BB5" s="72"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="67"/>
+      <c r="BF5" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="80"/>
+      <c r="BG5" s="133"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="103">
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="64">
         <v>1</v>
       </c>
-      <c r="E6" s="105">
+      <c r="E6" s="110">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2152,18 +2173,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="132"/>
-      <c r="BC6" s="133"/>
-      <c r="BD6" s="131"/>
-      <c r="BF6" s="77"/>
-      <c r="BG6" s="81"/>
+      <c r="BB6" s="72"/>
+      <c r="BC6" s="73"/>
+      <c r="BD6" s="67"/>
+      <c r="BF6" s="130"/>
+      <c r="BG6" s="134"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="106"/>
+      <c r="A7" s="97"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="111"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2212,24 +2233,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="132"/>
-      <c r="BC7" s="133"/>
-      <c r="BD7" s="131"/>
-      <c r="BF7" s="76" t="s">
+      <c r="BB7" s="72"/>
+      <c r="BC7" s="73"/>
+      <c r="BD7" s="67"/>
+      <c r="BF7" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="82"/>
+      <c r="BG7" s="135"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="93">
+      <c r="B8" s="108"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="70">
         <v>1.5</v>
       </c>
-      <c r="E8" s="110">
+      <c r="E8" s="62">
         <v>0.8</v>
       </c>
       <c r="F8" s="17"/>
@@ -2280,20 +2301,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="132"/>
-      <c r="BC8" s="133"/>
-      <c r="BD8" s="86" t="s">
+      <c r="BB8" s="72"/>
+      <c r="BC8" s="73"/>
+      <c r="BD8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="77"/>
-      <c r="BG8" s="83"/>
+      <c r="BF8" s="130"/>
+      <c r="BG8" s="136"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="90"/>
       <c r="B9" s="91"/>
       <c r="C9" s="92"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="111"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2342,24 +2363,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="132"/>
-      <c r="BC9" s="133"/>
-      <c r="BD9" s="86"/>
-      <c r="BF9" s="78" t="s">
+      <c r="BB9" s="72"/>
+      <c r="BC9" s="73"/>
+      <c r="BD9" s="71"/>
+      <c r="BF9" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="84"/>
+      <c r="BG9" s="137"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="103">
+      <c r="B10" s="88"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="64">
         <v>1.5</v>
       </c>
-      <c r="E10" s="112">
+      <c r="E10" s="66">
         <v>0.8</v>
       </c>
       <c r="F10" s="19"/>
@@ -2410,18 +2431,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="132"/>
-      <c r="BC10" s="133"/>
-      <c r="BD10" s="86"/>
-      <c r="BF10" s="79"/>
-      <c r="BG10" s="85"/>
+      <c r="BB10" s="72"/>
+      <c r="BC10" s="73"/>
+      <c r="BD10" s="71"/>
+      <c r="BF10" s="132"/>
+      <c r="BG10" s="138"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="113"/>
+      <c r="A11" s="97"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2470,20 +2491,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="132"/>
-      <c r="BC11" s="133"/>
-      <c r="BD11" s="86"/>
+      <c r="BB11" s="72"/>
+      <c r="BC11" s="73"/>
+      <c r="BD11" s="71"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="93">
+      <c r="B12" s="108"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="70">
         <v>1</v>
       </c>
-      <c r="E12" s="110">
+      <c r="E12" s="62">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2534,9 +2555,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="132"/>
-      <c r="BC12" s="133"/>
-      <c r="BD12" s="86" t="s">
+      <c r="BB12" s="72"/>
+      <c r="BC12" s="73"/>
+      <c r="BD12" s="71" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2553,8 +2574,8 @@
       <c r="A13" s="90"/>
       <c r="B13" s="91"/>
       <c r="C13" s="92"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="111"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="69"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2603,9 +2624,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="132"/>
-      <c r="BC13" s="133"/>
-      <c r="BD13" s="86"/>
+      <c r="BB13" s="72"/>
+      <c r="BC13" s="73"/>
+      <c r="BD13" s="71"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2617,15 +2638,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="98"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="103">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="64">
         <v>2</v>
       </c>
-      <c r="E14" s="112">
+      <c r="E14" s="66">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2676,16 +2697,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="132"/>
-      <c r="BC14" s="133"/>
-      <c r="BD14" s="86"/>
+      <c r="BB14" s="72"/>
+      <c r="BC14" s="73"/>
+      <c r="BD14" s="71"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="90"/>
       <c r="B15" s="91"/>
       <c r="C15" s="92"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="111"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2734,20 +2755,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="132"/>
-      <c r="BC15" s="133"/>
-      <c r="BD15" s="86"/>
+      <c r="BB15" s="72"/>
+      <c r="BC15" s="73"/>
+      <c r="BD15" s="71"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="98"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="103">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="64">
         <v>1</v>
       </c>
-      <c r="E16" s="112">
+      <c r="E16" s="66">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2798,16 +2819,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="132"/>
-      <c r="BC16" s="133"/>
-      <c r="BD16" s="86"/>
+      <c r="BB16" s="72"/>
+      <c r="BC16" s="73"/>
+      <c r="BD16" s="71"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="90"/>
       <c r="B17" s="91"/>
       <c r="C17" s="92"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="111"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2856,23 +2877,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="132"/>
-      <c r="BC17" s="133"/>
-      <c r="BD17" s="86"/>
+      <c r="BB17" s="72"/>
+      <c r="BC17" s="73"/>
+      <c r="BD17" s="71"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="98"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="103">
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="64">
         <v>2</v>
       </c>
-      <c r="E18" s="112">
+      <c r="E18" s="66">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2923,16 +2944,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="132"/>
-      <c r="BC18" s="133"/>
-      <c r="BD18" s="86"/>
+      <c r="BB18" s="72"/>
+      <c r="BC18" s="73"/>
+      <c r="BD18" s="71"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="90"/>
       <c r="B19" s="91"/>
       <c r="C19" s="92"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="111"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -2981,20 +3002,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="132"/>
-      <c r="BC19" s="133"/>
-      <c r="BD19" s="86"/>
+      <c r="BB19" s="72"/>
+      <c r="BC19" s="73"/>
+      <c r="BD19" s="71"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="103">
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="64">
         <v>1</v>
       </c>
-      <c r="E20" s="112">
+      <c r="E20" s="66">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3045,16 +3066,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="132"/>
-      <c r="BC20" s="133"/>
-      <c r="BD20" s="86"/>
+      <c r="BB20" s="72"/>
+      <c r="BC20" s="73"/>
+      <c r="BD20" s="71"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="113"/>
+      <c r="A21" s="97"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="63"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3103,20 +3124,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="132"/>
-      <c r="BC21" s="133"/>
-      <c r="BD21" s="86"/>
+      <c r="BB21" s="72"/>
+      <c r="BC21" s="73"/>
+      <c r="BD21" s="71"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="93">
+      <c r="B22" s="108"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="70">
         <v>0.5</v>
       </c>
-      <c r="E22" s="110">
+      <c r="E22" s="62">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3167,18 +3188,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="132"/>
-      <c r="BC22" s="133"/>
-      <c r="BD22" s="86" t="s">
+      <c r="BB22" s="72"/>
+      <c r="BC22" s="73"/>
+      <c r="BD22" s="71" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="101"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="113"/>
+      <c r="A23" s="97"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="63"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3227,20 +3248,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="132"/>
-      <c r="BC23" s="133"/>
-      <c r="BD23" s="86"/>
+      <c r="BB23" s="72"/>
+      <c r="BC23" s="73"/>
+      <c r="BD23" s="71"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="93">
+      <c r="B24" s="108"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="70">
         <v>2</v>
       </c>
-      <c r="E24" s="110">
+      <c r="E24" s="62">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3291,9 +3312,9 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="132"/>
-      <c r="BC24" s="133"/>
-      <c r="BD24" s="136" t="s">
+      <c r="BB24" s="72"/>
+      <c r="BC24" s="73"/>
+      <c r="BD24" s="76" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3301,8 +3322,8 @@
       <c r="A25" s="90"/>
       <c r="B25" s="91"/>
       <c r="C25" s="92"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="111"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3351,20 +3372,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="132"/>
-      <c r="BC25" s="133"/>
-      <c r="BD25" s="137"/>
+      <c r="BB25" s="72"/>
+      <c r="BC25" s="73"/>
+      <c r="BD25" s="77"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="98"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="103">
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="64">
         <v>1</v>
       </c>
-      <c r="E26" s="112">
+      <c r="E26" s="66">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3415,16 +3436,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="132"/>
-      <c r="BC26" s="133"/>
-      <c r="BD26" s="137"/>
+      <c r="BB26" s="72"/>
+      <c r="BC26" s="73"/>
+      <c r="BD26" s="77"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="90"/>
       <c r="B27" s="91"/>
       <c r="C27" s="92"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="111"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3473,20 +3494,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="132"/>
-      <c r="BC27" s="133"/>
-      <c r="BD27" s="137"/>
+      <c r="BB27" s="72"/>
+      <c r="BC27" s="73"/>
+      <c r="BD27" s="77"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="103">
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="64">
         <v>2</v>
       </c>
-      <c r="E28" s="112">
+      <c r="E28" s="66">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3537,16 +3558,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="132"/>
-      <c r="BC28" s="133"/>
-      <c r="BD28" s="137"/>
+      <c r="BB28" s="72"/>
+      <c r="BC28" s="73"/>
+      <c r="BD28" s="77"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="90"/>
       <c r="B29" s="91"/>
       <c r="C29" s="92"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="111"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3595,20 +3616,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="132"/>
-      <c r="BC29" s="133"/>
-      <c r="BD29" s="137"/>
+      <c r="BB29" s="72"/>
+      <c r="BC29" s="73"/>
+      <c r="BD29" s="77"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="97" t="s">
+      <c r="A30" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="98"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="103">
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="64">
         <v>2</v>
       </c>
-      <c r="E30" s="112">
+      <c r="E30" s="66">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3659,16 +3680,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="132"/>
-      <c r="BC30" s="133"/>
-      <c r="BD30" s="137"/>
+      <c r="BB30" s="72"/>
+      <c r="BC30" s="73"/>
+      <c r="BD30" s="77"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="90"/>
       <c r="B31" s="91"/>
       <c r="C31" s="92"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="111"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3717,20 +3738,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="132"/>
-      <c r="BC31" s="133"/>
-      <c r="BD31" s="137"/>
+      <c r="BB31" s="72"/>
+      <c r="BC31" s="73"/>
+      <c r="BD31" s="77"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="97" t="s">
+      <c r="A32" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="98"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="103">
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="64">
         <v>4</v>
       </c>
-      <c r="E32" s="112">
+      <c r="E32" s="66">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3781,16 +3802,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="132"/>
-      <c r="BC32" s="133"/>
-      <c r="BD32" s="137"/>
+      <c r="BB32" s="72"/>
+      <c r="BC32" s="73"/>
+      <c r="BD32" s="77"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="90"/>
       <c r="B33" s="91"/>
       <c r="C33" s="92"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="111"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3839,20 +3860,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="132"/>
-      <c r="BC33" s="133"/>
-      <c r="BD33" s="137"/>
+      <c r="BB33" s="72"/>
+      <c r="BC33" s="73"/>
+      <c r="BD33" s="77"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="97" t="s">
+      <c r="A34" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="98"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="103">
+      <c r="B34" s="140"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="64">
         <v>3</v>
       </c>
-      <c r="E34" s="112">
+      <c r="E34" s="66">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3903,16 +3924,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="132"/>
-      <c r="BC34" s="133"/>
-      <c r="BD34" s="137"/>
+      <c r="BB34" s="72"/>
+      <c r="BC34" s="73"/>
+      <c r="BD34" s="77"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="90"/>
-      <c r="B35" s="91"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="111"/>
+      <c r="A35" s="143"/>
+      <c r="B35" s="144"/>
+      <c r="C35" s="145"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="69"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3961,20 +3982,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="132"/>
-      <c r="BC35" s="133"/>
-      <c r="BD35" s="137"/>
+      <c r="BB35" s="72"/>
+      <c r="BC35" s="73"/>
+      <c r="BD35" s="77"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="97" t="s">
+      <c r="A36" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="98"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="103">
+      <c r="B36" s="140"/>
+      <c r="C36" s="141"/>
+      <c r="D36" s="64">
         <v>4</v>
       </c>
-      <c r="E36" s="112">
+      <c r="E36" s="66">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4024,16 +4045,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="132"/>
-      <c r="BC36" s="133"/>
-      <c r="BD36" s="137"/>
+      <c r="BB36" s="72"/>
+      <c r="BC36" s="73"/>
+      <c r="BD36" s="77"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="90"/>
-      <c r="B37" s="91"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="111"/>
+      <c r="A37" s="143"/>
+      <c r="B37" s="144"/>
+      <c r="C37" s="145"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="69"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4082,20 +4103,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="132"/>
-      <c r="BC37" s="133"/>
-      <c r="BD37" s="137"/>
+      <c r="BB37" s="72"/>
+      <c r="BC37" s="73"/>
+      <c r="BD37" s="77"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="98"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="103">
+      <c r="B38" s="140"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="64">
         <v>1</v>
       </c>
-      <c r="E38" s="112">
+      <c r="E38" s="66">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4144,16 +4165,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="132"/>
-      <c r="BC38" s="133"/>
-      <c r="BD38" s="137"/>
+      <c r="BB38" s="72"/>
+      <c r="BC38" s="73"/>
+      <c r="BD38" s="77"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="90"/>
-      <c r="B39" s="91"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="111"/>
+      <c r="A39" s="143"/>
+      <c r="B39" s="144"/>
+      <c r="C39" s="145"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4202,21 +4223,21 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="132"/>
-      <c r="BC39" s="133"/>
-      <c r="BD39" s="137"/>
+      <c r="BB39" s="72"/>
+      <c r="BC39" s="73"/>
+      <c r="BD39" s="77"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="97" t="s">
+      <c r="A40" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="98"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="103">
+      <c r="B40" s="140"/>
+      <c r="C40" s="141"/>
+      <c r="D40" s="64">
         <v>1</v>
       </c>
-      <c r="E40" s="112">
-        <v>1</v>
+      <c r="E40" s="66">
+        <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
@@ -4267,16 +4288,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="132"/>
-      <c r="BC40" s="133"/>
-      <c r="BD40" s="137"/>
+      <c r="BB40" s="72"/>
+      <c r="BC40" s="73"/>
+      <c r="BD40" s="77"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="90"/>
-      <c r="B41" s="91"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="111"/>
+      <c r="A41" s="143"/>
+      <c r="B41" s="144"/>
+      <c r="C41" s="145"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4325,20 +4346,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="132"/>
-      <c r="BC41" s="133"/>
-      <c r="BD41" s="137"/>
+      <c r="BB41" s="72"/>
+      <c r="BC41" s="73"/>
+      <c r="BD41" s="77"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="97" t="s">
+      <c r="A42" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="98"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="103">
+      <c r="B42" s="88"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="64">
         <v>2</v>
       </c>
-      <c r="E42" s="112"/>
+      <c r="E42" s="66"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -4387,16 +4408,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="132"/>
-      <c r="BC42" s="133"/>
-      <c r="BD42" s="137"/>
+      <c r="BB42" s="72"/>
+      <c r="BC42" s="73"/>
+      <c r="BD42" s="77"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="90"/>
       <c r="B43" s="91"/>
       <c r="C43" s="92"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="111"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4415,7 +4436,7 @@
       <c r="U43" s="8"/>
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
-      <c r="X43" s="30"/>
+      <c r="X43" s="24"/>
       <c r="Y43" s="4"/>
       <c r="Z43" s="8"/>
       <c r="AA43" s="9"/>
@@ -4445,20 +4466,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="132"/>
-      <c r="BC43" s="133"/>
-      <c r="BD43" s="137"/>
+      <c r="BB43" s="72"/>
+      <c r="BC43" s="73"/>
+      <c r="BD43" s="77"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="97" t="s">
+      <c r="A44" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="103">
+      <c r="B44" s="88"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="64">
         <v>2</v>
       </c>
-      <c r="E44" s="112"/>
+      <c r="E44" s="66"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4507,16 +4528,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="132"/>
-      <c r="BC44" s="133"/>
-      <c r="BD44" s="137"/>
+      <c r="BB44" s="72"/>
+      <c r="BC44" s="73"/>
+      <c r="BD44" s="77"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="100"/>
-      <c r="B45" s="101"/>
-      <c r="C45" s="102"/>
-      <c r="D45" s="104"/>
-      <c r="E45" s="113"/>
+      <c r="A45" s="97"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="63"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4565,20 +4586,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="132"/>
-      <c r="BC45" s="133"/>
-      <c r="BD45" s="138"/>
+      <c r="BB45" s="72"/>
+      <c r="BC45" s="73"/>
+      <c r="BD45" s="78"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="124" t="s">
+      <c r="A46" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="125"/>
-      <c r="C46" s="126"/>
-      <c r="D46" s="118">
+      <c r="B46" s="101"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="79">
         <v>1</v>
       </c>
-      <c r="E46" s="95"/>
+      <c r="E46" s="80"/>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4626,9 +4647,9 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="132"/>
-      <c r="BC46" s="133"/>
-      <c r="BD46" s="86" t="s">
+      <c r="BB46" s="72"/>
+      <c r="BC46" s="73"/>
+      <c r="BD46" s="71" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4636,8 +4657,8 @@
       <c r="A47" s="90"/>
       <c r="B47" s="91"/>
       <c r="C47" s="92"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="96"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="81"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4686,20 +4707,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="132"/>
-      <c r="BC47" s="133"/>
-      <c r="BD47" s="86"/>
+      <c r="BB47" s="72"/>
+      <c r="BC47" s="73"/>
+      <c r="BD47" s="71"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="97" t="s">
+      <c r="A48" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="98"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="103">
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="64">
         <v>2</v>
       </c>
-      <c r="E48" s="112"/>
+      <c r="E48" s="66"/>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4748,16 +4769,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="132"/>
-      <c r="BC48" s="133"/>
-      <c r="BD48" s="86"/>
+      <c r="BB48" s="72"/>
+      <c r="BC48" s="73"/>
+      <c r="BD48" s="71"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="100"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="102"/>
-      <c r="D49" s="104"/>
-      <c r="E49" s="113"/>
+      <c r="A49" s="97"/>
+      <c r="B49" s="98"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="63"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4806,20 +4827,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="132"/>
-      <c r="BC49" s="133"/>
-      <c r="BD49" s="86"/>
+      <c r="BB49" s="72"/>
+      <c r="BC49" s="73"/>
+      <c r="BD49" s="71"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="120" t="s">
+      <c r="A50" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="121"/>
-      <c r="C50" s="121"/>
-      <c r="D50" s="118">
+      <c r="B50" s="94"/>
+      <c r="C50" s="94"/>
+      <c r="D50" s="79">
         <v>5</v>
       </c>
-      <c r="E50" s="119"/>
+      <c r="E50" s="82"/>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4868,18 +4889,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="132"/>
-      <c r="BC50" s="133"/>
-      <c r="BD50" s="86" t="s">
+      <c r="BB50" s="72"/>
+      <c r="BC50" s="73"/>
+      <c r="BD50" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="122"/>
-      <c r="B51" s="123"/>
-      <c r="C51" s="123"/>
-      <c r="D51" s="94"/>
-      <c r="E51" s="111"/>
+      <c r="A51" s="95"/>
+      <c r="B51" s="96"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="69"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4928,20 +4949,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="132"/>
-      <c r="BC51" s="133"/>
-      <c r="BD51" s="86"/>
+      <c r="BB51" s="72"/>
+      <c r="BC51" s="73"/>
+      <c r="BD51" s="71"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="97" t="s">
+      <c r="A52" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="98"/>
-      <c r="C52" s="99"/>
-      <c r="D52" s="103">
+      <c r="B52" s="88"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="64">
         <v>2</v>
       </c>
-      <c r="E52" s="112"/>
+      <c r="E52" s="66"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -4982,16 +5003,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="23"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="132"/>
-      <c r="BC52" s="133"/>
-      <c r="BD52" s="86"/>
+      <c r="BB52" s="72"/>
+      <c r="BC52" s="73"/>
+      <c r="BD52" s="71"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="100"/>
-      <c r="B53" s="101"/>
-      <c r="C53" s="102"/>
-      <c r="D53" s="104"/>
-      <c r="E53" s="113"/>
+      <c r="A53" s="97"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="63"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5040,20 +5061,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="132"/>
-      <c r="BC53" s="133"/>
-      <c r="BD53" s="86"/>
+      <c r="BB53" s="72"/>
+      <c r="BC53" s="73"/>
+      <c r="BD53" s="71"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="124" t="s">
+      <c r="A54" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="125"/>
-      <c r="C54" s="126"/>
-      <c r="D54" s="118">
+      <c r="B54" s="101"/>
+      <c r="C54" s="102"/>
+      <c r="D54" s="79">
         <v>4.5</v>
       </c>
-      <c r="E54" s="119">
+      <c r="E54" s="82">
         <v>1</v>
       </c>
       <c r="F54" s="50"/>
@@ -5103,16 +5124,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="132"/>
-      <c r="BC54" s="133"/>
+      <c r="BB54" s="72"/>
+      <c r="BC54" s="73"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="90"/>
       <c r="B55" s="91"/>
       <c r="C55" s="92"/>
-      <c r="D55" s="94"/>
-      <c r="E55" s="111"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5161,16 +5182,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="132"/>
-      <c r="BC55" s="133"/>
+      <c r="BB55" s="72"/>
+      <c r="BC55" s="73"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="124"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="126"/>
-      <c r="D56" s="118"/>
-      <c r="E56" s="119"/>
+      <c r="A56" s="100"/>
+      <c r="B56" s="101"/>
+      <c r="C56" s="102"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="82"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5219,16 +5240,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="132"/>
-      <c r="BC56" s="133"/>
+      <c r="BB56" s="72"/>
+      <c r="BC56" s="73"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="90"/>
       <c r="B57" s="91"/>
       <c r="C57" s="92"/>
-      <c r="D57" s="94"/>
-      <c r="E57" s="111"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5277,16 +5298,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="132"/>
-      <c r="BC57" s="133"/>
+      <c r="BB57" s="72"/>
+      <c r="BC57" s="73"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="97"/>
-      <c r="B58" s="98"/>
-      <c r="C58" s="99"/>
-      <c r="D58" s="103"/>
-      <c r="E58" s="112"/>
+      <c r="A58" s="87"/>
+      <c r="B58" s="88"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="66"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5335,16 +5356,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="132"/>
-      <c r="BC58" s="133"/>
+      <c r="BB58" s="72"/>
+      <c r="BC58" s="73"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="100"/>
-      <c r="B59" s="101"/>
-      <c r="C59" s="102"/>
-      <c r="D59" s="104"/>
-      <c r="E59" s="113"/>
+      <c r="A59" s="97"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="63"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5393,35 +5414,135 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="134"/>
-      <c r="BC59" s="135"/>
+      <c r="BB59" s="74"/>
+      <c r="BC59" s="75"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="127" t="s">
+      <c r="A60" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="128"/>
-      <c r="C60" s="128"/>
-      <c r="D60" s="114">
+      <c r="B60" s="104"/>
+      <c r="C60" s="104"/>
+      <c r="D60" s="83">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="116">
+      <c r="E60" s="85">
         <f>SUM(E4:E59)</f>
-        <v>30.3</v>
+        <v>60.800000000000004</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="129"/>
-      <c r="B61" s="130"/>
-      <c r="C61" s="130"/>
-      <c r="D61" s="115"/>
-      <c r="E61" s="117"/>
+      <c r="A61" s="105"/>
+      <c r="B61" s="106"/>
+      <c r="C61" s="106"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="86"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
@@ -5446,106 +5567,6 @@
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="E34:E35"/>
     <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Form Settings Added und Colorierung der Ist Zahl vorgenommen kleinere Fehler noch behoben im Grid
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="637" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9454EDA-DBA2-47F3-9216-6724D0D371AA}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3552B326-4085-4773-A75F-818D028D10DD}"/>
   <bookViews>
     <workbookView xWindow="29985" yWindow="45" windowWidth="26760" windowHeight="15420" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
@@ -1076,36 +1076,235 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1126,205 +1325,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1649,8 +1649,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC44" sqref="AC44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,171 +1662,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="121" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="122"/>
-      <c r="F1" s="123" t="s">
+      <c r="E1" s="106"/>
+      <c r="F1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="115" t="s">
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="115" t="s">
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="115" t="s">
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="116"/>
-      <c r="W1" s="116"/>
-      <c r="X1" s="116"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="115" t="s">
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="116"/>
-      <c r="AB1" s="116"/>
-      <c r="AC1" s="116"/>
-      <c r="AD1" s="117"/>
-      <c r="AE1" s="115" t="s">
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="116"/>
-      <c r="AG1" s="116"/>
-      <c r="AH1" s="116"/>
-      <c r="AI1" s="117"/>
-      <c r="AJ1" s="115" t="s">
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="76"/>
+      <c r="AJ1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="116"/>
-      <c r="AL1" s="116"/>
-      <c r="AM1" s="116"/>
-      <c r="AN1" s="117"/>
-      <c r="AO1" s="115" t="s">
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="76"/>
+      <c r="AO1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="116"/>
-      <c r="AQ1" s="116"/>
-      <c r="AR1" s="116"/>
-      <c r="AS1" s="117"/>
-      <c r="AT1" s="115" t="s">
+      <c r="AP1" s="75"/>
+      <c r="AQ1" s="75"/>
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="76"/>
+      <c r="AT1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="116"/>
-      <c r="AV1" s="116"/>
-      <c r="AW1" s="116"/>
-      <c r="AX1" s="117"/>
-      <c r="AY1" s="115" t="s">
+      <c r="AU1" s="75"/>
+      <c r="AV1" s="75"/>
+      <c r="AW1" s="75"/>
+      <c r="AX1" s="76"/>
+      <c r="AY1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="116"/>
-      <c r="BA1" s="116"/>
-      <c r="BB1" s="116"/>
-      <c r="BC1" s="117"/>
-      <c r="BD1" s="71" t="s">
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="75"/>
+      <c r="BB1" s="75"/>
+      <c r="BC1" s="76"/>
+      <c r="BD1" s="73" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="126">
+      <c r="A2" s="103"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="110">
         <v>44957</v>
       </c>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="112">
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="77">
         <v>44958</v>
       </c>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="112">
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="77">
         <v>44959</v>
       </c>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="112">
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="77">
         <v>44960</v>
       </c>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="114"/>
-      <c r="Z2" s="112">
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="77">
         <v>44964</v>
       </c>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
-      <c r="AC2" s="113"/>
-      <c r="AD2" s="114"/>
-      <c r="AE2" s="112">
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="79"/>
+      <c r="AE2" s="77">
         <v>44965</v>
       </c>
-      <c r="AF2" s="113"/>
-      <c r="AG2" s="113"/>
-      <c r="AH2" s="113"/>
-      <c r="AI2" s="114"/>
-      <c r="AJ2" s="112">
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="77">
         <v>44966</v>
       </c>
-      <c r="AK2" s="113"/>
-      <c r="AL2" s="113"/>
-      <c r="AM2" s="113"/>
-      <c r="AN2" s="114"/>
-      <c r="AO2" s="112">
+      <c r="AK2" s="78"/>
+      <c r="AL2" s="78"/>
+      <c r="AM2" s="78"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="77">
         <v>44967</v>
       </c>
-      <c r="AP2" s="113"/>
-      <c r="AQ2" s="113"/>
-      <c r="AR2" s="113"/>
-      <c r="AS2" s="114"/>
-      <c r="AT2" s="112">
+      <c r="AP2" s="78"/>
+      <c r="AQ2" s="78"/>
+      <c r="AR2" s="78"/>
+      <c r="AS2" s="79"/>
+      <c r="AT2" s="77">
         <v>44971</v>
       </c>
-      <c r="AU2" s="113"/>
-      <c r="AV2" s="113"/>
-      <c r="AW2" s="113"/>
-      <c r="AX2" s="114"/>
-      <c r="AY2" s="112">
+      <c r="AU2" s="78"/>
+      <c r="AV2" s="78"/>
+      <c r="AW2" s="78"/>
+      <c r="AX2" s="79"/>
+      <c r="AY2" s="77">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="113"/>
-      <c r="BA2" s="113"/>
-      <c r="BB2" s="113"/>
-      <c r="BC2" s="114"/>
-      <c r="BD2" s="71"/>
+      <c r="AZ2" s="78"/>
+      <c r="BA2" s="78"/>
+      <c r="BB2" s="78"/>
+      <c r="BC2" s="79"/>
+      <c r="BD2" s="73"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="120"/>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1983,18 +1983,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="67"/>
+      <c r="BD3" s="138"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="70">
+      <c r="B4" s="85"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="82">
         <v>30</v>
       </c>
-      <c r="E4" s="80">
+      <c r="E4" s="91">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2045,18 +2045,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="72" t="s">
+      <c r="BB4" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="67"/>
+      <c r="BC4" s="140"/>
+      <c r="BD4" s="138"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="81"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2072,7 +2072,7 @@
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
       <c r="T5" s="47"/>
-      <c r="U5" s="142"/>
+      <c r="U5" s="62"/>
       <c r="V5" s="30"/>
       <c r="W5" s="30"/>
       <c r="X5" s="30"/>
@@ -2105,24 +2105,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="67"/>
-      <c r="BF5" s="129" t="s">
+      <c r="BB5" s="139"/>
+      <c r="BC5" s="140"/>
+      <c r="BD5" s="138"/>
+      <c r="BF5" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="133"/>
+      <c r="BG5" s="67"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="64">
+      <c r="B6" s="94"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="99">
         <v>1</v>
       </c>
-      <c r="E6" s="110">
+      <c r="E6" s="100">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2173,18 +2173,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="72"/>
-      <c r="BC6" s="73"/>
-      <c r="BD6" s="67"/>
-      <c r="BF6" s="130"/>
-      <c r="BG6" s="134"/>
+      <c r="BB6" s="139"/>
+      <c r="BC6" s="140"/>
+      <c r="BD6" s="138"/>
+      <c r="BF6" s="64"/>
+      <c r="BG6" s="68"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="97"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="111"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2233,24 +2233,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="72"/>
-      <c r="BC7" s="73"/>
-      <c r="BD7" s="67"/>
-      <c r="BF7" s="129" t="s">
+      <c r="BB7" s="139"/>
+      <c r="BC7" s="140"/>
+      <c r="BD7" s="138"/>
+      <c r="BF7" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="135"/>
+      <c r="BG7" s="69"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="70">
+      <c r="B8" s="85"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="82">
         <v>1.5</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="114">
         <v>0.8</v>
       </c>
       <c r="F8" s="17"/>
@@ -2301,20 +2301,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="72"/>
-      <c r="BC8" s="73"/>
-      <c r="BD8" s="71" t="s">
+      <c r="BB8" s="139"/>
+      <c r="BC8" s="140"/>
+      <c r="BD8" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="130"/>
-      <c r="BG8" s="136"/>
+      <c r="BF8" s="64"/>
+      <c r="BG8" s="70"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="69"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="81"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2363,24 +2363,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="72"/>
-      <c r="BC9" s="73"/>
-      <c r="BD9" s="71"/>
-      <c r="BF9" s="131" t="s">
+      <c r="BB9" s="139"/>
+      <c r="BC9" s="140"/>
+      <c r="BD9" s="73"/>
+      <c r="BF9" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="137"/>
+      <c r="BG9" s="71"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="64">
+      <c r="B10" s="94"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="99">
         <v>1.5</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="80">
         <v>0.8</v>
       </c>
       <c r="F10" s="19"/>
@@ -2431,18 +2431,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="72"/>
-      <c r="BC10" s="73"/>
-      <c r="BD10" s="71"/>
-      <c r="BF10" s="132"/>
-      <c r="BG10" s="138"/>
+      <c r="BB10" s="139"/>
+      <c r="BC10" s="140"/>
+      <c r="BD10" s="73"/>
+      <c r="BF10" s="66"/>
+      <c r="BG10" s="72"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="97"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="63"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="113"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2491,20 +2491,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="72"/>
-      <c r="BC11" s="73"/>
-      <c r="BD11" s="71"/>
+      <c r="BB11" s="139"/>
+      <c r="BC11" s="140"/>
+      <c r="BD11" s="73"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="107" t="s">
+      <c r="A12" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="108"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="70">
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="82">
         <v>1</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="114">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2555,9 +2555,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="72"/>
-      <c r="BC12" s="73"/>
-      <c r="BD12" s="71" t="s">
+      <c r="BB12" s="139"/>
+      <c r="BC12" s="140"/>
+      <c r="BD12" s="73" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2571,11 +2571,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="69"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="81"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2624,9 +2624,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="72"/>
-      <c r="BC13" s="73"/>
-      <c r="BD13" s="71"/>
+      <c r="BB13" s="139"/>
+      <c r="BC13" s="140"/>
+      <c r="BD13" s="73"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2638,15 +2638,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="64">
+      <c r="B14" s="94"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="99">
         <v>2</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="80">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2697,16 +2697,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="72"/>
-      <c r="BC14" s="73"/>
-      <c r="BD14" s="71"/>
+      <c r="BB14" s="139"/>
+      <c r="BC14" s="140"/>
+      <c r="BD14" s="73"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="90"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="81"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2755,20 +2755,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="72"/>
-      <c r="BC15" s="73"/>
-      <c r="BD15" s="71"/>
+      <c r="BB15" s="139"/>
+      <c r="BC15" s="140"/>
+      <c r="BD15" s="73"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="64">
+      <c r="B16" s="94"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="99">
         <v>1</v>
       </c>
-      <c r="E16" s="66">
+      <c r="E16" s="80">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2819,16 +2819,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="72"/>
-      <c r="BC16" s="73"/>
-      <c r="BD16" s="71"/>
+      <c r="BB16" s="139"/>
+      <c r="BC16" s="140"/>
+      <c r="BD16" s="73"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="90"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="69"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="81"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2877,23 +2877,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="72"/>
-      <c r="BC17" s="73"/>
-      <c r="BD17" s="71"/>
+      <c r="BB17" s="139"/>
+      <c r="BC17" s="140"/>
+      <c r="BD17" s="73"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="88"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="64">
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="99">
         <v>2</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="80">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2944,16 +2944,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="72"/>
-      <c r="BC18" s="73"/>
-      <c r="BD18" s="71"/>
+      <c r="BB18" s="139"/>
+      <c r="BC18" s="140"/>
+      <c r="BD18" s="73"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="90"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="69"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3002,20 +3002,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="72"/>
-      <c r="BC19" s="73"/>
-      <c r="BD19" s="71"/>
+      <c r="BB19" s="139"/>
+      <c r="BC19" s="140"/>
+      <c r="BD19" s="73"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="88"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="64">
+      <c r="B20" s="94"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="99">
         <v>1</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="80">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3066,16 +3066,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="72"/>
-      <c r="BC20" s="73"/>
-      <c r="BD20" s="71"/>
+      <c r="BB20" s="139"/>
+      <c r="BC20" s="140"/>
+      <c r="BD20" s="73"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="97"/>
-      <c r="B21" s="98"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="63"/>
+      <c r="A21" s="96"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="113"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3124,20 +3124,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="72"/>
-      <c r="BC21" s="73"/>
-      <c r="BD21" s="71"/>
+      <c r="BB21" s="139"/>
+      <c r="BC21" s="140"/>
+      <c r="BD21" s="73"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="107" t="s">
+      <c r="A22" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="108"/>
-      <c r="C22" s="109"/>
-      <c r="D22" s="70">
+      <c r="B22" s="85"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="82">
         <v>0.5</v>
       </c>
-      <c r="E22" s="62">
+      <c r="E22" s="114">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3188,18 +3188,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="72"/>
-      <c r="BC22" s="73"/>
-      <c r="BD22" s="71" t="s">
+      <c r="BB22" s="139"/>
+      <c r="BC22" s="140"/>
+      <c r="BD22" s="73" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="97"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="63"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="113"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3248,20 +3248,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="72"/>
-      <c r="BC23" s="73"/>
-      <c r="BD23" s="71"/>
+      <c r="BB23" s="139"/>
+      <c r="BC23" s="140"/>
+      <c r="BD23" s="73"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="108"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="70">
+      <c r="B24" s="85"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="82">
         <v>2</v>
       </c>
-      <c r="E24" s="62">
+      <c r="E24" s="114">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3312,18 +3312,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="72"/>
-      <c r="BC24" s="73"/>
-      <c r="BD24" s="76" t="s">
+      <c r="BB24" s="139"/>
+      <c r="BC24" s="140"/>
+      <c r="BD24" s="143" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="69"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="81"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3372,20 +3372,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="72"/>
-      <c r="BC25" s="73"/>
-      <c r="BD25" s="77"/>
+      <c r="BB25" s="139"/>
+      <c r="BC25" s="140"/>
+      <c r="BD25" s="144"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="88"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="64">
+      <c r="B26" s="94"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="99">
         <v>1</v>
       </c>
-      <c r="E26" s="66">
+      <c r="E26" s="80">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3436,16 +3436,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="72"/>
-      <c r="BC26" s="73"/>
-      <c r="BD26" s="77"/>
+      <c r="BB26" s="139"/>
+      <c r="BC26" s="140"/>
+      <c r="BD26" s="144"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="90"/>
-      <c r="B27" s="91"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="81"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3494,20 +3494,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="72"/>
-      <c r="BC27" s="73"/>
-      <c r="BD27" s="77"/>
+      <c r="BB27" s="139"/>
+      <c r="BC27" s="140"/>
+      <c r="BD27" s="144"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87" t="s">
+      <c r="A28" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="88"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="64">
+      <c r="B28" s="94"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="99">
         <v>2</v>
       </c>
-      <c r="E28" s="66">
+      <c r="E28" s="80">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3558,16 +3558,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="72"/>
-      <c r="BC28" s="73"/>
-      <c r="BD28" s="77"/>
+      <c r="BB28" s="139"/>
+      <c r="BC28" s="140"/>
+      <c r="BD28" s="144"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="90"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="92"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="81"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3616,20 +3616,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="72"/>
-      <c r="BC29" s="73"/>
-      <c r="BD29" s="77"/>
+      <c r="BB29" s="139"/>
+      <c r="BC29" s="140"/>
+      <c r="BD29" s="144"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="64">
+      <c r="B30" s="94"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="99">
         <v>2</v>
       </c>
-      <c r="E30" s="66">
+      <c r="E30" s="80">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3680,16 +3680,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="72"/>
-      <c r="BC30" s="73"/>
-      <c r="BD30" s="77"/>
+      <c r="BB30" s="139"/>
+      <c r="BC30" s="140"/>
+      <c r="BD30" s="144"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="90"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="69"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="81"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3738,20 +3738,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="72"/>
-      <c r="BC31" s="73"/>
-      <c r="BD31" s="77"/>
+      <c r="BB31" s="139"/>
+      <c r="BC31" s="140"/>
+      <c r="BD31" s="144"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="64">
+      <c r="B32" s="94"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="99">
         <v>4</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="80">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3802,16 +3802,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="72"/>
-      <c r="BC32" s="73"/>
-      <c r="BD32" s="77"/>
+      <c r="BB32" s="139"/>
+      <c r="BC32" s="140"/>
+      <c r="BD32" s="144"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
-      <c r="B33" s="91"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="69"/>
+      <c r="A33" s="87"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="81"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3860,20 +3860,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="72"/>
-      <c r="BC33" s="73"/>
-      <c r="BD33" s="77"/>
+      <c r="BB33" s="139"/>
+      <c r="BC33" s="140"/>
+      <c r="BD33" s="144"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="139" t="s">
+      <c r="A34" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="140"/>
-      <c r="C34" s="141"/>
-      <c r="D34" s="64">
+      <c r="B34" s="127"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="99">
         <v>3</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="80">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3924,16 +3924,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="72"/>
-      <c r="BC34" s="73"/>
-      <c r="BD34" s="77"/>
+      <c r="BB34" s="139"/>
+      <c r="BC34" s="140"/>
+      <c r="BD34" s="144"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="143"/>
-      <c r="B35" s="144"/>
-      <c r="C35" s="145"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="69"/>
+      <c r="A35" s="129"/>
+      <c r="B35" s="130"/>
+      <c r="C35" s="131"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="81"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3982,20 +3982,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="72"/>
-      <c r="BC35" s="73"/>
-      <c r="BD35" s="77"/>
+      <c r="BB35" s="139"/>
+      <c r="BC35" s="140"/>
+      <c r="BD35" s="144"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="139" t="s">
+      <c r="A36" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="140"/>
-      <c r="C36" s="141"/>
-      <c r="D36" s="64">
+      <c r="B36" s="127"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="99">
         <v>4</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="80">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4045,16 +4045,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="72"/>
-      <c r="BC36" s="73"/>
-      <c r="BD36" s="77"/>
+      <c r="BB36" s="139"/>
+      <c r="BC36" s="140"/>
+      <c r="BD36" s="144"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="143"/>
-      <c r="B37" s="144"/>
-      <c r="C37" s="145"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="69"/>
+      <c r="A37" s="129"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="131"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="81"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4103,20 +4103,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="72"/>
-      <c r="BC37" s="73"/>
-      <c r="BD37" s="77"/>
+      <c r="BB37" s="139"/>
+      <c r="BC37" s="140"/>
+      <c r="BD37" s="144"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="139" t="s">
+      <c r="A38" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="140"/>
-      <c r="C38" s="141"/>
-      <c r="D38" s="64">
+      <c r="B38" s="127"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="99">
         <v>1</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="80">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4165,16 +4165,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="72"/>
-      <c r="BC38" s="73"/>
-      <c r="BD38" s="77"/>
+      <c r="BB38" s="139"/>
+      <c r="BC38" s="140"/>
+      <c r="BD38" s="144"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="143"/>
-      <c r="B39" s="144"/>
-      <c r="C39" s="145"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="69"/>
+      <c r="A39" s="129"/>
+      <c r="B39" s="130"/>
+      <c r="C39" s="131"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="81"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4223,20 +4223,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="72"/>
-      <c r="BC39" s="73"/>
-      <c r="BD39" s="77"/>
+      <c r="BB39" s="139"/>
+      <c r="BC39" s="140"/>
+      <c r="BD39" s="144"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="139" t="s">
+      <c r="A40" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="140"/>
-      <c r="C40" s="141"/>
-      <c r="D40" s="64">
+      <c r="B40" s="127"/>
+      <c r="C40" s="128"/>
+      <c r="D40" s="99">
         <v>1</v>
       </c>
-      <c r="E40" s="66">
+      <c r="E40" s="80">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4288,16 +4288,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="72"/>
-      <c r="BC40" s="73"/>
-      <c r="BD40" s="77"/>
+      <c r="BB40" s="139"/>
+      <c r="BC40" s="140"/>
+      <c r="BD40" s="144"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="143"/>
-      <c r="B41" s="144"/>
-      <c r="C41" s="145"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="69"/>
+      <c r="A41" s="129"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="81"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4346,20 +4346,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="72"/>
-      <c r="BC41" s="73"/>
-      <c r="BD41" s="77"/>
+      <c r="BB41" s="139"/>
+      <c r="BC41" s="140"/>
+      <c r="BD41" s="144"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="87" t="s">
+      <c r="A42" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="88"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="64">
+      <c r="B42" s="94"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="99">
         <v>2</v>
       </c>
-      <c r="E42" s="66"/>
+      <c r="E42" s="80"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -4382,7 +4382,7 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="18"/>
       <c r="AA42" s="18"/>
-      <c r="AB42" s="18"/>
+      <c r="AB42" s="24"/>
       <c r="AC42" s="9"/>
       <c r="AD42" s="4"/>
       <c r="AE42" s="8"/>
@@ -4408,16 +4408,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="72"/>
-      <c r="BC42" s="73"/>
-      <c r="BD42" s="77"/>
+      <c r="BB42" s="139"/>
+      <c r="BC42" s="140"/>
+      <c r="BD42" s="144"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="69"/>
+      <c r="A43" s="87"/>
+      <c r="B43" s="88"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="81"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4438,9 +4438,9 @@
       <c r="W43" s="9"/>
       <c r="X43" s="24"/>
       <c r="Y43" s="4"/>
-      <c r="Z43" s="8"/>
-      <c r="AA43" s="9"/>
-      <c r="AB43" s="9"/>
+      <c r="Z43" s="36"/>
+      <c r="AA43" s="30"/>
+      <c r="AB43" s="24"/>
       <c r="AC43" s="9"/>
       <c r="AD43" s="4"/>
       <c r="AE43" s="8"/>
@@ -4466,20 +4466,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="72"/>
-      <c r="BC43" s="73"/>
-      <c r="BD43" s="77"/>
+      <c r="BB43" s="139"/>
+      <c r="BC43" s="140"/>
+      <c r="BD43" s="144"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="88"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="64">
+      <c r="B44" s="94"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="99">
         <v>2</v>
       </c>
-      <c r="E44" s="66"/>
+      <c r="E44" s="80"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4528,16 +4528,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="72"/>
-      <c r="BC44" s="73"/>
-      <c r="BD44" s="77"/>
+      <c r="BB44" s="139"/>
+      <c r="BC44" s="140"/>
+      <c r="BD44" s="144"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="97"/>
-      <c r="B45" s="98"/>
-      <c r="C45" s="99"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="63"/>
+      <c r="A45" s="96"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="113"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4586,20 +4586,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="72"/>
-      <c r="BC45" s="73"/>
-      <c r="BD45" s="78"/>
+      <c r="BB45" s="139"/>
+      <c r="BC45" s="140"/>
+      <c r="BD45" s="145"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="100" t="s">
+      <c r="A46" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="101"/>
-      <c r="C46" s="102"/>
-      <c r="D46" s="79">
+      <c r="B46" s="120"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="132">
         <v>1</v>
       </c>
-      <c r="E46" s="80"/>
+      <c r="E46" s="91"/>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4647,18 +4647,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="72"/>
-      <c r="BC46" s="73"/>
-      <c r="BD46" s="71" t="s">
+      <c r="BB46" s="139"/>
+      <c r="BC46" s="140"/>
+      <c r="BD46" s="73" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="90"/>
-      <c r="B47" s="91"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="81"/>
+      <c r="A47" s="87"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="92"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4707,20 +4707,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="72"/>
-      <c r="BC47" s="73"/>
-      <c r="BD47" s="71"/>
+      <c r="BB47" s="139"/>
+      <c r="BC47" s="140"/>
+      <c r="BD47" s="73"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="87" t="s">
+      <c r="A48" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="88"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="64">
+      <c r="B48" s="94"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="99">
         <v>2</v>
       </c>
-      <c r="E48" s="66"/>
+      <c r="E48" s="80"/>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4769,16 +4769,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="72"/>
-      <c r="BC48" s="73"/>
-      <c r="BD48" s="71"/>
+      <c r="BB48" s="139"/>
+      <c r="BC48" s="140"/>
+      <c r="BD48" s="73"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="97"/>
-      <c r="B49" s="98"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="65"/>
-      <c r="E49" s="63"/>
+      <c r="A49" s="96"/>
+      <c r="B49" s="97"/>
+      <c r="C49" s="98"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="113"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4827,20 +4827,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="72"/>
-      <c r="BC49" s="73"/>
-      <c r="BD49" s="71"/>
+      <c r="BB49" s="139"/>
+      <c r="BC49" s="140"/>
+      <c r="BD49" s="73"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="93" t="s">
+      <c r="A50" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="94"/>
-      <c r="C50" s="94"/>
-      <c r="D50" s="79">
+      <c r="B50" s="116"/>
+      <c r="C50" s="116"/>
+      <c r="D50" s="132">
         <v>5</v>
       </c>
-      <c r="E50" s="82"/>
+      <c r="E50" s="133"/>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4889,18 +4889,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="72"/>
-      <c r="BC50" s="73"/>
-      <c r="BD50" s="71" t="s">
+      <c r="BB50" s="139"/>
+      <c r="BC50" s="140"/>
+      <c r="BD50" s="73" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="95"/>
-      <c r="B51" s="96"/>
-      <c r="C51" s="96"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="69"/>
+      <c r="A51" s="117"/>
+      <c r="B51" s="118"/>
+      <c r="C51" s="118"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="81"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4949,20 +4949,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="72"/>
-      <c r="BC51" s="73"/>
-      <c r="BD51" s="71"/>
+      <c r="BB51" s="139"/>
+      <c r="BC51" s="140"/>
+      <c r="BD51" s="73"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="87" t="s">
+      <c r="A52" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="88"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="64">
+      <c r="B52" s="94"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="99">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
+      <c r="E52" s="80"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5003,16 +5003,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="23"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="72"/>
-      <c r="BC52" s="73"/>
-      <c r="BD52" s="71"/>
+      <c r="BB52" s="139"/>
+      <c r="BC52" s="140"/>
+      <c r="BD52" s="73"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="97"/>
-      <c r="B53" s="98"/>
-      <c r="C53" s="99"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="63"/>
+      <c r="A53" s="96"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="98"/>
+      <c r="D53" s="83"/>
+      <c r="E53" s="113"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5061,20 +5061,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="72"/>
-      <c r="BC53" s="73"/>
-      <c r="BD53" s="71"/>
+      <c r="BB53" s="139"/>
+      <c r="BC53" s="140"/>
+      <c r="BD53" s="73"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="100" t="s">
+      <c r="A54" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="101"/>
-      <c r="C54" s="102"/>
-      <c r="D54" s="79">
+      <c r="B54" s="120"/>
+      <c r="C54" s="121"/>
+      <c r="D54" s="132">
         <v>4.5</v>
       </c>
-      <c r="E54" s="82">
+      <c r="E54" s="133">
         <v>1</v>
       </c>
       <c r="F54" s="50"/>
@@ -5124,16 +5124,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="72"/>
-      <c r="BC54" s="73"/>
+      <c r="BB54" s="139"/>
+      <c r="BC54" s="140"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="90"/>
-      <c r="B55" s="91"/>
-      <c r="C55" s="92"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="69"/>
+      <c r="A55" s="87"/>
+      <c r="B55" s="88"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="90"/>
+      <c r="E55" s="81"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5182,16 +5182,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="72"/>
-      <c r="BC55" s="73"/>
+      <c r="BB55" s="139"/>
+      <c r="BC55" s="140"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="100"/>
-      <c r="B56" s="101"/>
-      <c r="C56" s="102"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="82"/>
+      <c r="A56" s="119"/>
+      <c r="B56" s="120"/>
+      <c r="C56" s="121"/>
+      <c r="D56" s="132"/>
+      <c r="E56" s="133"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5240,16 +5240,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="72"/>
-      <c r="BC56" s="73"/>
+      <c r="BB56" s="139"/>
+      <c r="BC56" s="140"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="90"/>
-      <c r="B57" s="91"/>
-      <c r="C57" s="92"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="69"/>
+      <c r="A57" s="87"/>
+      <c r="B57" s="88"/>
+      <c r="C57" s="89"/>
+      <c r="D57" s="90"/>
+      <c r="E57" s="81"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5298,16 +5298,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="72"/>
-      <c r="BC57" s="73"/>
+      <c r="BB57" s="139"/>
+      <c r="BC57" s="140"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="87"/>
-      <c r="B58" s="88"/>
-      <c r="C58" s="89"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="66"/>
+      <c r="A58" s="93"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="80"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5356,16 +5356,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="72"/>
-      <c r="BC58" s="73"/>
+      <c r="BB58" s="139"/>
+      <c r="BC58" s="140"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="97"/>
-      <c r="B59" s="98"/>
-      <c r="C59" s="99"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="63"/>
+      <c r="A59" s="96"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="83"/>
+      <c r="E59" s="113"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5414,72 +5414,94 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="74"/>
-      <c r="BC59" s="75"/>
+      <c r="BB59" s="141"/>
+      <c r="BC59" s="142"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="103" t="s">
+      <c r="A60" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="104"/>
-      <c r="C60" s="104"/>
-      <c r="D60" s="83">
+      <c r="B60" s="123"/>
+      <c r="C60" s="123"/>
+      <c r="D60" s="134">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="85">
+      <c r="E60" s="136">
         <f>SUM(E4:E59)</f>
         <v>60.800000000000004</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="105"/>
-      <c r="B61" s="106"/>
-      <c r="C61" s="106"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="86"/>
+      <c r="A61" s="124"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="125"/>
+      <c r="D61" s="135"/>
+      <c r="E61" s="137"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="BD8:BD11"/>
+    <mergeCell ref="BD12:BD21"/>
+    <mergeCell ref="BD22:BD23"/>
+    <mergeCell ref="BB4:BC59"/>
+    <mergeCell ref="BD50:BD53"/>
+    <mergeCell ref="BD46:BD49"/>
+    <mergeCell ref="BD24:BD45"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="A20:C21"/>
@@ -5504,69 +5526,47 @@
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="A14:C15"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
     <mergeCell ref="BD3:BD7"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="BD8:BD11"/>
-    <mergeCell ref="BD12:BD21"/>
-    <mergeCell ref="BD22:BD23"/>
-    <mergeCell ref="BB4:BC59"/>
-    <mergeCell ref="BD50:BD53"/>
-    <mergeCell ref="BD46:BD49"/>
-    <mergeCell ref="BD24:BD45"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D32:D33"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fehler gefunden im SR diesen behoben testumgebung angefangen zu gestalten
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="656" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69E390B3-4B7B-4F9B-BA81-3DFE5FAB3889}"/>
+  <xr:revisionPtr revIDLastSave="658" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F264590-2E13-42D6-A1B5-0C002A34C152}"/>
   <bookViews>
     <workbookView xWindow="29985" yWindow="45" windowWidth="26760" windowHeight="15420" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
@@ -1009,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1077,6 +1077,222 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1108,224 +1324,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1649,8 +1650,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z35" sqref="Z35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36:AK36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,171 +1663,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="107" t="s">
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="108"/>
-      <c r="F1" s="109" t="s">
+      <c r="E1" s="125"/>
+      <c r="F1" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="74" t="s">
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="74" t="s">
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="74" t="s">
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="134"/>
+      <c r="U1" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="74" t="s">
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="134"/>
+      <c r="Z1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="76"/>
-      <c r="AE1" s="74" t="s">
+      <c r="AA1" s="133"/>
+      <c r="AB1" s="133"/>
+      <c r="AC1" s="133"/>
+      <c r="AD1" s="134"/>
+      <c r="AE1" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="76"/>
-      <c r="AJ1" s="74" t="s">
+      <c r="AF1" s="133"/>
+      <c r="AG1" s="133"/>
+      <c r="AH1" s="133"/>
+      <c r="AI1" s="134"/>
+      <c r="AJ1" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="76"/>
-      <c r="AO1" s="74" t="s">
+      <c r="AK1" s="133"/>
+      <c r="AL1" s="133"/>
+      <c r="AM1" s="133"/>
+      <c r="AN1" s="134"/>
+      <c r="AO1" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="75"/>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="76"/>
-      <c r="AT1" s="74" t="s">
+      <c r="AP1" s="133"/>
+      <c r="AQ1" s="133"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
+      <c r="AT1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="75"/>
-      <c r="AV1" s="75"/>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="76"/>
-      <c r="AY1" s="74" t="s">
+      <c r="AU1" s="133"/>
+      <c r="AV1" s="133"/>
+      <c r="AW1" s="133"/>
+      <c r="AX1" s="134"/>
+      <c r="AY1" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="75"/>
-      <c r="BB1" s="75"/>
-      <c r="BC1" s="76"/>
-      <c r="BD1" s="73" t="s">
+      <c r="AZ1" s="133"/>
+      <c r="BA1" s="133"/>
+      <c r="BB1" s="133"/>
+      <c r="BC1" s="134"/>
+      <c r="BD1" s="69" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="112">
+      <c r="A2" s="122"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="129">
         <v>44957</v>
       </c>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="77">
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="118">
         <v>44958</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="77">
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="118">
         <v>44959</v>
       </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="77">
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="118">
         <v>44960</v>
       </c>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="77">
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="120"/>
+      <c r="Z2" s="118">
         <v>44964</v>
       </c>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="77">
+      <c r="AA2" s="119"/>
+      <c r="AB2" s="119"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="120"/>
+      <c r="AE2" s="118">
         <v>44965</v>
       </c>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="79"/>
-      <c r="AJ2" s="77">
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="119"/>
+      <c r="AI2" s="120"/>
+      <c r="AJ2" s="118">
         <v>44966</v>
       </c>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="79"/>
-      <c r="AO2" s="77">
+      <c r="AK2" s="119"/>
+      <c r="AL2" s="119"/>
+      <c r="AM2" s="119"/>
+      <c r="AN2" s="120"/>
+      <c r="AO2" s="118">
         <v>44967</v>
       </c>
-      <c r="AP2" s="78"/>
-      <c r="AQ2" s="78"/>
-      <c r="AR2" s="78"/>
-      <c r="AS2" s="79"/>
-      <c r="AT2" s="77">
+      <c r="AP2" s="119"/>
+      <c r="AQ2" s="119"/>
+      <c r="AR2" s="119"/>
+      <c r="AS2" s="120"/>
+      <c r="AT2" s="118">
         <v>44971</v>
       </c>
-      <c r="AU2" s="78"/>
-      <c r="AV2" s="78"/>
-      <c r="AW2" s="78"/>
-      <c r="AX2" s="79"/>
-      <c r="AY2" s="77">
+      <c r="AU2" s="119"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="119"/>
+      <c r="AX2" s="120"/>
+      <c r="AY2" s="118">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="78"/>
-      <c r="BA2" s="78"/>
-      <c r="BB2" s="78"/>
-      <c r="BC2" s="79"/>
-      <c r="BD2" s="73"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="119"/>
+      <c r="BB2" s="119"/>
+      <c r="BC2" s="120"/>
+      <c r="BD2" s="69"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="106"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
+      <c r="A3" s="123"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1983,18 +1984,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="80"/>
+      <c r="BD3" s="145"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="92">
+      <c r="B4" s="114"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="67">
         <v>30</v>
       </c>
-      <c r="E4" s="94">
+      <c r="E4" s="78">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2045,18 +2046,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="139" t="s">
+      <c r="BB4" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="140"/>
-      <c r="BD4" s="80"/>
+      <c r="BC4" s="71"/>
+      <c r="BD4" s="145"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="95"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2105,24 +2106,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="139"/>
-      <c r="BC5" s="140"/>
-      <c r="BD5" s="80"/>
-      <c r="BF5" s="63" t="s">
+      <c r="BB5" s="70"/>
+      <c r="BC5" s="71"/>
+      <c r="BD5" s="145"/>
+      <c r="BF5" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="67"/>
+      <c r="BG5" s="139"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="83">
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="63">
         <v>1</v>
       </c>
-      <c r="E6" s="102">
+      <c r="E6" s="116">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2173,18 +2174,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="139"/>
-      <c r="BC6" s="140"/>
-      <c r="BD6" s="80"/>
-      <c r="BF6" s="64"/>
-      <c r="BG6" s="68"/>
+      <c r="BB6" s="70"/>
+      <c r="BC6" s="71"/>
+      <c r="BD6" s="145"/>
+      <c r="BF6" s="136"/>
+      <c r="BG6" s="140"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
-      <c r="B7" s="100"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="103"/>
+      <c r="A7" s="97"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="117"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2233,24 +2234,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="139"/>
-      <c r="BC7" s="140"/>
-      <c r="BD7" s="80"/>
-      <c r="BF7" s="63" t="s">
+      <c r="BB7" s="70"/>
+      <c r="BC7" s="71"/>
+      <c r="BD7" s="145"/>
+      <c r="BF7" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="69"/>
+      <c r="BG7" s="141"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="92">
+      <c r="B8" s="114"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="67">
         <v>1.5</v>
       </c>
-      <c r="E8" s="81">
+      <c r="E8" s="68">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
@@ -2301,20 +2302,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="139"/>
-      <c r="BC8" s="140"/>
-      <c r="BD8" s="73" t="s">
+      <c r="BB8" s="70"/>
+      <c r="BC8" s="71"/>
+      <c r="BD8" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="64"/>
-      <c r="BG8" s="70"/>
+      <c r="BF8" s="136"/>
+      <c r="BG8" s="142"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="115"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="66"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2363,24 +2364,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="139"/>
-      <c r="BC9" s="140"/>
-      <c r="BD9" s="73"/>
-      <c r="BF9" s="65" t="s">
+      <c r="BB9" s="70"/>
+      <c r="BC9" s="71"/>
+      <c r="BD9" s="69"/>
+      <c r="BF9" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="71"/>
+      <c r="BG9" s="143"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="83">
+      <c r="B10" s="88"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="63">
         <v>1.5</v>
       </c>
-      <c r="E10" s="85">
+      <c r="E10" s="65">
         <v>1</v>
       </c>
       <c r="F10" s="19"/>
@@ -2431,18 +2432,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="139"/>
-      <c r="BC10" s="140"/>
-      <c r="BD10" s="73"/>
-      <c r="BF10" s="66"/>
-      <c r="BG10" s="72"/>
+      <c r="BB10" s="70"/>
+      <c r="BC10" s="71"/>
+      <c r="BD10" s="69"/>
+      <c r="BF10" s="138"/>
+      <c r="BG10" s="144"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="82"/>
+      <c r="A11" s="97"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2491,20 +2492,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="139"/>
-      <c r="BC11" s="140"/>
-      <c r="BD11" s="73"/>
+      <c r="BB11" s="70"/>
+      <c r="BC11" s="71"/>
+      <c r="BD11" s="69"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="92">
+      <c r="B12" s="114"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="67">
         <v>1</v>
       </c>
-      <c r="E12" s="81">
+      <c r="E12" s="68">
         <v>1.2</v>
       </c>
       <c r="F12" s="19"/>
@@ -2555,9 +2556,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="139"/>
-      <c r="BC12" s="140"/>
-      <c r="BD12" s="73" t="s">
+      <c r="BB12" s="70"/>
+      <c r="BC12" s="71"/>
+      <c r="BD12" s="69" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2571,11 +2572,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="89"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="115"/>
+      <c r="A13" s="90"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2624,9 +2625,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="139"/>
-      <c r="BC13" s="140"/>
-      <c r="BD13" s="73"/>
+      <c r="BB13" s="70"/>
+      <c r="BC13" s="71"/>
+      <c r="BD13" s="69"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2638,15 +2639,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="97"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="83">
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="63">
         <v>2</v>
       </c>
-      <c r="E14" s="85">
+      <c r="E14" s="65">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2697,16 +2698,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="139"/>
-      <c r="BC14" s="140"/>
-      <c r="BD14" s="73"/>
+      <c r="BB14" s="70"/>
+      <c r="BC14" s="71"/>
+      <c r="BD14" s="69"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="89"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="115"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="66"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2755,20 +2756,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="139"/>
-      <c r="BC15" s="140"/>
-      <c r="BD15" s="73"/>
+      <c r="BB15" s="70"/>
+      <c r="BC15" s="71"/>
+      <c r="BD15" s="69"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="97"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="83">
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="63">
         <v>1</v>
       </c>
-      <c r="E16" s="85">
+      <c r="E16" s="65">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2819,16 +2820,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="139"/>
-      <c r="BC16" s="140"/>
-      <c r="BD16" s="73"/>
+      <c r="BB16" s="70"/>
+      <c r="BC16" s="71"/>
+      <c r="BD16" s="69"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="89"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="115"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2877,23 +2878,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="139"/>
-      <c r="BC17" s="140"/>
-      <c r="BD17" s="73"/>
+      <c r="BB17" s="70"/>
+      <c r="BC17" s="71"/>
+      <c r="BD17" s="69"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="97"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="83">
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="63">
         <v>2</v>
       </c>
-      <c r="E18" s="85">
+      <c r="E18" s="65">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2944,16 +2945,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="139"/>
-      <c r="BC18" s="140"/>
-      <c r="BD18" s="73"/>
+      <c r="BB18" s="70"/>
+      <c r="BC18" s="71"/>
+      <c r="BD18" s="69"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="89"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="115"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3002,20 +3003,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="139"/>
-      <c r="BC19" s="140"/>
-      <c r="BD19" s="73"/>
+      <c r="BB19" s="70"/>
+      <c r="BC19" s="71"/>
+      <c r="BD19" s="69"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="96" t="s">
+      <c r="A20" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="97"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="83">
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="63">
         <v>1</v>
       </c>
-      <c r="E20" s="85">
+      <c r="E20" s="65">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3066,16 +3067,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="139"/>
-      <c r="BC20" s="140"/>
-      <c r="BD20" s="73"/>
+      <c r="BB20" s="70"/>
+      <c r="BC20" s="71"/>
+      <c r="BD20" s="69"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="82"/>
+      <c r="A21" s="97"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3124,20 +3125,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="139"/>
-      <c r="BC21" s="140"/>
-      <c r="BD21" s="73"/>
+      <c r="BB21" s="70"/>
+      <c r="BC21" s="71"/>
+      <c r="BD21" s="69"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="86" t="s">
+      <c r="A22" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="92">
+      <c r="B22" s="114"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="67">
         <v>0.5</v>
       </c>
-      <c r="E22" s="81">
+      <c r="E22" s="68">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3188,18 +3189,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="139"/>
-      <c r="BC22" s="140"/>
-      <c r="BD22" s="73" t="s">
+      <c r="BB22" s="70"/>
+      <c r="BC22" s="71"/>
+      <c r="BD22" s="69" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="99"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="82"/>
+      <c r="A23" s="97"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="81"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3248,20 +3249,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="139"/>
-      <c r="BC23" s="140"/>
-      <c r="BD23" s="73"/>
+      <c r="BB23" s="70"/>
+      <c r="BC23" s="71"/>
+      <c r="BD23" s="69"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="92">
+      <c r="B24" s="114"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="67">
         <v>2</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E24" s="68">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3312,18 +3313,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="139"/>
-      <c r="BC24" s="140"/>
-      <c r="BD24" s="143" t="s">
+      <c r="BB24" s="70"/>
+      <c r="BC24" s="71"/>
+      <c r="BD24" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="115"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="66"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3372,20 +3373,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="139"/>
-      <c r="BC25" s="140"/>
-      <c r="BD25" s="144"/>
+      <c r="BB25" s="70"/>
+      <c r="BC25" s="71"/>
+      <c r="BD25" s="75"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="97"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="83">
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="63">
         <v>1</v>
       </c>
-      <c r="E26" s="85">
+      <c r="E26" s="65">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3436,16 +3437,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="139"/>
-      <c r="BC26" s="140"/>
-      <c r="BD26" s="144"/>
+      <c r="BB26" s="70"/>
+      <c r="BC26" s="71"/>
+      <c r="BD26" s="75"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="89"/>
-      <c r="B27" s="90"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="115"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="66"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3494,20 +3495,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="139"/>
-      <c r="BC27" s="140"/>
-      <c r="BD27" s="144"/>
+      <c r="BB27" s="70"/>
+      <c r="BC27" s="71"/>
+      <c r="BD27" s="75"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="97"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="83">
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="63">
         <v>2</v>
       </c>
-      <c r="E28" s="85">
+      <c r="E28" s="65">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3558,16 +3559,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="139"/>
-      <c r="BC28" s="140"/>
-      <c r="BD28" s="144"/>
+      <c r="BB28" s="70"/>
+      <c r="BC28" s="71"/>
+      <c r="BD28" s="75"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="89"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="115"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="66"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3616,20 +3617,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="139"/>
-      <c r="BC29" s="140"/>
-      <c r="BD29" s="144"/>
+      <c r="BB29" s="70"/>
+      <c r="BC29" s="71"/>
+      <c r="BD29" s="75"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="97"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="83">
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="63">
         <v>2</v>
       </c>
-      <c r="E30" s="85">
+      <c r="E30" s="65">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3680,16 +3681,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="139"/>
-      <c r="BC30" s="140"/>
-      <c r="BD30" s="144"/>
+      <c r="BB30" s="70"/>
+      <c r="BC30" s="71"/>
+      <c r="BD30" s="75"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="115"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="66"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3738,20 +3739,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="139"/>
-      <c r="BC31" s="140"/>
-      <c r="BD31" s="144"/>
+      <c r="BB31" s="70"/>
+      <c r="BC31" s="71"/>
+      <c r="BD31" s="75"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="96" t="s">
+      <c r="A32" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="97"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="83">
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="63">
         <v>4</v>
       </c>
-      <c r="E32" s="85">
+      <c r="E32" s="65">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3802,16 +3803,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="139"/>
-      <c r="BC32" s="140"/>
-      <c r="BD32" s="144"/>
+      <c r="BB32" s="70"/>
+      <c r="BC32" s="71"/>
+      <c r="BD32" s="75"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="89"/>
-      <c r="B33" s="90"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="115"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="66"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3860,20 +3861,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="139"/>
-      <c r="BC33" s="140"/>
-      <c r="BD33" s="144"/>
+      <c r="BB33" s="70"/>
+      <c r="BC33" s="71"/>
+      <c r="BD33" s="75"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="133" t="s">
+      <c r="A34" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="134"/>
-      <c r="C34" s="135"/>
-      <c r="D34" s="83">
+      <c r="B34" s="108"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="63">
         <v>3</v>
       </c>
-      <c r="E34" s="85">
+      <c r="E34" s="65">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3924,16 +3925,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="139"/>
-      <c r="BC34" s="140"/>
-      <c r="BD34" s="144"/>
+      <c r="BB34" s="70"/>
+      <c r="BC34" s="71"/>
+      <c r="BD34" s="75"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="136"/>
-      <c r="B35" s="137"/>
-      <c r="C35" s="138"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="115"/>
+      <c r="A35" s="110"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="66"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3982,20 +3983,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="139"/>
-      <c r="BC35" s="140"/>
-      <c r="BD35" s="144"/>
+      <c r="BB35" s="70"/>
+      <c r="BC35" s="71"/>
+      <c r="BD35" s="75"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="133" t="s">
+      <c r="A36" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="134"/>
-      <c r="C36" s="135"/>
-      <c r="D36" s="83">
+      <c r="B36" s="108"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="63">
         <v>4</v>
       </c>
-      <c r="E36" s="85">
+      <c r="E36" s="65">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4045,16 +4046,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="139"/>
-      <c r="BC36" s="140"/>
-      <c r="BD36" s="144"/>
+      <c r="BB36" s="70"/>
+      <c r="BC36" s="71"/>
+      <c r="BD36" s="75"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="136"/>
-      <c r="B37" s="137"/>
-      <c r="C37" s="138"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="115"/>
+      <c r="A37" s="110"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="66"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4103,20 +4104,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="139"/>
-      <c r="BC37" s="140"/>
-      <c r="BD37" s="144"/>
+      <c r="BB37" s="70"/>
+      <c r="BC37" s="71"/>
+      <c r="BD37" s="75"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="133" t="s">
+      <c r="A38" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="134"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="83">
+      <c r="B38" s="108"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="63">
         <v>1</v>
       </c>
-      <c r="E38" s="85">
+      <c r="E38" s="65">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4165,16 +4166,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="139"/>
-      <c r="BC38" s="140"/>
-      <c r="BD38" s="144"/>
+      <c r="BB38" s="70"/>
+      <c r="BC38" s="71"/>
+      <c r="BD38" s="75"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="136"/>
-      <c r="B39" s="137"/>
-      <c r="C39" s="138"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="115"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="66"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4223,20 +4224,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="139"/>
-      <c r="BC39" s="140"/>
-      <c r="BD39" s="144"/>
+      <c r="BB39" s="70"/>
+      <c r="BC39" s="71"/>
+      <c r="BD39" s="75"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="133" t="s">
+      <c r="A40" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="134"/>
-      <c r="C40" s="135"/>
-      <c r="D40" s="83">
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="63">
         <v>1</v>
       </c>
-      <c r="E40" s="85">
+      <c r="E40" s="65">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4288,16 +4289,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="139"/>
-      <c r="BC40" s="140"/>
-      <c r="BD40" s="144"/>
+      <c r="BB40" s="70"/>
+      <c r="BC40" s="71"/>
+      <c r="BD40" s="75"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="136"/>
-      <c r="B41" s="137"/>
-      <c r="C41" s="138"/>
-      <c r="D41" s="93"/>
-      <c r="E41" s="115"/>
+      <c r="A41" s="110"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="66"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4346,20 +4347,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="139"/>
-      <c r="BC41" s="140"/>
-      <c r="BD41" s="144"/>
+      <c r="BB41" s="70"/>
+      <c r="BC41" s="71"/>
+      <c r="BD41" s="75"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="96" t="s">
+      <c r="A42" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="97"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="83">
+      <c r="B42" s="88"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="63">
         <v>2</v>
       </c>
-      <c r="E42" s="85">
+      <c r="E42" s="65">
         <v>2.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -4410,16 +4411,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="139"/>
-      <c r="BC42" s="140"/>
-      <c r="BD42" s="144"/>
+      <c r="BB42" s="70"/>
+      <c r="BC42" s="71"/>
+      <c r="BD42" s="75"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="89"/>
-      <c r="B43" s="90"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="115"/>
+      <c r="A43" s="90"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="66"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4468,20 +4469,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="139"/>
-      <c r="BC43" s="140"/>
-      <c r="BD43" s="144"/>
+      <c r="BB43" s="70"/>
+      <c r="BC43" s="71"/>
+      <c r="BD43" s="75"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="97"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="83">
+      <c r="B44" s="88"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="63">
         <v>2</v>
       </c>
-      <c r="E44" s="85"/>
+      <c r="E44" s="65"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -4530,16 +4531,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="139"/>
-      <c r="BC44" s="140"/>
-      <c r="BD44" s="144"/>
+      <c r="BB44" s="70"/>
+      <c r="BC44" s="71"/>
+      <c r="BD44" s="75"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="99"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="101"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="82"/>
+      <c r="A45" s="97"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="81"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4563,7 +4564,7 @@
       <c r="Z45" s="10"/>
       <c r="AA45" s="11"/>
       <c r="AB45" s="38"/>
-      <c r="AC45" s="11"/>
+      <c r="AC45" s="38"/>
       <c r="AD45" s="12"/>
       <c r="AE45" s="10"/>
       <c r="AF45" s="11"/>
@@ -4588,20 +4589,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="139"/>
-      <c r="BC45" s="140"/>
-      <c r="BD45" s="145"/>
+      <c r="BB45" s="70"/>
+      <c r="BC45" s="71"/>
+      <c r="BD45" s="76"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="126" t="s">
+      <c r="A46" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="127"/>
-      <c r="C46" s="128"/>
-      <c r="D46" s="120">
+      <c r="B46" s="101"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="77">
         <v>1</v>
       </c>
-      <c r="E46" s="94"/>
+      <c r="E46" s="78"/>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4649,18 +4650,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="139"/>
-      <c r="BC46" s="140"/>
-      <c r="BD46" s="73" t="s">
+      <c r="BB46" s="70"/>
+      <c r="BC46" s="71"/>
+      <c r="BD46" s="69" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="89"/>
-      <c r="B47" s="90"/>
-      <c r="C47" s="91"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="95"/>
+      <c r="A47" s="90"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="79"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4684,7 +4685,7 @@
       <c r="Z47" s="43"/>
       <c r="AA47" s="9"/>
       <c r="AB47" s="9"/>
-      <c r="AC47" s="43"/>
+      <c r="AC47" s="146"/>
       <c r="AD47" s="4"/>
       <c r="AE47" s="43"/>
       <c r="AF47" s="9"/>
@@ -4709,20 +4710,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="139"/>
-      <c r="BC47" s="140"/>
-      <c r="BD47" s="73"/>
+      <c r="BB47" s="70"/>
+      <c r="BC47" s="71"/>
+      <c r="BD47" s="69"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="96" t="s">
+      <c r="A48" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="97"/>
-      <c r="C48" s="98"/>
-      <c r="D48" s="83">
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="63">
         <v>2</v>
       </c>
-      <c r="E48" s="85"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4771,16 +4772,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="139"/>
-      <c r="BC48" s="140"/>
-      <c r="BD48" s="73"/>
+      <c r="BB48" s="70"/>
+      <c r="BC48" s="71"/>
+      <c r="BD48" s="69"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="99"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="101"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="82"/>
+      <c r="A49" s="97"/>
+      <c r="B49" s="98"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="81"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4829,20 +4830,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="139"/>
-      <c r="BC49" s="140"/>
-      <c r="BD49" s="73"/>
+      <c r="BB49" s="70"/>
+      <c r="BC49" s="71"/>
+      <c r="BD49" s="69"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="122" t="s">
+      <c r="A50" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="123"/>
-      <c r="C50" s="123"/>
-      <c r="D50" s="120">
+      <c r="B50" s="94"/>
+      <c r="C50" s="94"/>
+      <c r="D50" s="77">
         <v>5</v>
       </c>
-      <c r="E50" s="121"/>
+      <c r="E50" s="82"/>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4891,18 +4892,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="139"/>
-      <c r="BC50" s="140"/>
-      <c r="BD50" s="73" t="s">
+      <c r="BB50" s="70"/>
+      <c r="BC50" s="71"/>
+      <c r="BD50" s="69" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="124"/>
-      <c r="B51" s="125"/>
-      <c r="C51" s="125"/>
-      <c r="D51" s="93"/>
-      <c r="E51" s="115"/>
+      <c r="A51" s="95"/>
+      <c r="B51" s="96"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="66"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4951,20 +4952,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="139"/>
-      <c r="BC51" s="140"/>
-      <c r="BD51" s="73"/>
+      <c r="BB51" s="70"/>
+      <c r="BC51" s="71"/>
+      <c r="BD51" s="69"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="96" t="s">
+      <c r="A52" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="97"/>
-      <c r="C52" s="98"/>
-      <c r="D52" s="83">
+      <c r="B52" s="88"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="63">
         <v>2</v>
       </c>
-      <c r="E52" s="85"/>
+      <c r="E52" s="65"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5005,16 +5006,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="23"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="139"/>
-      <c r="BC52" s="140"/>
-      <c r="BD52" s="73"/>
+      <c r="BB52" s="70"/>
+      <c r="BC52" s="71"/>
+      <c r="BD52" s="69"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="99"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="101"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="82"/>
+      <c r="A53" s="97"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="81"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5063,20 +5064,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="139"/>
-      <c r="BC53" s="140"/>
-      <c r="BD53" s="73"/>
+      <c r="BB53" s="70"/>
+      <c r="BC53" s="71"/>
+      <c r="BD53" s="69"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="126" t="s">
+      <c r="A54" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="127"/>
-      <c r="C54" s="128"/>
-      <c r="D54" s="120">
+      <c r="B54" s="101"/>
+      <c r="C54" s="102"/>
+      <c r="D54" s="77">
         <v>4.5</v>
       </c>
-      <c r="E54" s="121">
+      <c r="E54" s="82">
         <v>1</v>
       </c>
       <c r="F54" s="50"/>
@@ -5126,16 +5127,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="139"/>
-      <c r="BC54" s="140"/>
+      <c r="BB54" s="70"/>
+      <c r="BC54" s="71"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="89"/>
-      <c r="B55" s="90"/>
-      <c r="C55" s="91"/>
-      <c r="D55" s="93"/>
-      <c r="E55" s="115"/>
+      <c r="A55" s="90"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="64"/>
+      <c r="E55" s="66"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5184,16 +5185,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="139"/>
-      <c r="BC55" s="140"/>
+      <c r="BB55" s="70"/>
+      <c r="BC55" s="71"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="126"/>
-      <c r="B56" s="127"/>
-      <c r="C56" s="128"/>
-      <c r="D56" s="120"/>
-      <c r="E56" s="121"/>
+      <c r="A56" s="100"/>
+      <c r="B56" s="101"/>
+      <c r="C56" s="102"/>
+      <c r="D56" s="77"/>
+      <c r="E56" s="82"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5242,16 +5243,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="139"/>
-      <c r="BC56" s="140"/>
+      <c r="BB56" s="70"/>
+      <c r="BC56" s="71"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="89"/>
-      <c r="B57" s="90"/>
-      <c r="C57" s="91"/>
-      <c r="D57" s="93"/>
-      <c r="E57" s="115"/>
+      <c r="A57" s="90"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="66"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5300,16 +5301,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="139"/>
-      <c r="BC57" s="140"/>
+      <c r="BB57" s="70"/>
+      <c r="BC57" s="71"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="96"/>
-      <c r="B58" s="97"/>
-      <c r="C58" s="98"/>
-      <c r="D58" s="83"/>
-      <c r="E58" s="85"/>
+      <c r="A58" s="87"/>
+      <c r="B58" s="88"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="65"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5358,16 +5359,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="139"/>
-      <c r="BC58" s="140"/>
+      <c r="BB58" s="70"/>
+      <c r="BC58" s="71"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="101"/>
-      <c r="D59" s="84"/>
-      <c r="E59" s="82"/>
+      <c r="A59" s="97"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="81"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5416,35 +5417,135 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="141"/>
-      <c r="BC59" s="142"/>
+      <c r="BB59" s="72"/>
+      <c r="BC59" s="73"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="129" t="s">
+      <c r="A60" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="130"/>
-      <c r="C60" s="130"/>
-      <c r="D60" s="116">
+      <c r="B60" s="104"/>
+      <c r="C60" s="104"/>
+      <c r="D60" s="83">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="118">
+      <c r="E60" s="85">
         <f>SUM(E4:E59)</f>
         <v>63.7</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="131"/>
-      <c r="B61" s="132"/>
-      <c r="C61" s="132"/>
-      <c r="D61" s="117"/>
-      <c r="E61" s="119"/>
+      <c r="A61" s="105"/>
+      <c r="B61" s="106"/>
+      <c r="C61" s="106"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="86"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="D26:D27"/>
@@ -5469,106 +5570,6 @@
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BD3:BD7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing durch, mit einzelnen BugFixes funktioniert jetzt Tadellos.
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="662" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B9E74FF-B8D7-4533-A982-DBCFA78E7552}"/>
+  <xr:revisionPtr revIDLastSave="686" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CF938CD-BD89-478C-BB66-3CD445AA555F}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="45" windowWidth="26760" windowHeight="15420" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1009,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1078,6 +1078,222 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1109,224 +1325,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1650,8 +1651,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56:D57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S63" sqref="S63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,171 +1664,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="108" t="s">
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="110" t="s">
+      <c r="E1" s="126"/>
+      <c r="F1" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="75" t="s">
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="75" t="s">
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="75" t="s">
+      <c r="Q1" s="134"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="75" t="s">
+      <c r="V1" s="134"/>
+      <c r="W1" s="134"/>
+      <c r="X1" s="134"/>
+      <c r="Y1" s="135"/>
+      <c r="Z1" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="75" t="s">
+      <c r="AA1" s="134"/>
+      <c r="AB1" s="134"/>
+      <c r="AC1" s="134"/>
+      <c r="AD1" s="135"/>
+      <c r="AE1" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="76"/>
-      <c r="AG1" s="76"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="77"/>
-      <c r="AJ1" s="75" t="s">
+      <c r="AF1" s="134"/>
+      <c r="AG1" s="134"/>
+      <c r="AH1" s="134"/>
+      <c r="AI1" s="135"/>
+      <c r="AJ1" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="76"/>
-      <c r="AL1" s="76"/>
-      <c r="AM1" s="76"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="75" t="s">
+      <c r="AK1" s="134"/>
+      <c r="AL1" s="134"/>
+      <c r="AM1" s="134"/>
+      <c r="AN1" s="135"/>
+      <c r="AO1" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="76"/>
-      <c r="AQ1" s="76"/>
-      <c r="AR1" s="76"/>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="75" t="s">
+      <c r="AP1" s="134"/>
+      <c r="AQ1" s="134"/>
+      <c r="AR1" s="134"/>
+      <c r="AS1" s="135"/>
+      <c r="AT1" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="76"/>
-      <c r="AV1" s="76"/>
-      <c r="AW1" s="76"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="75" t="s">
+      <c r="AU1" s="134"/>
+      <c r="AV1" s="134"/>
+      <c r="AW1" s="134"/>
+      <c r="AX1" s="135"/>
+      <c r="AY1" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="76"/>
-      <c r="BA1" s="76"/>
-      <c r="BB1" s="76"/>
-      <c r="BC1" s="77"/>
-      <c r="BD1" s="74" t="s">
+      <c r="AZ1" s="134"/>
+      <c r="BA1" s="134"/>
+      <c r="BB1" s="134"/>
+      <c r="BC1" s="135"/>
+      <c r="BD1" s="70" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="113">
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="130">
         <v>44957</v>
       </c>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="78">
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="119">
         <v>44958</v>
       </c>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="78">
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="119">
         <v>44959</v>
       </c>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="78">
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="119">
         <v>44960</v>
       </c>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="80"/>
-      <c r="Z2" s="78">
+      <c r="V2" s="120"/>
+      <c r="W2" s="120"/>
+      <c r="X2" s="120"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="119">
         <v>44964</v>
       </c>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="79"/>
-      <c r="AD2" s="80"/>
-      <c r="AE2" s="78">
+      <c r="AA2" s="120"/>
+      <c r="AB2" s="120"/>
+      <c r="AC2" s="120"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="119">
         <v>44965</v>
       </c>
-      <c r="AF2" s="79"/>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="79"/>
-      <c r="AI2" s="80"/>
-      <c r="AJ2" s="78">
+      <c r="AF2" s="120"/>
+      <c r="AG2" s="120"/>
+      <c r="AH2" s="120"/>
+      <c r="AI2" s="121"/>
+      <c r="AJ2" s="119">
         <v>44966</v>
       </c>
-      <c r="AK2" s="79"/>
-      <c r="AL2" s="79"/>
-      <c r="AM2" s="79"/>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="78">
+      <c r="AK2" s="120"/>
+      <c r="AL2" s="120"/>
+      <c r="AM2" s="120"/>
+      <c r="AN2" s="121"/>
+      <c r="AO2" s="119">
         <v>44967</v>
       </c>
-      <c r="AP2" s="79"/>
-      <c r="AQ2" s="79"/>
-      <c r="AR2" s="79"/>
-      <c r="AS2" s="80"/>
-      <c r="AT2" s="78">
+      <c r="AP2" s="120"/>
+      <c r="AQ2" s="120"/>
+      <c r="AR2" s="120"/>
+      <c r="AS2" s="121"/>
+      <c r="AT2" s="119">
         <v>44971</v>
       </c>
-      <c r="AU2" s="79"/>
-      <c r="AV2" s="79"/>
-      <c r="AW2" s="79"/>
-      <c r="AX2" s="80"/>
-      <c r="AY2" s="78">
+      <c r="AU2" s="120"/>
+      <c r="AV2" s="120"/>
+      <c r="AW2" s="120"/>
+      <c r="AX2" s="121"/>
+      <c r="AY2" s="119">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="79"/>
-      <c r="BA2" s="79"/>
-      <c r="BB2" s="79"/>
-      <c r="BC2" s="80"/>
-      <c r="BD2" s="74"/>
+      <c r="AZ2" s="120"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="120"/>
+      <c r="BC2" s="121"/>
+      <c r="BD2" s="70"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="107"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1984,18 +1985,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="81"/>
+      <c r="BD3" s="146"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="93">
+      <c r="B4" s="115"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="68">
         <v>30</v>
       </c>
-      <c r="E4" s="95">
+      <c r="E4" s="79">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2046,18 +2047,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="140" t="s">
+      <c r="BB4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="81"/>
+      <c r="BC4" s="72"/>
+      <c r="BD4" s="146"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="96"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2079,14 +2080,14 @@
       <c r="X5" s="30"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="8"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="30"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="8"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="8"/>
       <c r="AK5" s="9"/>
@@ -2106,24 +2107,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="140"/>
-      <c r="BC5" s="141"/>
-      <c r="BD5" s="81"/>
-      <c r="BF5" s="64" t="s">
+      <c r="BB5" s="71"/>
+      <c r="BC5" s="72"/>
+      <c r="BD5" s="146"/>
+      <c r="BF5" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="68"/>
+      <c r="BG5" s="140"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="84">
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="64">
         <v>1</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="117">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2174,18 +2175,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="140"/>
-      <c r="BC6" s="141"/>
-      <c r="BD6" s="81"/>
-      <c r="BF6" s="65"/>
-      <c r="BG6" s="69"/>
+      <c r="BB6" s="71"/>
+      <c r="BC6" s="72"/>
+      <c r="BD6" s="146"/>
+      <c r="BF6" s="137"/>
+      <c r="BG6" s="141"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="104"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="118"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2234,24 +2235,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="140"/>
-      <c r="BC7" s="141"/>
-      <c r="BD7" s="81"/>
-      <c r="BF7" s="64" t="s">
+      <c r="BB7" s="71"/>
+      <c r="BC7" s="72"/>
+      <c r="BD7" s="146"/>
+      <c r="BF7" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="70"/>
+      <c r="BG7" s="142"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="93">
+      <c r="B8" s="115"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="68">
         <v>1.5</v>
       </c>
-      <c r="E8" s="82">
+      <c r="E8" s="69">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
@@ -2302,20 +2303,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="140"/>
-      <c r="BC8" s="141"/>
-      <c r="BD8" s="74" t="s">
+      <c r="BB8" s="71"/>
+      <c r="BC8" s="72"/>
+      <c r="BD8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="65"/>
-      <c r="BG8" s="71"/>
+      <c r="BF8" s="137"/>
+      <c r="BG8" s="143"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="116"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2341,7 +2342,7 @@
       <c r="AB9" s="9"/>
       <c r="AC9" s="9"/>
       <c r="AD9" s="4"/>
-      <c r="AE9" s="8"/>
+      <c r="AE9" s="36"/>
       <c r="AF9" s="9"/>
       <c r="AG9" s="9"/>
       <c r="AH9" s="9"/>
@@ -2364,25 +2365,25 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="140"/>
-      <c r="BC9" s="141"/>
-      <c r="BD9" s="74"/>
-      <c r="BF9" s="66" t="s">
+      <c r="BB9" s="71"/>
+      <c r="BC9" s="72"/>
+      <c r="BD9" s="70"/>
+      <c r="BF9" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="72"/>
+      <c r="BG9" s="144"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="84">
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="64">
         <v>1.5</v>
       </c>
-      <c r="E10" s="86">
-        <v>1</v>
+      <c r="E10" s="66">
+        <v>1.5</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
@@ -2432,18 +2433,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="140"/>
-      <c r="BC10" s="141"/>
-      <c r="BD10" s="74"/>
-      <c r="BF10" s="67"/>
-      <c r="BG10" s="73"/>
+      <c r="BB10" s="71"/>
+      <c r="BC10" s="72"/>
+      <c r="BD10" s="70"/>
+      <c r="BF10" s="139"/>
+      <c r="BG10" s="145"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="83"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2469,7 +2470,7 @@
       <c r="AB11" s="11"/>
       <c r="AC11" s="11"/>
       <c r="AD11" s="12"/>
-      <c r="AE11" s="10"/>
+      <c r="AE11" s="37"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="11"/>
       <c r="AH11" s="11"/>
@@ -2492,21 +2493,21 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="140"/>
-      <c r="BC11" s="141"/>
-      <c r="BD11" s="74"/>
+      <c r="BB11" s="71"/>
+      <c r="BC11" s="72"/>
+      <c r="BD11" s="70"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="93">
+      <c r="B12" s="115"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="68">
         <v>1</v>
       </c>
-      <c r="E12" s="82">
-        <v>1.2</v>
+      <c r="E12" s="69">
+        <v>1.5</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="22"/>
@@ -2556,9 +2557,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="140"/>
-      <c r="BC12" s="141"/>
-      <c r="BD12" s="74" t="s">
+      <c r="BB12" s="71"/>
+      <c r="BC12" s="72"/>
+      <c r="BD12" s="70" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2572,11 +2573,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="116"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2625,9 +2626,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="140"/>
-      <c r="BC13" s="141"/>
-      <c r="BD13" s="74"/>
+      <c r="BB13" s="71"/>
+      <c r="BC13" s="72"/>
+      <c r="BD13" s="70"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2639,15 +2640,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="98"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="84">
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="64">
         <v>2</v>
       </c>
-      <c r="E14" s="86">
+      <c r="E14" s="66">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2698,16 +2699,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="140"/>
-      <c r="BC14" s="141"/>
-      <c r="BD14" s="74"/>
+      <c r="BB14" s="71"/>
+      <c r="BC14" s="72"/>
+      <c r="BD14" s="70"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="90"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="116"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2756,20 +2757,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="140"/>
-      <c r="BC15" s="141"/>
-      <c r="BD15" s="74"/>
+      <c r="BB15" s="71"/>
+      <c r="BC15" s="72"/>
+      <c r="BD15" s="70"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="98"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="84">
+      <c r="B16" s="89"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="64">
         <v>1</v>
       </c>
-      <c r="E16" s="86">
+      <c r="E16" s="66">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2820,16 +2821,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="140"/>
-      <c r="BC16" s="141"/>
-      <c r="BD16" s="74"/>
+      <c r="BB16" s="71"/>
+      <c r="BC16" s="72"/>
+      <c r="BD16" s="70"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="90"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="116"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2878,23 +2879,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="140"/>
-      <c r="BC17" s="141"/>
-      <c r="BD17" s="74"/>
+      <c r="BB17" s="71"/>
+      <c r="BC17" s="72"/>
+      <c r="BD17" s="70"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="98"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="84">
+      <c r="B18" s="89"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="64">
         <v>2</v>
       </c>
-      <c r="E18" s="86">
+      <c r="E18" s="66">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2945,16 +2946,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="140"/>
-      <c r="BC18" s="141"/>
-      <c r="BD18" s="74"/>
+      <c r="BB18" s="71"/>
+      <c r="BC18" s="72"/>
+      <c r="BD18" s="70"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="90"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="116"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3003,20 +3004,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="140"/>
-      <c r="BC19" s="141"/>
-      <c r="BD19" s="74"/>
+      <c r="BB19" s="71"/>
+      <c r="BC19" s="72"/>
+      <c r="BD19" s="70"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="84">
+      <c r="B20" s="89"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="64">
         <v>1</v>
       </c>
-      <c r="E20" s="86">
+      <c r="E20" s="66">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3067,16 +3068,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="140"/>
-      <c r="BC20" s="141"/>
-      <c r="BD20" s="74"/>
+      <c r="BB20" s="71"/>
+      <c r="BC20" s="72"/>
+      <c r="BD20" s="70"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="83"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="82"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3125,20 +3126,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="140"/>
-      <c r="BC21" s="141"/>
-      <c r="BD21" s="74"/>
+      <c r="BB21" s="71"/>
+      <c r="BC21" s="72"/>
+      <c r="BD21" s="70"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="93">
+      <c r="B22" s="115"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="68">
         <v>0.5</v>
       </c>
-      <c r="E22" s="82">
+      <c r="E22" s="69">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3189,18 +3190,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="140"/>
-      <c r="BC22" s="141"/>
-      <c r="BD22" s="74" t="s">
+      <c r="BB22" s="71"/>
+      <c r="BC22" s="72"/>
+      <c r="BD22" s="70" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="101"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="83"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3249,20 +3250,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="140"/>
-      <c r="BC23" s="141"/>
-      <c r="BD23" s="74"/>
+      <c r="BB23" s="71"/>
+      <c r="BC23" s="72"/>
+      <c r="BD23" s="70"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="93">
+      <c r="B24" s="115"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="68">
         <v>2</v>
       </c>
-      <c r="E24" s="82">
+      <c r="E24" s="69">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3313,18 +3314,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="140"/>
-      <c r="BC24" s="141"/>
-      <c r="BD24" s="144" t="s">
+      <c r="BB24" s="71"/>
+      <c r="BC24" s="72"/>
+      <c r="BD24" s="75" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="116"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="67"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3373,20 +3374,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="140"/>
-      <c r="BC25" s="141"/>
-      <c r="BD25" s="145"/>
+      <c r="BB25" s="71"/>
+      <c r="BC25" s="72"/>
+      <c r="BD25" s="76"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="98"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="84">
+      <c r="B26" s="89"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="64">
         <v>1</v>
       </c>
-      <c r="E26" s="86">
+      <c r="E26" s="66">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3437,16 +3438,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="140"/>
-      <c r="BC26" s="141"/>
-      <c r="BD26" s="145"/>
+      <c r="BB26" s="71"/>
+      <c r="BC26" s="72"/>
+      <c r="BD26" s="76"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="90"/>
-      <c r="B27" s="91"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="116"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3495,20 +3496,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="140"/>
-      <c r="BC27" s="141"/>
-      <c r="BD27" s="145"/>
+      <c r="BB27" s="71"/>
+      <c r="BC27" s="72"/>
+      <c r="BD27" s="76"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="84">
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="64">
         <v>2</v>
       </c>
-      <c r="E28" s="86">
+      <c r="E28" s="66">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3559,16 +3560,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="140"/>
-      <c r="BC28" s="141"/>
-      <c r="BD28" s="145"/>
+      <c r="BB28" s="71"/>
+      <c r="BC28" s="72"/>
+      <c r="BD28" s="76"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="90"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="92"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="116"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="67"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3617,20 +3618,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="140"/>
-      <c r="BC29" s="141"/>
-      <c r="BD29" s="145"/>
+      <c r="BB29" s="71"/>
+      <c r="BC29" s="72"/>
+      <c r="BD29" s="76"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="97" t="s">
+      <c r="A30" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="98"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="84">
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="64">
         <v>2</v>
       </c>
-      <c r="E30" s="86">
+      <c r="E30" s="66">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3681,16 +3682,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="140"/>
-      <c r="BC30" s="141"/>
-      <c r="BD30" s="145"/>
+      <c r="BB30" s="71"/>
+      <c r="BC30" s="72"/>
+      <c r="BD30" s="76"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="90"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="116"/>
+      <c r="A31" s="91"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="67"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3739,20 +3740,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="140"/>
-      <c r="BC31" s="141"/>
-      <c r="BD31" s="145"/>
+      <c r="BB31" s="71"/>
+      <c r="BC31" s="72"/>
+      <c r="BD31" s="76"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="97" t="s">
+      <c r="A32" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="98"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="84">
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="64">
         <v>4</v>
       </c>
-      <c r="E32" s="86">
+      <c r="E32" s="66">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3803,16 +3804,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="140"/>
-      <c r="BC32" s="141"/>
-      <c r="BD32" s="145"/>
+      <c r="BB32" s="71"/>
+      <c r="BC32" s="72"/>
+      <c r="BD32" s="76"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
-      <c r="B33" s="91"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="116"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3861,20 +3862,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="140"/>
-      <c r="BC33" s="141"/>
-      <c r="BD33" s="145"/>
+      <c r="BB33" s="71"/>
+      <c r="BC33" s="72"/>
+      <c r="BD33" s="76"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="134" t="s">
+      <c r="A34" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="135"/>
-      <c r="C34" s="136"/>
-      <c r="D34" s="84">
+      <c r="B34" s="109"/>
+      <c r="C34" s="110"/>
+      <c r="D34" s="64">
         <v>3</v>
       </c>
-      <c r="E34" s="86">
+      <c r="E34" s="66">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3925,16 +3926,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="140"/>
-      <c r="BC34" s="141"/>
-      <c r="BD34" s="145"/>
+      <c r="BB34" s="71"/>
+      <c r="BC34" s="72"/>
+      <c r="BD34" s="76"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="137"/>
-      <c r="B35" s="138"/>
-      <c r="C35" s="139"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="116"/>
+      <c r="A35" s="111"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="67"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3951,7 +3952,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="32"/>
       <c r="U35" s="36"/>
-      <c r="V35" s="9"/>
+      <c r="V35" s="147"/>
       <c r="W35" s="9"/>
       <c r="X35" s="9"/>
       <c r="Y35" s="4"/>
@@ -3983,20 +3984,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="140"/>
-      <c r="BC35" s="141"/>
-      <c r="BD35" s="145"/>
+      <c r="BB35" s="71"/>
+      <c r="BC35" s="72"/>
+      <c r="BD35" s="76"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="134" t="s">
+      <c r="A36" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="135"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="84">
+      <c r="B36" s="109"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="64">
         <v>4</v>
       </c>
-      <c r="E36" s="86">
+      <c r="E36" s="66">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4046,16 +4047,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="140"/>
-      <c r="BC36" s="141"/>
-      <c r="BD36" s="145"/>
+      <c r="BB36" s="71"/>
+      <c r="BC36" s="72"/>
+      <c r="BD36" s="76"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="137"/>
-      <c r="B37" s="138"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="116"/>
+      <c r="A37" s="111"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="67"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4104,20 +4105,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="140"/>
-      <c r="BC37" s="141"/>
-      <c r="BD37" s="145"/>
+      <c r="BB37" s="71"/>
+      <c r="BC37" s="72"/>
+      <c r="BD37" s="76"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="134" t="s">
+      <c r="A38" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="135"/>
-      <c r="C38" s="136"/>
-      <c r="D38" s="84">
+      <c r="B38" s="109"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="64">
         <v>1</v>
       </c>
-      <c r="E38" s="86">
+      <c r="E38" s="66">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4166,16 +4167,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="140"/>
-      <c r="BC38" s="141"/>
-      <c r="BD38" s="145"/>
+      <c r="BB38" s="71"/>
+      <c r="BC38" s="72"/>
+      <c r="BD38" s="76"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="137"/>
-      <c r="B39" s="138"/>
-      <c r="C39" s="139"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="116"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4224,20 +4225,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="140"/>
-      <c r="BC39" s="141"/>
-      <c r="BD39" s="145"/>
+      <c r="BB39" s="71"/>
+      <c r="BC39" s="72"/>
+      <c r="BD39" s="76"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="134" t="s">
+      <c r="A40" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="135"/>
-      <c r="C40" s="136"/>
-      <c r="D40" s="84">
+      <c r="B40" s="109"/>
+      <c r="C40" s="110"/>
+      <c r="D40" s="64">
         <v>1</v>
       </c>
-      <c r="E40" s="86">
+      <c r="E40" s="66">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4289,16 +4290,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="140"/>
-      <c r="BC40" s="141"/>
-      <c r="BD40" s="145"/>
+      <c r="BB40" s="71"/>
+      <c r="BC40" s="72"/>
+      <c r="BD40" s="76"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="137"/>
-      <c r="B41" s="138"/>
-      <c r="C41" s="139"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="116"/>
+      <c r="A41" s="111"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="67"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4318,7 +4319,7 @@
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
       <c r="X41" s="30"/>
-      <c r="Y41" s="4"/>
+      <c r="Y41" s="47"/>
       <c r="Z41" s="8"/>
       <c r="AA41" s="9"/>
       <c r="AB41" s="9"/>
@@ -4347,20 +4348,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="140"/>
-      <c r="BC41" s="141"/>
-      <c r="BD41" s="145"/>
+      <c r="BB41" s="71"/>
+      <c r="BC41" s="72"/>
+      <c r="BD41" s="76"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="97" t="s">
+      <c r="A42" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="98"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="84">
+      <c r="B42" s="89"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="64">
         <v>2</v>
       </c>
-      <c r="E42" s="86">
+      <c r="E42" s="66">
         <v>2.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -4411,16 +4412,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="140"/>
-      <c r="BC42" s="141"/>
-      <c r="BD42" s="145"/>
+      <c r="BB42" s="71"/>
+      <c r="BC42" s="72"/>
+      <c r="BD42" s="76"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="116"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="93"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="67"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4443,7 +4444,7 @@
       <c r="Y43" s="4"/>
       <c r="Z43" s="36"/>
       <c r="AA43" s="30"/>
-      <c r="AB43" s="24"/>
+      <c r="AB43" s="30"/>
       <c r="AC43" s="9"/>
       <c r="AD43" s="4"/>
       <c r="AE43" s="8"/>
@@ -4469,20 +4470,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="140"/>
-      <c r="BC43" s="141"/>
-      <c r="BD43" s="145"/>
+      <c r="BB43" s="71"/>
+      <c r="BC43" s="72"/>
+      <c r="BD43" s="76"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="97" t="s">
+      <c r="A44" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="84">
+      <c r="B44" s="89"/>
+      <c r="C44" s="90"/>
+      <c r="D44" s="64">
         <v>2</v>
       </c>
-      <c r="E44" s="86">
+      <c r="E44" s="66">
         <v>2</v>
       </c>
       <c r="F44" s="8"/>
@@ -4533,16 +4534,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="140"/>
-      <c r="BC44" s="141"/>
-      <c r="BD44" s="145"/>
+      <c r="BB44" s="71"/>
+      <c r="BC44" s="72"/>
+      <c r="BD44" s="76"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="100"/>
-      <c r="B45" s="101"/>
-      <c r="C45" s="102"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="83"/>
+      <c r="A45" s="98"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="100"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="82"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4591,20 +4592,22 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="140"/>
-      <c r="BC45" s="141"/>
-      <c r="BD45" s="146"/>
+      <c r="BB45" s="71"/>
+      <c r="BC45" s="72"/>
+      <c r="BD45" s="77"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="127" t="s">
+      <c r="A46" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="128"/>
-      <c r="C46" s="129"/>
-      <c r="D46" s="121">
+      <c r="B46" s="102"/>
+      <c r="C46" s="103"/>
+      <c r="D46" s="78">
         <v>1</v>
       </c>
-      <c r="E46" s="95"/>
+      <c r="E46" s="79">
+        <v>1.5</v>
+      </c>
       <c r="F46" s="50"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -4652,18 +4655,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="140"/>
-      <c r="BC46" s="141"/>
-      <c r="BD46" s="74" t="s">
+      <c r="BB46" s="71"/>
+      <c r="BC46" s="72"/>
+      <c r="BD46" s="70" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="90"/>
-      <c r="B47" s="91"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="96"/>
+      <c r="A47" s="91"/>
+      <c r="B47" s="92"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="80"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4689,7 +4692,7 @@
       <c r="AB47" s="9"/>
       <c r="AC47" s="63"/>
       <c r="AD47" s="4"/>
-      <c r="AE47" s="43"/>
+      <c r="AE47" s="63"/>
       <c r="AF47" s="9"/>
       <c r="AG47" s="9"/>
       <c r="AH47" s="9"/>
@@ -4712,20 +4715,22 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="140"/>
-      <c r="BC47" s="141"/>
-      <c r="BD47" s="74"/>
+      <c r="BB47" s="71"/>
+      <c r="BC47" s="72"/>
+      <c r="BD47" s="70"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="97" t="s">
+      <c r="A48" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="98"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="84">
+      <c r="B48" s="89"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="64">
         <v>2</v>
       </c>
-      <c r="E48" s="86"/>
+      <c r="E48" s="66">
+        <v>3</v>
+      </c>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -4774,16 +4779,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="140"/>
-      <c r="BC48" s="141"/>
-      <c r="BD48" s="74"/>
+      <c r="BB48" s="71"/>
+      <c r="BC48" s="72"/>
+      <c r="BD48" s="70"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="100"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="102"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="83"/>
+      <c r="A49" s="98"/>
+      <c r="B49" s="99"/>
+      <c r="C49" s="100"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="82"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4809,9 +4814,9 @@
       <c r="AB49" s="11"/>
       <c r="AC49" s="11"/>
       <c r="AD49" s="12"/>
-      <c r="AE49" s="10"/>
-      <c r="AF49" s="11"/>
-      <c r="AG49" s="11"/>
+      <c r="AE49" s="37"/>
+      <c r="AF49" s="38"/>
+      <c r="AG49" s="38"/>
       <c r="AH49" s="11"/>
       <c r="AI49" s="12"/>
       <c r="AJ49" s="10"/>
@@ -4832,20 +4837,22 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="140"/>
-      <c r="BC49" s="141"/>
-      <c r="BD49" s="74"/>
+      <c r="BB49" s="71"/>
+      <c r="BC49" s="72"/>
+      <c r="BD49" s="70"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="123" t="s">
+      <c r="A50" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="124"/>
-      <c r="C50" s="124"/>
-      <c r="D50" s="121">
+      <c r="B50" s="95"/>
+      <c r="C50" s="95"/>
+      <c r="D50" s="78">
         <v>5</v>
       </c>
-      <c r="E50" s="122"/>
+      <c r="E50" s="83">
+        <v>5</v>
+      </c>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
@@ -4894,18 +4901,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="140"/>
-      <c r="BC50" s="141"/>
-      <c r="BD50" s="74" t="s">
+      <c r="BB50" s="71"/>
+      <c r="BC50" s="72"/>
+      <c r="BD50" s="70" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="125"/>
-      <c r="B51" s="126"/>
-      <c r="C51" s="126"/>
-      <c r="D51" s="94"/>
-      <c r="E51" s="116"/>
+      <c r="A51" s="96"/>
+      <c r="B51" s="97"/>
+      <c r="C51" s="97"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="67"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4954,20 +4961,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="140"/>
-      <c r="BC51" s="141"/>
-      <c r="BD51" s="74"/>
+      <c r="BB51" s="71"/>
+      <c r="BC51" s="72"/>
+      <c r="BD51" s="70"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="97" t="s">
+      <c r="A52" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="98"/>
-      <c r="C52" s="99"/>
-      <c r="D52" s="84">
+      <c r="B52" s="89"/>
+      <c r="C52" s="90"/>
+      <c r="D52" s="64">
         <v>2</v>
       </c>
-      <c r="E52" s="86"/>
+      <c r="E52" s="66"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5006,18 +5013,18 @@
       <c r="AV52" s="23"/>
       <c r="AX52" s="51"/>
       <c r="AY52" s="50"/>
-      <c r="AZ52" s="23"/>
+      <c r="AZ52" s="44"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="140"/>
-      <c r="BC52" s="141"/>
-      <c r="BD52" s="74"/>
+      <c r="BB52" s="71"/>
+      <c r="BC52" s="72"/>
+      <c r="BD52" s="70"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="100"/>
-      <c r="B53" s="101"/>
-      <c r="C53" s="102"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="83"/>
+      <c r="A53" s="98"/>
+      <c r="B53" s="99"/>
+      <c r="C53" s="100"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="82"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5066,20 +5073,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="140"/>
-      <c r="BC53" s="141"/>
-      <c r="BD53" s="74"/>
+      <c r="BB53" s="71"/>
+      <c r="BC53" s="72"/>
+      <c r="BD53" s="70"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="127" t="s">
+      <c r="A54" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="128"/>
-      <c r="C54" s="129"/>
-      <c r="D54" s="121">
+      <c r="B54" s="102"/>
+      <c r="C54" s="103"/>
+      <c r="D54" s="78">
         <v>4.5</v>
       </c>
-      <c r="E54" s="122">
+      <c r="E54" s="83">
         <v>2</v>
       </c>
       <c r="F54" s="50"/>
@@ -5129,16 +5136,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="140"/>
-      <c r="BC54" s="141"/>
+      <c r="BB54" s="71"/>
+      <c r="BC54" s="72"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="90"/>
-      <c r="B55" s="91"/>
-      <c r="C55" s="92"/>
-      <c r="D55" s="94"/>
-      <c r="E55" s="116"/>
+      <c r="A55" s="91"/>
+      <c r="B55" s="92"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="67"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5187,16 +5194,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="140"/>
-      <c r="BC55" s="141"/>
+      <c r="BB55" s="71"/>
+      <c r="BC55" s="72"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="127"/>
-      <c r="B56" s="128"/>
-      <c r="C56" s="129"/>
-      <c r="D56" s="121"/>
-      <c r="E56" s="122"/>
+      <c r="A56" s="101"/>
+      <c r="B56" s="102"/>
+      <c r="C56" s="103"/>
+      <c r="D56" s="78"/>
+      <c r="E56" s="83"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5245,16 +5252,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="140"/>
-      <c r="BC56" s="141"/>
+      <c r="BB56" s="71"/>
+      <c r="BC56" s="72"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="90"/>
-      <c r="B57" s="91"/>
-      <c r="C57" s="92"/>
-      <c r="D57" s="94"/>
-      <c r="E57" s="116"/>
+      <c r="A57" s="91"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="93"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="67"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5303,16 +5310,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="140"/>
-      <c r="BC57" s="141"/>
+      <c r="BB57" s="71"/>
+      <c r="BC57" s="72"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="97"/>
-      <c r="B58" s="98"/>
-      <c r="C58" s="99"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="86"/>
+      <c r="A58" s="88"/>
+      <c r="B58" s="89"/>
+      <c r="C58" s="90"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="66"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5361,16 +5368,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="140"/>
-      <c r="BC58" s="141"/>
+      <c r="BB58" s="71"/>
+      <c r="BC58" s="72"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="100"/>
-      <c r="B59" s="101"/>
-      <c r="C59" s="102"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="83"/>
+      <c r="A59" s="98"/>
+      <c r="B59" s="99"/>
+      <c r="C59" s="100"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="82"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5419,35 +5426,135 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="142"/>
-      <c r="BC59" s="143"/>
+      <c r="BB59" s="73"/>
+      <c r="BC59" s="74"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="130" t="s">
+      <c r="A60" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="131"/>
-      <c r="C60" s="131"/>
-      <c r="D60" s="117">
+      <c r="B60" s="105"/>
+      <c r="C60" s="105"/>
+      <c r="D60" s="84">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="119">
+      <c r="E60" s="86">
         <f>SUM(E4:E59)</f>
-        <v>66.7</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="132"/>
-      <c r="B61" s="133"/>
-      <c r="C61" s="133"/>
-      <c r="D61" s="118"/>
-      <c r="E61" s="120"/>
+      <c r="A61" s="106"/>
+      <c r="B61" s="107"/>
+      <c r="C61" s="107"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="87"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="D26:D27"/>
@@ -5472,106 +5579,6 @@
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BD3:BD7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Doku, Arboeitsjournal, Bugs, Layoutänderungen, TestRapporte
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="686" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CF938CD-BD89-478C-BB66-3CD445AA555F}"/>
+  <xr:revisionPtr revIDLastSave="692" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4530C779-012A-41CF-866D-1AFB4CB3BDB6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1078,26 +1078,234 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1120,214 +1328,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1652,7 +1652,7 @@
   <dimension ref="A1:BN62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S63" sqref="S63"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,171 +1664,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="125" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="126"/>
-      <c r="F1" s="127" t="s">
+      <c r="E1" s="110"/>
+      <c r="F1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="133" t="s">
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="133" t="s">
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="134"/>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
-      <c r="T1" s="135"/>
-      <c r="U1" s="133" t="s">
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="134"/>
-      <c r="W1" s="134"/>
-      <c r="X1" s="134"/>
-      <c r="Y1" s="135"/>
-      <c r="Z1" s="133" t="s">
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="134"/>
-      <c r="AB1" s="134"/>
-      <c r="AC1" s="134"/>
-      <c r="AD1" s="135"/>
-      <c r="AE1" s="133" t="s">
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="134"/>
-      <c r="AG1" s="134"/>
-      <c r="AH1" s="134"/>
-      <c r="AI1" s="135"/>
-      <c r="AJ1" s="133" t="s">
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="134"/>
-      <c r="AL1" s="134"/>
-      <c r="AM1" s="134"/>
-      <c r="AN1" s="135"/>
-      <c r="AO1" s="133" t="s">
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="134"/>
-      <c r="AQ1" s="134"/>
-      <c r="AR1" s="134"/>
-      <c r="AS1" s="135"/>
-      <c r="AT1" s="133" t="s">
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="134"/>
-      <c r="AV1" s="134"/>
-      <c r="AW1" s="134"/>
-      <c r="AX1" s="135"/>
-      <c r="AY1" s="133" t="s">
+      <c r="AU1" s="77"/>
+      <c r="AV1" s="77"/>
+      <c r="AW1" s="77"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="134"/>
-      <c r="BA1" s="134"/>
-      <c r="BB1" s="134"/>
-      <c r="BC1" s="135"/>
-      <c r="BD1" s="70" t="s">
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="77"/>
+      <c r="BB1" s="77"/>
+      <c r="BC1" s="78"/>
+      <c r="BD1" s="75" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="130">
+      <c r="A2" s="107"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="114">
         <v>44957</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="119">
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="79">
         <v>44958</v>
       </c>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="119">
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="79">
         <v>44959</v>
       </c>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="119">
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="79">
         <v>44960</v>
       </c>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="121"/>
-      <c r="Z2" s="119">
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="79">
         <v>44964</v>
       </c>
-      <c r="AA2" s="120"/>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="120"/>
-      <c r="AD2" s="121"/>
-      <c r="AE2" s="119">
+      <c r="AA2" s="80"/>
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="80"/>
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="79">
         <v>44965</v>
       </c>
-      <c r="AF2" s="120"/>
-      <c r="AG2" s="120"/>
-      <c r="AH2" s="120"/>
-      <c r="AI2" s="121"/>
-      <c r="AJ2" s="119">
+      <c r="AF2" s="80"/>
+      <c r="AG2" s="80"/>
+      <c r="AH2" s="80"/>
+      <c r="AI2" s="81"/>
+      <c r="AJ2" s="79">
         <v>44966</v>
       </c>
-      <c r="AK2" s="120"/>
-      <c r="AL2" s="120"/>
-      <c r="AM2" s="120"/>
-      <c r="AN2" s="121"/>
-      <c r="AO2" s="119">
+      <c r="AK2" s="80"/>
+      <c r="AL2" s="80"/>
+      <c r="AM2" s="80"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="79">
         <v>44967</v>
       </c>
-      <c r="AP2" s="120"/>
-      <c r="AQ2" s="120"/>
-      <c r="AR2" s="120"/>
-      <c r="AS2" s="121"/>
-      <c r="AT2" s="119">
+      <c r="AP2" s="80"/>
+      <c r="AQ2" s="80"/>
+      <c r="AR2" s="80"/>
+      <c r="AS2" s="81"/>
+      <c r="AT2" s="79">
         <v>44971</v>
       </c>
-      <c r="AU2" s="120"/>
-      <c r="AV2" s="120"/>
-      <c r="AW2" s="120"/>
-      <c r="AX2" s="121"/>
-      <c r="AY2" s="119">
+      <c r="AU2" s="80"/>
+      <c r="AV2" s="80"/>
+      <c r="AW2" s="80"/>
+      <c r="AX2" s="81"/>
+      <c r="AY2" s="79">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="120"/>
-      <c r="BA2" s="120"/>
-      <c r="BB2" s="120"/>
-      <c r="BC2" s="121"/>
-      <c r="BD2" s="70"/>
+      <c r="AZ2" s="80"/>
+      <c r="BA2" s="80"/>
+      <c r="BB2" s="80"/>
+      <c r="BC2" s="81"/>
+      <c r="BD2" s="75"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,18 +1985,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="146"/>
+      <c r="BD3" s="82"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="68">
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="94">
         <v>30</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="96">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2047,18 +2047,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="71" t="s">
+      <c r="BB4" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="146"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="82"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="91"/>
       <c r="B5" s="92"/>
       <c r="C5" s="93"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="80"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="97"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2107,24 +2107,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="71"/>
-      <c r="BC5" s="72"/>
-      <c r="BD5" s="146"/>
-      <c r="BF5" s="136" t="s">
+      <c r="BB5" s="141"/>
+      <c r="BC5" s="142"/>
+      <c r="BD5" s="82"/>
+      <c r="BF5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="140"/>
+      <c r="BG5" s="69"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="64">
+      <c r="B6" s="99"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="85">
         <v>1</v>
       </c>
-      <c r="E6" s="117">
+      <c r="E6" s="104">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2175,18 +2175,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="71"/>
-      <c r="BC6" s="72"/>
-      <c r="BD6" s="146"/>
-      <c r="BF6" s="137"/>
-      <c r="BG6" s="141"/>
+      <c r="BB6" s="141"/>
+      <c r="BC6" s="142"/>
+      <c r="BD6" s="82"/>
+      <c r="BF6" s="66"/>
+      <c r="BG6" s="70"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="118"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="105"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2235,24 +2235,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="71"/>
-      <c r="BC7" s="72"/>
-      <c r="BD7" s="146"/>
-      <c r="BF7" s="136" t="s">
+      <c r="BB7" s="141"/>
+      <c r="BC7" s="142"/>
+      <c r="BD7" s="82"/>
+      <c r="BF7" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="142"/>
+      <c r="BG7" s="71"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="114" t="s">
+      <c r="A8" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="115"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="68">
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="94">
         <v>1.5</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="83">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
@@ -2303,20 +2303,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="71"/>
-      <c r="BC8" s="72"/>
-      <c r="BD8" s="70" t="s">
+      <c r="BB8" s="141"/>
+      <c r="BC8" s="142"/>
+      <c r="BD8" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="137"/>
-      <c r="BG8" s="143"/>
+      <c r="BF8" s="66"/>
+      <c r="BG8" s="72"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="91"/>
       <c r="B9" s="92"/>
       <c r="C9" s="93"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="117"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2365,24 +2365,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="71"/>
-      <c r="BC9" s="72"/>
-      <c r="BD9" s="70"/>
-      <c r="BF9" s="138" t="s">
+      <c r="BB9" s="141"/>
+      <c r="BC9" s="142"/>
+      <c r="BD9" s="75"/>
+      <c r="BF9" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="144"/>
+      <c r="BG9" s="73"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="64">
+      <c r="B10" s="99"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="85">
         <v>1.5</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="87">
         <v>1.5</v>
       </c>
       <c r="F10" s="19"/>
@@ -2433,18 +2433,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="71"/>
-      <c r="BC10" s="72"/>
-      <c r="BD10" s="70"/>
-      <c r="BF10" s="139"/>
-      <c r="BG10" s="145"/>
+      <c r="BB10" s="141"/>
+      <c r="BC10" s="142"/>
+      <c r="BD10" s="75"/>
+      <c r="BF10" s="68"/>
+      <c r="BG10" s="74"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="98"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="82"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="84"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2493,20 +2493,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="71"/>
-      <c r="BC11" s="72"/>
-      <c r="BD11" s="70"/>
+      <c r="BB11" s="141"/>
+      <c r="BC11" s="142"/>
+      <c r="BD11" s="75"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="115"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="68">
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="94">
         <v>1</v>
       </c>
-      <c r="E12" s="69">
+      <c r="E12" s="83">
         <v>1.5</v>
       </c>
       <c r="F12" s="19"/>
@@ -2557,9 +2557,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="71"/>
-      <c r="BC12" s="72"/>
-      <c r="BD12" s="70" t="s">
+      <c r="BB12" s="141"/>
+      <c r="BC12" s="142"/>
+      <c r="BD12" s="75" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2576,8 +2576,8 @@
       <c r="A13" s="91"/>
       <c r="B13" s="92"/>
       <c r="C13" s="93"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="67"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="117"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2626,9 +2626,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="71"/>
-      <c r="BC13" s="72"/>
-      <c r="BD13" s="70"/>
+      <c r="BB13" s="141"/>
+      <c r="BC13" s="142"/>
+      <c r="BD13" s="75"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2640,15 +2640,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="64">
+      <c r="B14" s="99"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="85">
         <v>2</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="87">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2699,16 +2699,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="71"/>
-      <c r="BC14" s="72"/>
-      <c r="BD14" s="70"/>
+      <c r="BB14" s="141"/>
+      <c r="BC14" s="142"/>
+      <c r="BD14" s="75"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="91"/>
       <c r="B15" s="92"/>
       <c r="C15" s="93"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="67"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="117"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2757,20 +2757,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="71"/>
-      <c r="BC15" s="72"/>
-      <c r="BD15" s="70"/>
+      <c r="BB15" s="141"/>
+      <c r="BC15" s="142"/>
+      <c r="BD15" s="75"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="64">
+      <c r="B16" s="99"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="85">
         <v>1</v>
       </c>
-      <c r="E16" s="66">
+      <c r="E16" s="87">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2821,16 +2821,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="71"/>
-      <c r="BC16" s="72"/>
-      <c r="BD16" s="70"/>
+      <c r="BB16" s="141"/>
+      <c r="BC16" s="142"/>
+      <c r="BD16" s="75"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="91"/>
       <c r="B17" s="92"/>
       <c r="C17" s="93"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="67"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="117"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2879,23 +2879,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="71"/>
-      <c r="BC17" s="72"/>
-      <c r="BD17" s="70"/>
+      <c r="BB17" s="141"/>
+      <c r="BC17" s="142"/>
+      <c r="BD17" s="75"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="64">
+      <c r="B18" s="99"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="85">
         <v>2</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="87">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2946,16 +2946,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="71"/>
-      <c r="BC18" s="72"/>
-      <c r="BD18" s="70"/>
+      <c r="BB18" s="141"/>
+      <c r="BC18" s="142"/>
+      <c r="BD18" s="75"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="91"/>
       <c r="B19" s="92"/>
       <c r="C19" s="93"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="67"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="117"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3004,20 +3004,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="71"/>
-      <c r="BC19" s="72"/>
-      <c r="BD19" s="70"/>
+      <c r="BB19" s="141"/>
+      <c r="BC19" s="142"/>
+      <c r="BD19" s="75"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="64">
+      <c r="B20" s="99"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="85">
         <v>1</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="87">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3068,16 +3068,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="71"/>
-      <c r="BC20" s="72"/>
-      <c r="BD20" s="70"/>
+      <c r="BB20" s="141"/>
+      <c r="BC20" s="142"/>
+      <c r="BD20" s="75"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="98"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="82"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="84"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3126,20 +3126,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="71"/>
-      <c r="BC21" s="72"/>
-      <c r="BD21" s="70"/>
+      <c r="BB21" s="141"/>
+      <c r="BC21" s="142"/>
+      <c r="BD21" s="75"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="115"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="68">
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="94">
         <v>0.5</v>
       </c>
-      <c r="E22" s="69">
+      <c r="E22" s="83">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3190,18 +3190,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="71"/>
-      <c r="BC22" s="72"/>
-      <c r="BD22" s="70" t="s">
+      <c r="BB22" s="141"/>
+      <c r="BC22" s="142"/>
+      <c r="BD22" s="75" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="98"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="82"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="84"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3250,20 +3250,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="71"/>
-      <c r="BC23" s="72"/>
-      <c r="BD23" s="70"/>
+      <c r="BB23" s="141"/>
+      <c r="BC23" s="142"/>
+      <c r="BD23" s="75"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="114" t="s">
+      <c r="A24" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="115"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="68">
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="94">
         <v>2</v>
       </c>
-      <c r="E24" s="69">
+      <c r="E24" s="83">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3314,9 +3314,9 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="71"/>
-      <c r="BC24" s="72"/>
-      <c r="BD24" s="75" t="s">
+      <c r="BB24" s="141"/>
+      <c r="BC24" s="142"/>
+      <c r="BD24" s="145" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3324,8 +3324,8 @@
       <c r="A25" s="91"/>
       <c r="B25" s="92"/>
       <c r="C25" s="93"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="67"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="117"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3374,20 +3374,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="71"/>
-      <c r="BC25" s="72"/>
-      <c r="BD25" s="76"/>
+      <c r="BB25" s="141"/>
+      <c r="BC25" s="142"/>
+      <c r="BD25" s="146"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="64">
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="85">
         <v>1</v>
       </c>
-      <c r="E26" s="66">
+      <c r="E26" s="87">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3438,16 +3438,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="71"/>
-      <c r="BC26" s="72"/>
-      <c r="BD26" s="76"/>
+      <c r="BB26" s="141"/>
+      <c r="BC26" s="142"/>
+      <c r="BD26" s="146"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="91"/>
       <c r="B27" s="92"/>
       <c r="C27" s="93"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="67"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="117"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3496,20 +3496,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="71"/>
-      <c r="BC27" s="72"/>
-      <c r="BD27" s="76"/>
+      <c r="BB27" s="141"/>
+      <c r="BC27" s="142"/>
+      <c r="BD27" s="146"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="88" t="s">
+      <c r="A28" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="64">
+      <c r="B28" s="99"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="85">
         <v>2</v>
       </c>
-      <c r="E28" s="66">
+      <c r="E28" s="87">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3560,16 +3560,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="71"/>
-      <c r="BC28" s="72"/>
-      <c r="BD28" s="76"/>
+      <c r="BB28" s="141"/>
+      <c r="BC28" s="142"/>
+      <c r="BD28" s="146"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="91"/>
       <c r="B29" s="92"/>
       <c r="C29" s="93"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="67"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="117"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3618,20 +3618,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="71"/>
-      <c r="BC29" s="72"/>
-      <c r="BD29" s="76"/>
+      <c r="BB29" s="141"/>
+      <c r="BC29" s="142"/>
+      <c r="BD29" s="146"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="64">
+      <c r="B30" s="99"/>
+      <c r="C30" s="100"/>
+      <c r="D30" s="85">
         <v>2</v>
       </c>
-      <c r="E30" s="66">
+      <c r="E30" s="87">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3682,16 +3682,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="71"/>
-      <c r="BC30" s="72"/>
-      <c r="BD30" s="76"/>
+      <c r="BB30" s="141"/>
+      <c r="BC30" s="142"/>
+      <c r="BD30" s="146"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="91"/>
       <c r="B31" s="92"/>
       <c r="C31" s="93"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="67"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="117"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3740,20 +3740,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="71"/>
-      <c r="BC31" s="72"/>
-      <c r="BD31" s="76"/>
+      <c r="BB31" s="141"/>
+      <c r="BC31" s="142"/>
+      <c r="BD31" s="146"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="64">
+      <c r="B32" s="99"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="85">
         <v>4</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="87">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3804,16 +3804,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="71"/>
-      <c r="BC32" s="72"/>
-      <c r="BD32" s="76"/>
+      <c r="BB32" s="141"/>
+      <c r="BC32" s="142"/>
+      <c r="BD32" s="146"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="91"/>
       <c r="B33" s="92"/>
       <c r="C33" s="93"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="67"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="117"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3862,20 +3862,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="71"/>
-      <c r="BC33" s="72"/>
-      <c r="BD33" s="76"/>
+      <c r="BB33" s="141"/>
+      <c r="BC33" s="142"/>
+      <c r="BD33" s="146"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="108" t="s">
+      <c r="A34" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="109"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="64">
+      <c r="B34" s="136"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="85">
         <v>3</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="87">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3926,16 +3926,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="71"/>
-      <c r="BC34" s="72"/>
-      <c r="BD34" s="76"/>
+      <c r="BB34" s="141"/>
+      <c r="BC34" s="142"/>
+      <c r="BD34" s="146"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
-      <c r="B35" s="112"/>
-      <c r="C35" s="113"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="67"/>
+      <c r="A35" s="138"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="140"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="117"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3952,7 +3952,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="32"/>
       <c r="U35" s="36"/>
-      <c r="V35" s="147"/>
+      <c r="V35" s="64"/>
       <c r="W35" s="9"/>
       <c r="X35" s="9"/>
       <c r="Y35" s="4"/>
@@ -3984,20 +3984,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="71"/>
-      <c r="BC35" s="72"/>
-      <c r="BD35" s="76"/>
+      <c r="BB35" s="141"/>
+      <c r="BC35" s="142"/>
+      <c r="BD35" s="146"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="108" t="s">
+      <c r="A36" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="109"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="64">
+      <c r="B36" s="136"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="85">
         <v>4</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="87">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4047,16 +4047,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="71"/>
-      <c r="BC36" s="72"/>
-      <c r="BD36" s="76"/>
+      <c r="BB36" s="141"/>
+      <c r="BC36" s="142"/>
+      <c r="BD36" s="146"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="111"/>
-      <c r="B37" s="112"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="67"/>
+      <c r="A37" s="138"/>
+      <c r="B37" s="139"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="117"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4105,20 +4105,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="71"/>
-      <c r="BC37" s="72"/>
-      <c r="BD37" s="76"/>
+      <c r="BB37" s="141"/>
+      <c r="BC37" s="142"/>
+      <c r="BD37" s="146"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="108" t="s">
+      <c r="A38" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="109"/>
-      <c r="C38" s="110"/>
-      <c r="D38" s="64">
+      <c r="B38" s="136"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="85">
         <v>1</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="87">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4167,16 +4167,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="71"/>
-      <c r="BC38" s="72"/>
-      <c r="BD38" s="76"/>
+      <c r="BB38" s="141"/>
+      <c r="BC38" s="142"/>
+      <c r="BD38" s="146"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
-      <c r="B39" s="112"/>
-      <c r="C39" s="113"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="67"/>
+      <c r="A39" s="138"/>
+      <c r="B39" s="139"/>
+      <c r="C39" s="140"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="117"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4225,20 +4225,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="71"/>
-      <c r="BC39" s="72"/>
-      <c r="BD39" s="76"/>
+      <c r="BB39" s="141"/>
+      <c r="BC39" s="142"/>
+      <c r="BD39" s="146"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="108" t="s">
+      <c r="A40" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="109"/>
-      <c r="C40" s="110"/>
-      <c r="D40" s="64">
+      <c r="B40" s="136"/>
+      <c r="C40" s="137"/>
+      <c r="D40" s="85">
         <v>1</v>
       </c>
-      <c r="E40" s="66">
+      <c r="E40" s="87">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4290,16 +4290,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="71"/>
-      <c r="BC40" s="72"/>
-      <c r="BD40" s="76"/>
+      <c r="BB40" s="141"/>
+      <c r="BC40" s="142"/>
+      <c r="BD40" s="146"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
-      <c r="B41" s="112"/>
-      <c r="C41" s="113"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="67"/>
+      <c r="A41" s="138"/>
+      <c r="B41" s="139"/>
+      <c r="C41" s="140"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="117"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4348,20 +4348,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="71"/>
-      <c r="BC41" s="72"/>
-      <c r="BD41" s="76"/>
+      <c r="BB41" s="141"/>
+      <c r="BC41" s="142"/>
+      <c r="BD41" s="146"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="89"/>
-      <c r="C42" s="90"/>
-      <c r="D42" s="64">
+      <c r="B42" s="99"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="85">
         <v>2</v>
       </c>
-      <c r="E42" s="66">
+      <c r="E42" s="87">
         <v>2.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -4412,16 +4412,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="71"/>
-      <c r="BC42" s="72"/>
-      <c r="BD42" s="76"/>
+      <c r="BB42" s="141"/>
+      <c r="BC42" s="142"/>
+      <c r="BD42" s="146"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="91"/>
       <c r="B43" s="92"/>
       <c r="C43" s="93"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="67"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="117"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4470,20 +4470,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="71"/>
-      <c r="BC43" s="72"/>
-      <c r="BD43" s="76"/>
+      <c r="BB43" s="141"/>
+      <c r="BC43" s="142"/>
+      <c r="BD43" s="146"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="89"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="64">
+      <c r="B44" s="99"/>
+      <c r="C44" s="100"/>
+      <c r="D44" s="85">
         <v>2</v>
       </c>
-      <c r="E44" s="66">
+      <c r="E44" s="87">
         <v>2</v>
       </c>
       <c r="F44" s="8"/>
@@ -4534,16 +4534,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="71"/>
-      <c r="BC44" s="72"/>
-      <c r="BD44" s="76"/>
+      <c r="BB44" s="141"/>
+      <c r="BC44" s="142"/>
+      <c r="BD44" s="146"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="98"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="100"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="82"/>
+      <c r="A45" s="101"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="84"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4592,20 +4592,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="71"/>
-      <c r="BC45" s="72"/>
-      <c r="BD45" s="77"/>
+      <c r="BB45" s="141"/>
+      <c r="BC45" s="142"/>
+      <c r="BD45" s="147"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="101" t="s">
+      <c r="A46" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="102"/>
-      <c r="C46" s="103"/>
-      <c r="D46" s="78">
+      <c r="B46" s="129"/>
+      <c r="C46" s="130"/>
+      <c r="D46" s="122">
         <v>1</v>
       </c>
-      <c r="E46" s="79">
+      <c r="E46" s="96">
         <v>1.5</v>
       </c>
       <c r="F46" s="50"/>
@@ -4655,9 +4655,9 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="71"/>
-      <c r="BC46" s="72"/>
-      <c r="BD46" s="70" t="s">
+      <c r="BB46" s="141"/>
+      <c r="BC46" s="142"/>
+      <c r="BD46" s="75" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4665,8 +4665,8 @@
       <c r="A47" s="91"/>
       <c r="B47" s="92"/>
       <c r="C47" s="93"/>
-      <c r="D47" s="65"/>
-      <c r="E47" s="80"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="97"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4715,21 +4715,21 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="71"/>
-      <c r="BC47" s="72"/>
-      <c r="BD47" s="70"/>
+      <c r="BB47" s="141"/>
+      <c r="BC47" s="142"/>
+      <c r="BD47" s="75"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="88" t="s">
+      <c r="A48" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="89"/>
-      <c r="C48" s="90"/>
-      <c r="D48" s="64">
+      <c r="B48" s="99"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="85">
         <v>2</v>
       </c>
-      <c r="E48" s="66">
-        <v>3</v>
+      <c r="E48" s="87">
+        <v>3.5</v>
       </c>
       <c r="F48" s="50"/>
       <c r="G48" s="23"/>
@@ -4779,16 +4779,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="71"/>
-      <c r="BC48" s="72"/>
-      <c r="BD48" s="70"/>
+      <c r="BB48" s="141"/>
+      <c r="BC48" s="142"/>
+      <c r="BD48" s="75"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="98"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="82"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="103"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="84"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4837,21 +4837,21 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="71"/>
-      <c r="BC49" s="72"/>
-      <c r="BD49" s="70"/>
+      <c r="BB49" s="141"/>
+      <c r="BC49" s="142"/>
+      <c r="BD49" s="75"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="94" t="s">
+      <c r="A50" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="95"/>
-      <c r="C50" s="95"/>
-      <c r="D50" s="78">
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
+      <c r="D50" s="122">
         <v>5</v>
       </c>
-      <c r="E50" s="83">
-        <v>5</v>
+      <c r="E50" s="123">
+        <v>4.5</v>
       </c>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
@@ -4901,18 +4901,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="71"/>
-      <c r="BC50" s="72"/>
-      <c r="BD50" s="70" t="s">
+      <c r="BB50" s="141"/>
+      <c r="BC50" s="142"/>
+      <c r="BD50" s="75" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="96"/>
-      <c r="B51" s="97"/>
-      <c r="C51" s="97"/>
-      <c r="D51" s="65"/>
-      <c r="E51" s="67"/>
+      <c r="A51" s="126"/>
+      <c r="B51" s="127"/>
+      <c r="C51" s="127"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="117"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4931,17 +4931,17 @@
       <c r="U51" s="8"/>
       <c r="V51" s="9"/>
       <c r="W51" s="48"/>
-      <c r="X51" s="42"/>
+      <c r="X51" s="30"/>
       <c r="Y51" s="21"/>
       <c r="Z51" s="8"/>
       <c r="AA51" s="9"/>
       <c r="AB51" s="48"/>
-      <c r="AC51" s="42"/>
+      <c r="AC51" s="30"/>
       <c r="AD51" s="21"/>
       <c r="AE51" s="8"/>
       <c r="AF51" s="9"/>
       <c r="AG51" s="48"/>
-      <c r="AH51" s="42"/>
+      <c r="AH51" s="30"/>
       <c r="AI51" s="21"/>
       <c r="AJ51" s="8"/>
       <c r="AK51" s="9"/>
@@ -4961,20 +4961,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="71"/>
-      <c r="BC51" s="72"/>
-      <c r="BD51" s="70"/>
+      <c r="BB51" s="141"/>
+      <c r="BC51" s="142"/>
+      <c r="BD51" s="75"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="88" t="s">
+      <c r="A52" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="64">
+      <c r="B52" s="99"/>
+      <c r="C52" s="100"/>
+      <c r="D52" s="85">
         <v>2</v>
       </c>
-      <c r="E52" s="66"/>
+      <c r="E52" s="87"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5015,16 +5015,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="44"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="71"/>
-      <c r="BC52" s="72"/>
-      <c r="BD52" s="70"/>
+      <c r="BB52" s="141"/>
+      <c r="BC52" s="142"/>
+      <c r="BD52" s="75"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="98"/>
-      <c r="B53" s="99"/>
-      <c r="C53" s="100"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="82"/>
+      <c r="A53" s="101"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="84"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5073,20 +5073,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="71"/>
-      <c r="BC53" s="72"/>
-      <c r="BD53" s="70"/>
+      <c r="BB53" s="141"/>
+      <c r="BC53" s="142"/>
+      <c r="BD53" s="75"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="101" t="s">
+      <c r="A54" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="102"/>
-      <c r="C54" s="103"/>
-      <c r="D54" s="78">
+      <c r="B54" s="129"/>
+      <c r="C54" s="130"/>
+      <c r="D54" s="122">
         <v>4.5</v>
       </c>
-      <c r="E54" s="83">
+      <c r="E54" s="123">
         <v>2</v>
       </c>
       <c r="F54" s="50"/>
@@ -5136,16 +5136,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="71"/>
-      <c r="BC54" s="72"/>
+      <c r="BB54" s="141"/>
+      <c r="BC54" s="142"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="91"/>
       <c r="B55" s="92"/>
       <c r="C55" s="93"/>
-      <c r="D55" s="65"/>
-      <c r="E55" s="67"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="117"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5194,16 +5194,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="71"/>
-      <c r="BC55" s="72"/>
+      <c r="BB55" s="141"/>
+      <c r="BC55" s="142"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="101"/>
-      <c r="B56" s="102"/>
-      <c r="C56" s="103"/>
-      <c r="D56" s="78"/>
-      <c r="E56" s="83"/>
+      <c r="A56" s="128"/>
+      <c r="B56" s="129"/>
+      <c r="C56" s="130"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="123"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5252,16 +5252,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="71"/>
-      <c r="BC56" s="72"/>
+      <c r="BB56" s="141"/>
+      <c r="BC56" s="142"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="91"/>
       <c r="B57" s="92"/>
       <c r="C57" s="93"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="67"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="117"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5310,16 +5310,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="71"/>
-      <c r="BC57" s="72"/>
+      <c r="BB57" s="141"/>
+      <c r="BC57" s="142"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="88"/>
-      <c r="B58" s="89"/>
-      <c r="C58" s="90"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="66"/>
+      <c r="A58" s="98"/>
+      <c r="B58" s="99"/>
+      <c r="C58" s="100"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="87"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5368,16 +5368,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="71"/>
-      <c r="BC58" s="72"/>
+      <c r="BB58" s="141"/>
+      <c r="BC58" s="142"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="98"/>
-      <c r="B59" s="99"/>
-      <c r="C59" s="100"/>
-      <c r="D59" s="81"/>
-      <c r="E59" s="82"/>
+      <c r="A59" s="101"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="103"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="84"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5426,74 +5426,96 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="73"/>
-      <c r="BC59" s="74"/>
+      <c r="BB59" s="143"/>
+      <c r="BC59" s="144"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="104" t="s">
+      <c r="A60" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="105"/>
-      <c r="C60" s="105"/>
-      <c r="D60" s="84">
+      <c r="B60" s="132"/>
+      <c r="C60" s="132"/>
+      <c r="D60" s="118">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="86">
+      <c r="E60" s="120">
         <f>SUM(E4:E59)</f>
         <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="106"/>
-      <c r="B61" s="107"/>
-      <c r="C61" s="107"/>
-      <c r="D61" s="85"/>
-      <c r="E61" s="87"/>
+      <c r="A61" s="133"/>
+      <c r="B61" s="134"/>
+      <c r="C61" s="134"/>
+      <c r="D61" s="119"/>
+      <c r="E61" s="121"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BD3:BD7"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="BD8:BD11"/>
+    <mergeCell ref="BD12:BD21"/>
+    <mergeCell ref="BD22:BD23"/>
+    <mergeCell ref="BB4:BC59"/>
+    <mergeCell ref="BD50:BD53"/>
+    <mergeCell ref="BD46:BD49"/>
+    <mergeCell ref="BD24:BD45"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
     <mergeCell ref="A20:C21"/>
     <mergeCell ref="A22:C23"/>
     <mergeCell ref="A24:C25"/>
@@ -5518,67 +5540,45 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="BD8:BD11"/>
-    <mergeCell ref="BD12:BD21"/>
-    <mergeCell ref="BD22:BD23"/>
-    <mergeCell ref="BB4:BC59"/>
-    <mergeCell ref="BD50:BD53"/>
-    <mergeCell ref="BD46:BD49"/>
-    <mergeCell ref="BD24:BD45"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BD3:BD7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
DOku und Excel angepasst
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="692" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4530C779-012A-41CF-866D-1AFB4CB3BDB6}"/>
+  <xr:revisionPtr revIDLastSave="700" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDE3586C-046C-4C52-8C35-92661D3D4C36}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1079,6 +1079,222 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1110,223 +1326,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1651,8 +1651,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AJ44" sqref="AJ44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,171 +1664,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="109" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="110"/>
-      <c r="F1" s="111" t="s">
+      <c r="E1" s="127"/>
+      <c r="F1" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="76" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="76" t="s">
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="76" t="s">
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="136"/>
+      <c r="U1" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="V1" s="135"/>
+      <c r="W1" s="135"/>
+      <c r="X1" s="135"/>
+      <c r="Y1" s="136"/>
+      <c r="Z1" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="76" t="s">
+      <c r="AA1" s="135"/>
+      <c r="AB1" s="135"/>
+      <c r="AC1" s="135"/>
+      <c r="AD1" s="136"/>
+      <c r="AE1" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="76" t="s">
+      <c r="AF1" s="135"/>
+      <c r="AG1" s="135"/>
+      <c r="AH1" s="135"/>
+      <c r="AI1" s="136"/>
+      <c r="AJ1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="76" t="s">
+      <c r="AK1" s="135"/>
+      <c r="AL1" s="135"/>
+      <c r="AM1" s="135"/>
+      <c r="AN1" s="136"/>
+      <c r="AO1" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="76" t="s">
+      <c r="AP1" s="135"/>
+      <c r="AQ1" s="135"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
+      <c r="AT1" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="78"/>
-      <c r="AY1" s="76" t="s">
+      <c r="AU1" s="135"/>
+      <c r="AV1" s="135"/>
+      <c r="AW1" s="135"/>
+      <c r="AX1" s="136"/>
+      <c r="AY1" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="77"/>
-      <c r="BB1" s="77"/>
-      <c r="BC1" s="78"/>
-      <c r="BD1" s="75" t="s">
+      <c r="AZ1" s="135"/>
+      <c r="BA1" s="135"/>
+      <c r="BB1" s="135"/>
+      <c r="BC1" s="136"/>
+      <c r="BD1" s="71" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="114">
+      <c r="A2" s="124"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="131">
         <v>44957</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="79">
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="120">
         <v>44958</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="79">
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="120">
         <v>44959</v>
       </c>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="79">
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="120">
         <v>44960</v>
       </c>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="79">
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="120">
         <v>44964</v>
       </c>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="80"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="79">
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="122"/>
+      <c r="AE2" s="120">
         <v>44965</v>
       </c>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
-      <c r="AH2" s="80"/>
-      <c r="AI2" s="81"/>
-      <c r="AJ2" s="79">
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="121"/>
+      <c r="AH2" s="121"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="120">
         <v>44966</v>
       </c>
-      <c r="AK2" s="80"/>
-      <c r="AL2" s="80"/>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="81"/>
-      <c r="AO2" s="79">
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121"/>
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="120">
         <v>44967</v>
       </c>
-      <c r="AP2" s="80"/>
-      <c r="AQ2" s="80"/>
-      <c r="AR2" s="80"/>
-      <c r="AS2" s="81"/>
-      <c r="AT2" s="79">
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="120">
         <v>44971</v>
       </c>
-      <c r="AU2" s="80"/>
-      <c r="AV2" s="80"/>
-      <c r="AW2" s="80"/>
-      <c r="AX2" s="81"/>
-      <c r="AY2" s="79">
+      <c r="AU2" s="121"/>
+      <c r="AV2" s="121"/>
+      <c r="AW2" s="121"/>
+      <c r="AX2" s="122"/>
+      <c r="AY2" s="120">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="80"/>
-      <c r="BA2" s="80"/>
-      <c r="BB2" s="80"/>
-      <c r="BC2" s="81"/>
-      <c r="BD2" s="75"/>
+      <c r="AZ2" s="121"/>
+      <c r="BA2" s="121"/>
+      <c r="BB2" s="121"/>
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="71"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,18 +1985,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="82"/>
+      <c r="BD3" s="147"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="94">
+      <c r="B4" s="116"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="69">
         <v>30</v>
       </c>
-      <c r="E4" s="96">
+      <c r="E4" s="80">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2047,18 +2047,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="141" t="s">
+      <c r="BB4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="142"/>
-      <c r="BD4" s="82"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="147"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="97"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2089,10 +2089,10 @@
       <c r="AG5" s="30"/>
       <c r="AH5" s="30"/>
       <c r="AI5" s="4"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="30"/>
+      <c r="AL5" s="30"/>
+      <c r="AM5" s="30"/>
       <c r="AN5" s="4"/>
       <c r="AO5" s="8"/>
       <c r="AP5" s="9"/>
@@ -2107,24 +2107,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="141"/>
-      <c r="BC5" s="142"/>
-      <c r="BD5" s="82"/>
-      <c r="BF5" s="65" t="s">
+      <c r="BB5" s="72"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="147"/>
+      <c r="BF5" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="69"/>
+      <c r="BG5" s="141"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="98" t="s">
+      <c r="A6" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="99"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="85">
+      <c r="B6" s="90"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="65">
         <v>1</v>
       </c>
-      <c r="E6" s="104">
+      <c r="E6" s="118">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2157,7 +2157,7 @@
       <c r="AG6" s="9"/>
       <c r="AH6" s="9"/>
       <c r="AI6" s="4"/>
-      <c r="AJ6" s="8"/>
+      <c r="AJ6" s="20"/>
       <c r="AK6" s="9"/>
       <c r="AL6" s="9"/>
       <c r="AM6" s="9"/>
@@ -2175,18 +2175,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="141"/>
-      <c r="BC6" s="142"/>
-      <c r="BD6" s="82"/>
-      <c r="BF6" s="66"/>
-      <c r="BG6" s="70"/>
+      <c r="BB6" s="72"/>
+      <c r="BC6" s="73"/>
+      <c r="BD6" s="147"/>
+      <c r="BF6" s="138"/>
+      <c r="BG6" s="142"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="105"/>
+      <c r="A7" s="99"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="119"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2235,24 +2235,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="141"/>
-      <c r="BC7" s="142"/>
-      <c r="BD7" s="82"/>
-      <c r="BF7" s="65" t="s">
+      <c r="BB7" s="72"/>
+      <c r="BC7" s="73"/>
+      <c r="BD7" s="147"/>
+      <c r="BF7" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="71"/>
+      <c r="BG7" s="143"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="94">
+      <c r="B8" s="116"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="69">
         <v>1.5</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="70">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
@@ -2303,20 +2303,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="141"/>
-      <c r="BC8" s="142"/>
-      <c r="BD8" s="75" t="s">
+      <c r="BB8" s="72"/>
+      <c r="BC8" s="73"/>
+      <c r="BD8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="66"/>
-      <c r="BG8" s="72"/>
+      <c r="BF8" s="138"/>
+      <c r="BG8" s="144"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="91"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="117"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2347,7 +2347,7 @@
       <c r="AG9" s="9"/>
       <c r="AH9" s="9"/>
       <c r="AI9" s="4"/>
-      <c r="AJ9" s="8"/>
+      <c r="AJ9" s="36"/>
       <c r="AK9" s="9"/>
       <c r="AL9" s="9"/>
       <c r="AM9" s="9"/>
@@ -2365,24 +2365,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="141"/>
-      <c r="BC9" s="142"/>
-      <c r="BD9" s="75"/>
-      <c r="BF9" s="67" t="s">
+      <c r="BB9" s="72"/>
+      <c r="BC9" s="73"/>
+      <c r="BD9" s="71"/>
+      <c r="BF9" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="73"/>
+      <c r="BG9" s="145"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="85">
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="65">
         <v>1.5</v>
       </c>
-      <c r="E10" s="87">
+      <c r="E10" s="67">
         <v>1.5</v>
       </c>
       <c r="F10" s="19"/>
@@ -2433,18 +2433,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="141"/>
-      <c r="BC10" s="142"/>
-      <c r="BD10" s="75"/>
-      <c r="BF10" s="68"/>
-      <c r="BG10" s="74"/>
+      <c r="BB10" s="72"/>
+      <c r="BC10" s="73"/>
+      <c r="BD10" s="71"/>
+      <c r="BF10" s="140"/>
+      <c r="BG10" s="146"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="84"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="83"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2475,7 +2475,7 @@
       <c r="AG11" s="11"/>
       <c r="AH11" s="11"/>
       <c r="AI11" s="12"/>
-      <c r="AJ11" s="10"/>
+      <c r="AJ11" s="36"/>
       <c r="AK11" s="11"/>
       <c r="AL11" s="11"/>
       <c r="AM11" s="11"/>
@@ -2493,20 +2493,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="141"/>
-      <c r="BC11" s="142"/>
-      <c r="BD11" s="75"/>
+      <c r="BB11" s="72"/>
+      <c r="BC11" s="73"/>
+      <c r="BD11" s="71"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="94">
+      <c r="B12" s="116"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="69">
         <v>1</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="70">
         <v>1.5</v>
       </c>
       <c r="F12" s="19"/>
@@ -2557,9 +2557,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="141"/>
-      <c r="BC12" s="142"/>
-      <c r="BD12" s="75" t="s">
+      <c r="BB12" s="72"/>
+      <c r="BC12" s="73"/>
+      <c r="BD12" s="71" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2573,11 +2573,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="91"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="117"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2626,9 +2626,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="141"/>
-      <c r="BC13" s="142"/>
-      <c r="BD13" s="75"/>
+      <c r="BB13" s="72"/>
+      <c r="BC13" s="73"/>
+      <c r="BD13" s="71"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2640,15 +2640,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="98" t="s">
+      <c r="A14" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="85">
+      <c r="B14" s="90"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="65">
         <v>2</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="67">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2699,16 +2699,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="141"/>
-      <c r="BC14" s="142"/>
-      <c r="BD14" s="75"/>
+      <c r="BB14" s="72"/>
+      <c r="BC14" s="73"/>
+      <c r="BD14" s="71"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="91"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="117"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="68"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2757,20 +2757,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="141"/>
-      <c r="BC15" s="142"/>
-      <c r="BD15" s="75"/>
+      <c r="BB15" s="72"/>
+      <c r="BC15" s="73"/>
+      <c r="BD15" s="71"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="85">
+      <c r="B16" s="90"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="65">
         <v>1</v>
       </c>
-      <c r="E16" s="87">
+      <c r="E16" s="67">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2821,16 +2821,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="141"/>
-      <c r="BC16" s="142"/>
-      <c r="BD16" s="75"/>
+      <c r="BB16" s="72"/>
+      <c r="BC16" s="73"/>
+      <c r="BD16" s="71"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="117"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="68"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2879,23 +2879,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="141"/>
-      <c r="BC17" s="142"/>
-      <c r="BD17" s="75"/>
+      <c r="BB17" s="72"/>
+      <c r="BC17" s="73"/>
+      <c r="BD17" s="71"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="99"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="85">
+      <c r="B18" s="90"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="65">
         <v>2</v>
       </c>
-      <c r="E18" s="87">
+      <c r="E18" s="67">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2946,16 +2946,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="141"/>
-      <c r="BC18" s="142"/>
-      <c r="BD18" s="75"/>
+      <c r="BB18" s="72"/>
+      <c r="BC18" s="73"/>
+      <c r="BD18" s="71"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="91"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="117"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="68"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3004,20 +3004,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="141"/>
-      <c r="BC19" s="142"/>
-      <c r="BD19" s="75"/>
+      <c r="BB19" s="72"/>
+      <c r="BC19" s="73"/>
+      <c r="BD19" s="71"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="99"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="85">
+      <c r="B20" s="90"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="65">
         <v>1</v>
       </c>
-      <c r="E20" s="87">
+      <c r="E20" s="67">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3068,16 +3068,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="141"/>
-      <c r="BC20" s="142"/>
-      <c r="BD20" s="75"/>
+      <c r="BB20" s="72"/>
+      <c r="BC20" s="73"/>
+      <c r="BD20" s="71"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="101"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="84"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3126,20 +3126,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="141"/>
-      <c r="BC21" s="142"/>
-      <c r="BD21" s="75"/>
+      <c r="BB21" s="72"/>
+      <c r="BC21" s="73"/>
+      <c r="BD21" s="71"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="88" t="s">
+      <c r="A22" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="94">
+      <c r="B22" s="116"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="69">
         <v>0.5</v>
       </c>
-      <c r="E22" s="83">
+      <c r="E22" s="70">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3190,18 +3190,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="141"/>
-      <c r="BC22" s="142"/>
-      <c r="BD22" s="75" t="s">
+      <c r="BB22" s="72"/>
+      <c r="BC22" s="73"/>
+      <c r="BD22" s="71" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="101"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="84"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="83"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3250,20 +3250,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="141"/>
-      <c r="BC23" s="142"/>
-      <c r="BD23" s="75"/>
+      <c r="BB23" s="72"/>
+      <c r="BC23" s="73"/>
+      <c r="BD23" s="71"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="94">
+      <c r="B24" s="116"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="69">
         <v>2</v>
       </c>
-      <c r="E24" s="83">
+      <c r="E24" s="70">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3314,18 +3314,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="141"/>
-      <c r="BC24" s="142"/>
-      <c r="BD24" s="145" t="s">
+      <c r="BB24" s="72"/>
+      <c r="BC24" s="73"/>
+      <c r="BD24" s="76" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="91"/>
-      <c r="B25" s="92"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="117"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="68"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3374,20 +3374,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="141"/>
-      <c r="BC25" s="142"/>
-      <c r="BD25" s="146"/>
+      <c r="BB25" s="72"/>
+      <c r="BC25" s="73"/>
+      <c r="BD25" s="77"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="85">
+      <c r="B26" s="90"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="67">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3438,16 +3438,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="141"/>
-      <c r="BC26" s="142"/>
-      <c r="BD26" s="146"/>
+      <c r="BB26" s="72"/>
+      <c r="BC26" s="73"/>
+      <c r="BD26" s="77"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="91"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="117"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="68"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3496,20 +3496,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="141"/>
-      <c r="BC27" s="142"/>
-      <c r="BD27" s="146"/>
+      <c r="BB27" s="72"/>
+      <c r="BC27" s="73"/>
+      <c r="BD27" s="77"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="99"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="85">
+      <c r="B28" s="90"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="65">
         <v>2</v>
       </c>
-      <c r="E28" s="87">
+      <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3560,16 +3560,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="141"/>
-      <c r="BC28" s="142"/>
-      <c r="BD28" s="146"/>
+      <c r="BB28" s="72"/>
+      <c r="BC28" s="73"/>
+      <c r="BD28" s="77"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="91"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="117"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="93"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="68"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3618,20 +3618,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="141"/>
-      <c r="BC29" s="142"/>
-      <c r="BD29" s="146"/>
+      <c r="BB29" s="72"/>
+      <c r="BC29" s="73"/>
+      <c r="BD29" s="77"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="99"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="85">
+      <c r="B30" s="90"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="65">
         <v>2</v>
       </c>
-      <c r="E30" s="87">
+      <c r="E30" s="67">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3682,16 +3682,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="141"/>
-      <c r="BC30" s="142"/>
-      <c r="BD30" s="146"/>
+      <c r="BB30" s="72"/>
+      <c r="BC30" s="73"/>
+      <c r="BD30" s="77"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="117"/>
+      <c r="A31" s="92"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="68"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3740,20 +3740,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="141"/>
-      <c r="BC31" s="142"/>
-      <c r="BD31" s="146"/>
+      <c r="BB31" s="72"/>
+      <c r="BC31" s="73"/>
+      <c r="BD31" s="77"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="98" t="s">
+      <c r="A32" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="99"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="85">
+      <c r="B32" s="90"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="65">
         <v>4</v>
       </c>
-      <c r="E32" s="87">
+      <c r="E32" s="67">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3804,16 +3804,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="141"/>
-      <c r="BC32" s="142"/>
-      <c r="BD32" s="146"/>
+      <c r="BB32" s="72"/>
+      <c r="BC32" s="73"/>
+      <c r="BD32" s="77"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="91"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="117"/>
+      <c r="A33" s="92"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3862,20 +3862,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="141"/>
-      <c r="BC33" s="142"/>
-      <c r="BD33" s="146"/>
+      <c r="BB33" s="72"/>
+      <c r="BC33" s="73"/>
+      <c r="BD33" s="77"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135" t="s">
+      <c r="A34" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="136"/>
-      <c r="C34" s="137"/>
-      <c r="D34" s="85">
+      <c r="B34" s="110"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="65">
         <v>3</v>
       </c>
-      <c r="E34" s="87">
+      <c r="E34" s="67">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3926,16 +3926,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="141"/>
-      <c r="BC34" s="142"/>
-      <c r="BD34" s="146"/>
+      <c r="BB34" s="72"/>
+      <c r="BC34" s="73"/>
+      <c r="BD34" s="77"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="138"/>
-      <c r="B35" s="139"/>
-      <c r="C35" s="140"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="117"/>
+      <c r="A35" s="112"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="68"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3984,20 +3984,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="141"/>
-      <c r="BC35" s="142"/>
-      <c r="BD35" s="146"/>
+      <c r="BB35" s="72"/>
+      <c r="BC35" s="73"/>
+      <c r="BD35" s="77"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="135" t="s">
+      <c r="A36" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="136"/>
-      <c r="C36" s="137"/>
-      <c r="D36" s="85">
+      <c r="B36" s="110"/>
+      <c r="C36" s="111"/>
+      <c r="D36" s="65">
         <v>4</v>
       </c>
-      <c r="E36" s="87">
+      <c r="E36" s="67">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4047,16 +4047,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="141"/>
-      <c r="BC36" s="142"/>
-      <c r="BD36" s="146"/>
+      <c r="BB36" s="72"/>
+      <c r="BC36" s="73"/>
+      <c r="BD36" s="77"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="138"/>
-      <c r="B37" s="139"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="117"/>
+      <c r="A37" s="112"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="114"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="68"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4105,20 +4105,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="141"/>
-      <c r="BC37" s="142"/>
-      <c r="BD37" s="146"/>
+      <c r="BB37" s="72"/>
+      <c r="BC37" s="73"/>
+      <c r="BD37" s="77"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="135" t="s">
+      <c r="A38" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="136"/>
-      <c r="C38" s="137"/>
-      <c r="D38" s="85">
+      <c r="B38" s="110"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="65">
         <v>1</v>
       </c>
-      <c r="E38" s="87">
+      <c r="E38" s="67">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4167,16 +4167,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="141"/>
-      <c r="BC38" s="142"/>
-      <c r="BD38" s="146"/>
+      <c r="BB38" s="72"/>
+      <c r="BC38" s="73"/>
+      <c r="BD38" s="77"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="138"/>
-      <c r="B39" s="139"/>
-      <c r="C39" s="140"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="117"/>
+      <c r="A39" s="112"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4225,20 +4225,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="141"/>
-      <c r="BC39" s="142"/>
-      <c r="BD39" s="146"/>
+      <c r="BB39" s="72"/>
+      <c r="BC39" s="73"/>
+      <c r="BD39" s="77"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="135" t="s">
+      <c r="A40" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="136"/>
-      <c r="C40" s="137"/>
-      <c r="D40" s="85">
+      <c r="B40" s="110"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="65">
         <v>1</v>
       </c>
-      <c r="E40" s="87">
+      <c r="E40" s="67">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4290,16 +4290,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="141"/>
-      <c r="BC40" s="142"/>
-      <c r="BD40" s="146"/>
+      <c r="BB40" s="72"/>
+      <c r="BC40" s="73"/>
+      <c r="BD40" s="77"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="138"/>
-      <c r="B41" s="139"/>
-      <c r="C41" s="140"/>
-      <c r="D41" s="95"/>
-      <c r="E41" s="117"/>
+      <c r="A41" s="112"/>
+      <c r="B41" s="113"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="68"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4348,20 +4348,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="141"/>
-      <c r="BC41" s="142"/>
-      <c r="BD41" s="146"/>
+      <c r="BB41" s="72"/>
+      <c r="BC41" s="73"/>
+      <c r="BD41" s="77"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="98" t="s">
+      <c r="A42" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="99"/>
-      <c r="C42" s="100"/>
-      <c r="D42" s="85">
+      <c r="B42" s="90"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="65">
         <v>2</v>
       </c>
-      <c r="E42" s="87">
+      <c r="E42" s="67">
         <v>2.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -4412,16 +4412,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="141"/>
-      <c r="BC42" s="142"/>
-      <c r="BD42" s="146"/>
+      <c r="BB42" s="72"/>
+      <c r="BC42" s="73"/>
+      <c r="BD42" s="77"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="91"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="93"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="117"/>
+      <c r="A43" s="92"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="68"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4470,20 +4470,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="141"/>
-      <c r="BC43" s="142"/>
-      <c r="BD43" s="146"/>
+      <c r="BB43" s="72"/>
+      <c r="BC43" s="73"/>
+      <c r="BD43" s="77"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="99"/>
-      <c r="C44" s="100"/>
-      <c r="D44" s="85">
+      <c r="B44" s="90"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="65">
         <v>2</v>
       </c>
-      <c r="E44" s="87">
+      <c r="E44" s="67">
         <v>2</v>
       </c>
       <c r="F44" s="8"/>
@@ -4534,16 +4534,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="141"/>
-      <c r="BC44" s="142"/>
-      <c r="BD44" s="146"/>
+      <c r="BB44" s="72"/>
+      <c r="BC44" s="73"/>
+      <c r="BD44" s="77"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="101"/>
-      <c r="B45" s="102"/>
-      <c r="C45" s="103"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="84"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="83"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4592,20 +4592,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="141"/>
-      <c r="BC45" s="142"/>
-      <c r="BD45" s="147"/>
+      <c r="BB45" s="72"/>
+      <c r="BC45" s="73"/>
+      <c r="BD45" s="78"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="128" t="s">
+      <c r="A46" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="129"/>
-      <c r="C46" s="130"/>
-      <c r="D46" s="122">
+      <c r="B46" s="103"/>
+      <c r="C46" s="104"/>
+      <c r="D46" s="79">
         <v>1</v>
       </c>
-      <c r="E46" s="96">
+      <c r="E46" s="80">
         <v>1.5</v>
       </c>
       <c r="F46" s="50"/>
@@ -4655,18 +4655,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="141"/>
-      <c r="BC46" s="142"/>
-      <c r="BD46" s="75" t="s">
+      <c r="BB46" s="72"/>
+      <c r="BC46" s="73"/>
+      <c r="BD46" s="71" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="91"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="95"/>
-      <c r="E47" s="97"/>
+      <c r="A47" s="92"/>
+      <c r="B47" s="93"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="81"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4715,20 +4715,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="141"/>
-      <c r="BC47" s="142"/>
-      <c r="BD47" s="75"/>
+      <c r="BB47" s="72"/>
+      <c r="BC47" s="73"/>
+      <c r="BD47" s="71"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="99"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="85">
+      <c r="B48" s="90"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="65">
         <v>2</v>
       </c>
-      <c r="E48" s="87">
+      <c r="E48" s="67">
         <v>3.5</v>
       </c>
       <c r="F48" s="50"/>
@@ -4779,16 +4779,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="141"/>
-      <c r="BC48" s="142"/>
-      <c r="BD48" s="75"/>
+      <c r="BB48" s="72"/>
+      <c r="BC48" s="73"/>
+      <c r="BD48" s="71"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="101"/>
-      <c r="B49" s="102"/>
-      <c r="C49" s="103"/>
-      <c r="D49" s="86"/>
-      <c r="E49" s="84"/>
+      <c r="A49" s="99"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="83"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4837,20 +4837,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="141"/>
-      <c r="BC49" s="142"/>
-      <c r="BD49" s="75"/>
+      <c r="BB49" s="72"/>
+      <c r="BC49" s="73"/>
+      <c r="BD49" s="71"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="124" t="s">
+      <c r="A50" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
-      <c r="D50" s="122">
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="79">
         <v>5</v>
       </c>
-      <c r="E50" s="123">
+      <c r="E50" s="84">
         <v>4.5</v>
       </c>
       <c r="F50" s="50"/>
@@ -4901,18 +4901,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="141"/>
-      <c r="BC50" s="142"/>
-      <c r="BD50" s="75" t="s">
+      <c r="BB50" s="72"/>
+      <c r="BC50" s="73"/>
+      <c r="BD50" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="126"/>
-      <c r="B51" s="127"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="95"/>
-      <c r="E51" s="117"/>
+      <c r="A51" s="97"/>
+      <c r="B51" s="98"/>
+      <c r="C51" s="98"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="68"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4946,7 +4946,7 @@
       <c r="AJ51" s="8"/>
       <c r="AK51" s="9"/>
       <c r="AL51" s="48"/>
-      <c r="AM51" s="42"/>
+      <c r="AM51" s="30"/>
       <c r="AN51" s="21"/>
       <c r="AO51" s="8"/>
       <c r="AP51" s="9"/>
@@ -4961,20 +4961,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="141"/>
-      <c r="BC51" s="142"/>
-      <c r="BD51" s="75"/>
+      <c r="BB51" s="72"/>
+      <c r="BC51" s="73"/>
+      <c r="BD51" s="71"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="99"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="85">
+      <c r="B52" s="90"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="87"/>
+      <c r="E52" s="67"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5015,16 +5015,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="44"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="141"/>
-      <c r="BC52" s="142"/>
-      <c r="BD52" s="75"/>
+      <c r="BB52" s="72"/>
+      <c r="BC52" s="73"/>
+      <c r="BD52" s="71"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="101"/>
-      <c r="B53" s="102"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="84"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="101"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="83"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5073,20 +5073,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="141"/>
-      <c r="BC53" s="142"/>
-      <c r="BD53" s="75"/>
+      <c r="BB53" s="72"/>
+      <c r="BC53" s="73"/>
+      <c r="BD53" s="71"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="128" t="s">
+      <c r="A54" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="129"/>
-      <c r="C54" s="130"/>
-      <c r="D54" s="122">
+      <c r="B54" s="103"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="79">
         <v>4.5</v>
       </c>
-      <c r="E54" s="123">
+      <c r="E54" s="84">
         <v>2</v>
       </c>
       <c r="F54" s="50"/>
@@ -5136,16 +5136,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="141"/>
-      <c r="BC54" s="142"/>
+      <c r="BB54" s="72"/>
+      <c r="BC54" s="73"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="91"/>
-      <c r="B55" s="92"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="95"/>
-      <c r="E55" s="117"/>
+      <c r="A55" s="92"/>
+      <c r="B55" s="93"/>
+      <c r="C55" s="94"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5194,16 +5194,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="141"/>
-      <c r="BC55" s="142"/>
+      <c r="BB55" s="72"/>
+      <c r="BC55" s="73"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="128"/>
-      <c r="B56" s="129"/>
-      <c r="C56" s="130"/>
-      <c r="D56" s="122"/>
-      <c r="E56" s="123"/>
+      <c r="A56" s="102"/>
+      <c r="B56" s="103"/>
+      <c r="C56" s="104"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="84"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5252,16 +5252,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="141"/>
-      <c r="BC56" s="142"/>
+      <c r="BB56" s="72"/>
+      <c r="BC56" s="73"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="91"/>
-      <c r="B57" s="92"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="95"/>
-      <c r="E57" s="117"/>
+      <c r="A57" s="92"/>
+      <c r="B57" s="93"/>
+      <c r="C57" s="94"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="68"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5310,16 +5310,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="141"/>
-      <c r="BC57" s="142"/>
+      <c r="BB57" s="72"/>
+      <c r="BC57" s="73"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="98"/>
-      <c r="B58" s="99"/>
-      <c r="C58" s="100"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="87"/>
+      <c r="A58" s="89"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="91"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="67"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5368,16 +5368,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="141"/>
-      <c r="BC58" s="142"/>
+      <c r="BB58" s="72"/>
+      <c r="BC58" s="73"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="101"/>
-      <c r="B59" s="102"/>
-      <c r="C59" s="103"/>
-      <c r="D59" s="86"/>
-      <c r="E59" s="84"/>
+      <c r="A59" s="99"/>
+      <c r="B59" s="100"/>
+      <c r="C59" s="101"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="83"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5426,35 +5426,135 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="143"/>
-      <c r="BC59" s="144"/>
+      <c r="BB59" s="74"/>
+      <c r="BC59" s="75"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="131" t="s">
+      <c r="A60" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="132"/>
-      <c r="C60" s="132"/>
-      <c r="D60" s="118">
+      <c r="B60" s="106"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="85">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="120">
+      <c r="E60" s="87">
         <f>SUM(E4:E59)</f>
         <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="133"/>
-      <c r="B61" s="134"/>
-      <c r="C61" s="134"/>
-      <c r="D61" s="119"/>
-      <c r="E61" s="121"/>
+      <c r="A61" s="107"/>
+      <c r="B61" s="108"/>
+      <c r="C61" s="108"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="88"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="D26:D27"/>
@@ -5479,106 +5579,6 @@
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BD3:BD7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Dokumentation Entscheid absgeschlossen und Realisation begonnen
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="700" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDE3586C-046C-4C52-8C35-92661D3D4C36}"/>
+  <xr:revisionPtr revIDLastSave="705" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C75B34E-D863-4B2C-B724-83C5B32905B6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1079,26 +1079,233 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1120,213 +1327,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1652,7 +1652,7 @@
   <dimension ref="A1:BN62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AJ44" sqref="AJ44"/>
+      <selection activeCell="AQ56" sqref="AQ56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,171 +1664,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="126" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="127"/>
-      <c r="F1" s="128" t="s">
+      <c r="E1" s="110"/>
+      <c r="F1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="134" t="s">
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="136"/>
-      <c r="U1" s="134" t="s">
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="135"/>
-      <c r="W1" s="135"/>
-      <c r="X1" s="135"/>
-      <c r="Y1" s="136"/>
-      <c r="Z1" s="134" t="s">
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="135"/>
-      <c r="AB1" s="135"/>
-      <c r="AC1" s="135"/>
-      <c r="AD1" s="136"/>
-      <c r="AE1" s="134" t="s">
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="135"/>
-      <c r="AG1" s="135"/>
-      <c r="AH1" s="135"/>
-      <c r="AI1" s="136"/>
-      <c r="AJ1" s="134" t="s">
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="135"/>
-      <c r="AL1" s="135"/>
-      <c r="AM1" s="135"/>
-      <c r="AN1" s="136"/>
-      <c r="AO1" s="134" t="s">
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="135"/>
-      <c r="AQ1" s="135"/>
-      <c r="AR1" s="135"/>
-      <c r="AS1" s="136"/>
-      <c r="AT1" s="134" t="s">
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="135"/>
-      <c r="AV1" s="135"/>
-      <c r="AW1" s="135"/>
-      <c r="AX1" s="136"/>
-      <c r="AY1" s="134" t="s">
+      <c r="AU1" s="77"/>
+      <c r="AV1" s="77"/>
+      <c r="AW1" s="77"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="135"/>
-      <c r="BA1" s="135"/>
-      <c r="BB1" s="135"/>
-      <c r="BC1" s="136"/>
-      <c r="BD1" s="71" t="s">
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="77"/>
+      <c r="BB1" s="77"/>
+      <c r="BC1" s="78"/>
+      <c r="BD1" s="75" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="131">
+      <c r="A2" s="107"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="114">
         <v>44957</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="120">
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="79">
         <v>44958</v>
       </c>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="120">
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="79">
         <v>44959</v>
       </c>
-      <c r="Q2" s="121"/>
-      <c r="R2" s="121"/>
-      <c r="S2" s="121"/>
-      <c r="T2" s="122"/>
-      <c r="U2" s="120">
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="79">
         <v>44960</v>
       </c>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
-      <c r="Y2" s="122"/>
-      <c r="Z2" s="120">
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="79">
         <v>44964</v>
       </c>
-      <c r="AA2" s="121"/>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="121"/>
-      <c r="AD2" s="122"/>
-      <c r="AE2" s="120">
+      <c r="AA2" s="80"/>
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="80"/>
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="79">
         <v>44965</v>
       </c>
-      <c r="AF2" s="121"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="121"/>
-      <c r="AI2" s="122"/>
-      <c r="AJ2" s="120">
+      <c r="AF2" s="80"/>
+      <c r="AG2" s="80"/>
+      <c r="AH2" s="80"/>
+      <c r="AI2" s="81"/>
+      <c r="AJ2" s="79">
         <v>44966</v>
       </c>
-      <c r="AK2" s="121"/>
-      <c r="AL2" s="121"/>
-      <c r="AM2" s="121"/>
-      <c r="AN2" s="122"/>
-      <c r="AO2" s="120">
+      <c r="AK2" s="80"/>
+      <c r="AL2" s="80"/>
+      <c r="AM2" s="80"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="79">
         <v>44967</v>
       </c>
-      <c r="AP2" s="121"/>
-      <c r="AQ2" s="121"/>
-      <c r="AR2" s="121"/>
-      <c r="AS2" s="122"/>
-      <c r="AT2" s="120">
+      <c r="AP2" s="80"/>
+      <c r="AQ2" s="80"/>
+      <c r="AR2" s="80"/>
+      <c r="AS2" s="81"/>
+      <c r="AT2" s="79">
         <v>44971</v>
       </c>
-      <c r="AU2" s="121"/>
-      <c r="AV2" s="121"/>
-      <c r="AW2" s="121"/>
-      <c r="AX2" s="122"/>
-      <c r="AY2" s="120">
+      <c r="AU2" s="80"/>
+      <c r="AV2" s="80"/>
+      <c r="AW2" s="80"/>
+      <c r="AX2" s="81"/>
+      <c r="AY2" s="79">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="121"/>
-      <c r="BA2" s="121"/>
-      <c r="BB2" s="121"/>
-      <c r="BC2" s="122"/>
-      <c r="BD2" s="71"/>
+      <c r="AZ2" s="80"/>
+      <c r="BA2" s="80"/>
+      <c r="BB2" s="80"/>
+      <c r="BC2" s="81"/>
+      <c r="BD2" s="75"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125"/>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,18 +1985,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="147"/>
+      <c r="BD3" s="82"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="116"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="69">
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="94">
         <v>30</v>
       </c>
-      <c r="E4" s="80">
+      <c r="E4" s="96">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2047,18 +2047,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="72" t="s">
+      <c r="BB4" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="147"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="82"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="81"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="97"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2094,10 +2094,10 @@
       <c r="AL5" s="30"/>
       <c r="AM5" s="30"/>
       <c r="AN5" s="4"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
+      <c r="AO5" s="30"/>
+      <c r="AP5" s="30"/>
+      <c r="AQ5" s="30"/>
+      <c r="AR5" s="30"/>
       <c r="AS5" s="4"/>
       <c r="AT5" s="8"/>
       <c r="AU5" s="9"/>
@@ -2107,24 +2107,24 @@
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="147"/>
-      <c r="BF5" s="137" t="s">
+      <c r="BB5" s="141"/>
+      <c r="BC5" s="142"/>
+      <c r="BD5" s="82"/>
+      <c r="BF5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="141"/>
+      <c r="BG5" s="69"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="65">
+      <c r="B6" s="99"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="85">
         <v>1</v>
       </c>
-      <c r="E6" s="118">
+      <c r="E6" s="104">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2175,18 +2175,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="72"/>
-      <c r="BC6" s="73"/>
-      <c r="BD6" s="147"/>
-      <c r="BF6" s="138"/>
-      <c r="BG6" s="142"/>
+      <c r="BB6" s="141"/>
+      <c r="BC6" s="142"/>
+      <c r="BD6" s="82"/>
+      <c r="BF6" s="66"/>
+      <c r="BG6" s="70"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
-      <c r="B7" s="100"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="119"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="105"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2235,24 +2235,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="72"/>
-      <c r="BC7" s="73"/>
-      <c r="BD7" s="147"/>
-      <c r="BF7" s="137" t="s">
+      <c r="BB7" s="141"/>
+      <c r="BC7" s="142"/>
+      <c r="BD7" s="82"/>
+      <c r="BF7" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="143"/>
+      <c r="BG7" s="71"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="115" t="s">
+      <c r="A8" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="116"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="69">
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="94">
         <v>1.5</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="83">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
@@ -2303,20 +2303,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="72"/>
-      <c r="BC8" s="73"/>
-      <c r="BD8" s="71" t="s">
+      <c r="BB8" s="141"/>
+      <c r="BC8" s="142"/>
+      <c r="BD8" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="138"/>
-      <c r="BG8" s="144"/>
+      <c r="BF8" s="66"/>
+      <c r="BG8" s="72"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
-      <c r="B9" s="93"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="68"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="117"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2352,7 +2352,7 @@
       <c r="AL9" s="9"/>
       <c r="AM9" s="9"/>
       <c r="AN9" s="4"/>
-      <c r="AO9" s="8"/>
+      <c r="AO9" s="30"/>
       <c r="AP9" s="9"/>
       <c r="AQ9" s="9"/>
       <c r="AR9" s="9"/>
@@ -2365,24 +2365,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="72"/>
-      <c r="BC9" s="73"/>
-      <c r="BD9" s="71"/>
-      <c r="BF9" s="139" t="s">
+      <c r="BB9" s="141"/>
+      <c r="BC9" s="142"/>
+      <c r="BD9" s="75"/>
+      <c r="BF9" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="145"/>
+      <c r="BG9" s="73"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="65">
+      <c r="B10" s="99"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="85">
         <v>1.5</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="87">
         <v>1.5</v>
       </c>
       <c r="F10" s="19"/>
@@ -2433,18 +2433,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="72"/>
-      <c r="BC10" s="73"/>
-      <c r="BD10" s="71"/>
-      <c r="BF10" s="140"/>
-      <c r="BG10" s="146"/>
+      <c r="BB10" s="141"/>
+      <c r="BC10" s="142"/>
+      <c r="BD10" s="75"/>
+      <c r="BF10" s="68"/>
+      <c r="BG10" s="74"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="83"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="84"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2480,7 +2480,7 @@
       <c r="AL11" s="11"/>
       <c r="AM11" s="11"/>
       <c r="AN11" s="12"/>
-      <c r="AO11" s="10"/>
+      <c r="AO11" s="30"/>
       <c r="AP11" s="11"/>
       <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
@@ -2493,20 +2493,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="72"/>
-      <c r="BC11" s="73"/>
-      <c r="BD11" s="71"/>
+      <c r="BB11" s="141"/>
+      <c r="BC11" s="142"/>
+      <c r="BD11" s="75"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="115" t="s">
+      <c r="A12" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="117"/>
-      <c r="D12" s="69">
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="94">
         <v>1</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="83">
         <v>1.5</v>
       </c>
       <c r="F12" s="19"/>
@@ -2557,9 +2557,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="72"/>
-      <c r="BC12" s="73"/>
-      <c r="BD12" s="71" t="s">
+      <c r="BB12" s="141"/>
+      <c r="BC12" s="142"/>
+      <c r="BD12" s="75" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2573,11 +2573,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="92"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="68"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="117"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2626,9 +2626,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="72"/>
-      <c r="BC13" s="73"/>
-      <c r="BD13" s="71"/>
+      <c r="BB13" s="141"/>
+      <c r="BC13" s="142"/>
+      <c r="BD13" s="75"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2640,15 +2640,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="65">
+      <c r="B14" s="99"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="85">
         <v>2</v>
       </c>
-      <c r="E14" s="67">
+      <c r="E14" s="87">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2699,16 +2699,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="72"/>
-      <c r="BC14" s="73"/>
-      <c r="BD14" s="71"/>
+      <c r="BB14" s="141"/>
+      <c r="BC14" s="142"/>
+      <c r="BD14" s="75"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="92"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="68"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="117"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2757,20 +2757,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="72"/>
-      <c r="BC15" s="73"/>
-      <c r="BD15" s="71"/>
+      <c r="BB15" s="141"/>
+      <c r="BC15" s="142"/>
+      <c r="BD15" s="75"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="90"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="65">
+      <c r="B16" s="99"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="85">
         <v>1</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="87">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2821,16 +2821,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="72"/>
-      <c r="BC16" s="73"/>
-      <c r="BD16" s="71"/>
+      <c r="BB16" s="141"/>
+      <c r="BC16" s="142"/>
+      <c r="BD16" s="75"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="92"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="68"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="117"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2879,23 +2879,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="72"/>
-      <c r="BC17" s="73"/>
-      <c r="BD17" s="71"/>
+      <c r="BB17" s="141"/>
+      <c r="BC17" s="142"/>
+      <c r="BD17" s="75"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="90"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="65">
+      <c r="B18" s="99"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="85">
         <v>2</v>
       </c>
-      <c r="E18" s="67">
+      <c r="E18" s="87">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2946,16 +2946,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="72"/>
-      <c r="BC18" s="73"/>
-      <c r="BD18" s="71"/>
+      <c r="BB18" s="141"/>
+      <c r="BC18" s="142"/>
+      <c r="BD18" s="75"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="92"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="68"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="117"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3004,20 +3004,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="72"/>
-      <c r="BC19" s="73"/>
-      <c r="BD19" s="71"/>
+      <c r="BB19" s="141"/>
+      <c r="BC19" s="142"/>
+      <c r="BD19" s="75"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="89" t="s">
+      <c r="A20" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="90"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="65">
+      <c r="B20" s="99"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="85">
         <v>1</v>
       </c>
-      <c r="E20" s="67">
+      <c r="E20" s="87">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3068,16 +3068,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="72"/>
-      <c r="BC20" s="73"/>
-      <c r="BD20" s="71"/>
+      <c r="BB20" s="141"/>
+      <c r="BC20" s="142"/>
+      <c r="BD20" s="75"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="83"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="84"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3126,20 +3126,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="72"/>
-      <c r="BC21" s="73"/>
-      <c r="BD21" s="71"/>
+      <c r="BB21" s="141"/>
+      <c r="BC21" s="142"/>
+      <c r="BD21" s="75"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="115" t="s">
+      <c r="A22" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="69">
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="94">
         <v>0.5</v>
       </c>
-      <c r="E22" s="70">
+      <c r="E22" s="83">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3190,18 +3190,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="72"/>
-      <c r="BC22" s="73"/>
-      <c r="BD22" s="71" t="s">
+      <c r="BB22" s="141"/>
+      <c r="BC22" s="142"/>
+      <c r="BD22" s="75" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="99"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="83"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="84"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3250,20 +3250,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="72"/>
-      <c r="BC23" s="73"/>
-      <c r="BD23" s="71"/>
+      <c r="BB23" s="141"/>
+      <c r="BC23" s="142"/>
+      <c r="BD23" s="75"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="115" t="s">
+      <c r="A24" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="116"/>
-      <c r="C24" s="117"/>
-      <c r="D24" s="69">
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="94">
         <v>2</v>
       </c>
-      <c r="E24" s="70">
+      <c r="E24" s="83">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3314,18 +3314,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="72"/>
-      <c r="BC24" s="73"/>
-      <c r="BD24" s="76" t="s">
+      <c r="BB24" s="141"/>
+      <c r="BC24" s="142"/>
+      <c r="BD24" s="145" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="68"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="117"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3374,20 +3374,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="72"/>
-      <c r="BC25" s="73"/>
-      <c r="BD25" s="77"/>
+      <c r="BB25" s="141"/>
+      <c r="BC25" s="142"/>
+      <c r="BD25" s="146"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="89" t="s">
+      <c r="A26" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="90"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="65">
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="85">
         <v>1</v>
       </c>
-      <c r="E26" s="67">
+      <c r="E26" s="87">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3438,16 +3438,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="72"/>
-      <c r="BC26" s="73"/>
-      <c r="BD26" s="77"/>
+      <c r="BB26" s="141"/>
+      <c r="BC26" s="142"/>
+      <c r="BD26" s="146"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
-      <c r="B27" s="93"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="68"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="117"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3496,20 +3496,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="72"/>
-      <c r="BC27" s="73"/>
-      <c r="BD27" s="77"/>
+      <c r="BB27" s="141"/>
+      <c r="BC27" s="142"/>
+      <c r="BD27" s="146"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="90"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="65">
+      <c r="B28" s="99"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="85">
         <v>2</v>
       </c>
-      <c r="E28" s="67">
+      <c r="E28" s="87">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3560,16 +3560,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="72"/>
-      <c r="BC28" s="73"/>
-      <c r="BD28" s="77"/>
+      <c r="BB28" s="141"/>
+      <c r="BC28" s="142"/>
+      <c r="BD28" s="146"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="92"/>
-      <c r="B29" s="93"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="68"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="117"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3618,20 +3618,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="72"/>
-      <c r="BC29" s="73"/>
-      <c r="BD29" s="77"/>
+      <c r="BB29" s="141"/>
+      <c r="BC29" s="142"/>
+      <c r="BD29" s="146"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="90"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="65">
+      <c r="B30" s="99"/>
+      <c r="C30" s="100"/>
+      <c r="D30" s="85">
         <v>2</v>
       </c>
-      <c r="E30" s="67">
+      <c r="E30" s="87">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3682,16 +3682,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="72"/>
-      <c r="BC30" s="73"/>
-      <c r="BD30" s="77"/>
+      <c r="BB30" s="141"/>
+      <c r="BC30" s="142"/>
+      <c r="BD30" s="146"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="92"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="68"/>
+      <c r="A31" s="91"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="117"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3740,20 +3740,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="72"/>
-      <c r="BC31" s="73"/>
-      <c r="BD31" s="77"/>
+      <c r="BB31" s="141"/>
+      <c r="BC31" s="142"/>
+      <c r="BD31" s="146"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="89" t="s">
+      <c r="A32" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="90"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="65">
+      <c r="B32" s="99"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="85">
         <v>4</v>
       </c>
-      <c r="E32" s="67">
+      <c r="E32" s="87">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3804,16 +3804,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="72"/>
-      <c r="BC32" s="73"/>
-      <c r="BD32" s="77"/>
+      <c r="BB32" s="141"/>
+      <c r="BC32" s="142"/>
+      <c r="BD32" s="146"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="68"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="117"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3862,20 +3862,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="72"/>
-      <c r="BC33" s="73"/>
-      <c r="BD33" s="77"/>
+      <c r="BB33" s="141"/>
+      <c r="BC33" s="142"/>
+      <c r="BD33" s="146"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="110"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="65">
+      <c r="B34" s="136"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="85">
         <v>3</v>
       </c>
-      <c r="E34" s="67">
+      <c r="E34" s="87">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3926,16 +3926,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="72"/>
-      <c r="BC34" s="73"/>
-      <c r="BD34" s="77"/>
+      <c r="BB34" s="141"/>
+      <c r="BC34" s="142"/>
+      <c r="BD34" s="146"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="112"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="68"/>
+      <c r="A35" s="138"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="140"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="117"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3984,20 +3984,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="72"/>
-      <c r="BC35" s="73"/>
-      <c r="BD35" s="77"/>
+      <c r="BB35" s="141"/>
+      <c r="BC35" s="142"/>
+      <c r="BD35" s="146"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="110"/>
-      <c r="C36" s="111"/>
-      <c r="D36" s="65">
+      <c r="B36" s="136"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="85">
         <v>4</v>
       </c>
-      <c r="E36" s="67">
+      <c r="E36" s="87">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4047,16 +4047,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="72"/>
-      <c r="BC36" s="73"/>
-      <c r="BD36" s="77"/>
+      <c r="BB36" s="141"/>
+      <c r="BC36" s="142"/>
+      <c r="BD36" s="146"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
-      <c r="B37" s="113"/>
-      <c r="C37" s="114"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="68"/>
+      <c r="A37" s="138"/>
+      <c r="B37" s="139"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="117"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4105,20 +4105,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="72"/>
-      <c r="BC37" s="73"/>
-      <c r="BD37" s="77"/>
+      <c r="BB37" s="141"/>
+      <c r="BC37" s="142"/>
+      <c r="BD37" s="146"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="109" t="s">
+      <c r="A38" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="110"/>
-      <c r="C38" s="111"/>
-      <c r="D38" s="65">
+      <c r="B38" s="136"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="85">
         <v>1</v>
       </c>
-      <c r="E38" s="67">
+      <c r="E38" s="87">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4167,16 +4167,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="72"/>
-      <c r="BC38" s="73"/>
-      <c r="BD38" s="77"/>
+      <c r="BB38" s="141"/>
+      <c r="BC38" s="142"/>
+      <c r="BD38" s="146"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
-      <c r="B39" s="113"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="68"/>
+      <c r="A39" s="138"/>
+      <c r="B39" s="139"/>
+      <c r="C39" s="140"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="117"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4225,20 +4225,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="72"/>
-      <c r="BC39" s="73"/>
-      <c r="BD39" s="77"/>
+      <c r="BB39" s="141"/>
+      <c r="BC39" s="142"/>
+      <c r="BD39" s="146"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="109" t="s">
+      <c r="A40" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="110"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="65">
+      <c r="B40" s="136"/>
+      <c r="C40" s="137"/>
+      <c r="D40" s="85">
         <v>1</v>
       </c>
-      <c r="E40" s="67">
+      <c r="E40" s="87">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4290,16 +4290,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="72"/>
-      <c r="BC40" s="73"/>
-      <c r="BD40" s="77"/>
+      <c r="BB40" s="141"/>
+      <c r="BC40" s="142"/>
+      <c r="BD40" s="146"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="112"/>
-      <c r="B41" s="113"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="68"/>
+      <c r="A41" s="138"/>
+      <c r="B41" s="139"/>
+      <c r="C41" s="140"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="117"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4348,20 +4348,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="72"/>
-      <c r="BC41" s="73"/>
-      <c r="BD41" s="77"/>
+      <c r="BB41" s="141"/>
+      <c r="BC41" s="142"/>
+      <c r="BD41" s="146"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="89" t="s">
+      <c r="A42" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="90"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="65">
+      <c r="B42" s="99"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="85">
         <v>2</v>
       </c>
-      <c r="E42" s="67">
+      <c r="E42" s="87">
         <v>2.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -4412,16 +4412,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="72"/>
-      <c r="BC42" s="73"/>
-      <c r="BD42" s="77"/>
+      <c r="BB42" s="141"/>
+      <c r="BC42" s="142"/>
+      <c r="BD42" s="146"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="92"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="68"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="93"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="117"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4470,20 +4470,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="72"/>
-      <c r="BC43" s="73"/>
-      <c r="BD43" s="77"/>
+      <c r="BB43" s="141"/>
+      <c r="BC43" s="142"/>
+      <c r="BD43" s="146"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="89" t="s">
+      <c r="A44" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="65">
+      <c r="B44" s="99"/>
+      <c r="C44" s="100"/>
+      <c r="D44" s="85">
         <v>2</v>
       </c>
-      <c r="E44" s="67">
+      <c r="E44" s="87">
         <v>2</v>
       </c>
       <c r="F44" s="8"/>
@@ -4534,16 +4534,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="72"/>
-      <c r="BC44" s="73"/>
-      <c r="BD44" s="77"/>
+      <c r="BB44" s="141"/>
+      <c r="BC44" s="142"/>
+      <c r="BD44" s="146"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="99"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="101"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="83"/>
+      <c r="A45" s="101"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="84"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4592,20 +4592,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="72"/>
-      <c r="BC45" s="73"/>
-      <c r="BD45" s="78"/>
+      <c r="BB45" s="141"/>
+      <c r="BC45" s="142"/>
+      <c r="BD45" s="147"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="102" t="s">
+      <c r="A46" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="103"/>
-      <c r="C46" s="104"/>
-      <c r="D46" s="79">
+      <c r="B46" s="129"/>
+      <c r="C46" s="130"/>
+      <c r="D46" s="122">
         <v>1</v>
       </c>
-      <c r="E46" s="80">
+      <c r="E46" s="96">
         <v>1.5</v>
       </c>
       <c r="F46" s="50"/>
@@ -4655,18 +4655,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="72"/>
-      <c r="BC46" s="73"/>
-      <c r="BD46" s="71" t="s">
+      <c r="BB46" s="141"/>
+      <c r="BC46" s="142"/>
+      <c r="BD46" s="75" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="92"/>
-      <c r="B47" s="93"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="81"/>
+      <c r="A47" s="91"/>
+      <c r="B47" s="92"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="97"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4715,20 +4715,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="72"/>
-      <c r="BC47" s="73"/>
-      <c r="BD47" s="71"/>
+      <c r="BB47" s="141"/>
+      <c r="BC47" s="142"/>
+      <c r="BD47" s="75"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="89" t="s">
+      <c r="A48" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="90"/>
-      <c r="C48" s="91"/>
-      <c r="D48" s="65">
+      <c r="B48" s="99"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="85">
         <v>2</v>
       </c>
-      <c r="E48" s="67">
+      <c r="E48" s="87">
         <v>3.5</v>
       </c>
       <c r="F48" s="50"/>
@@ -4779,16 +4779,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="72"/>
-      <c r="BC48" s="73"/>
-      <c r="BD48" s="71"/>
+      <c r="BB48" s="141"/>
+      <c r="BC48" s="142"/>
+      <c r="BD48" s="75"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="99"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="101"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="83"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="103"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="84"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4837,20 +4837,20 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="72"/>
-      <c r="BC49" s="73"/>
-      <c r="BD49" s="71"/>
+      <c r="BB49" s="141"/>
+      <c r="BC49" s="142"/>
+      <c r="BD49" s="75"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="95" t="s">
+      <c r="A50" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="96"/>
-      <c r="C50" s="96"/>
-      <c r="D50" s="79">
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
+      <c r="D50" s="122">
         <v>5</v>
       </c>
-      <c r="E50" s="84">
+      <c r="E50" s="123">
         <v>4.5</v>
       </c>
       <c r="F50" s="50"/>
@@ -4901,18 +4901,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="72"/>
-      <c r="BC50" s="73"/>
-      <c r="BD50" s="71" t="s">
+      <c r="BB50" s="141"/>
+      <c r="BC50" s="142"/>
+      <c r="BD50" s="75" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="97"/>
-      <c r="B51" s="98"/>
-      <c r="C51" s="98"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="68"/>
+      <c r="A51" s="126"/>
+      <c r="B51" s="127"/>
+      <c r="C51" s="127"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="117"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4951,7 +4951,7 @@
       <c r="AO51" s="8"/>
       <c r="AP51" s="9"/>
       <c r="AQ51" s="48"/>
-      <c r="AR51" s="42"/>
+      <c r="AR51" s="30"/>
       <c r="AS51" s="21"/>
       <c r="AT51" s="8"/>
       <c r="AU51" s="9"/>
@@ -4961,20 +4961,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="72"/>
-      <c r="BC51" s="73"/>
-      <c r="BD51" s="71"/>
+      <c r="BB51" s="141"/>
+      <c r="BC51" s="142"/>
+      <c r="BD51" s="75"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="89" t="s">
+      <c r="A52" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="90"/>
-      <c r="C52" s="91"/>
-      <c r="D52" s="65">
+      <c r="B52" s="99"/>
+      <c r="C52" s="100"/>
+      <c r="D52" s="85">
         <v>2</v>
       </c>
-      <c r="E52" s="67"/>
+      <c r="E52" s="87"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5015,16 +5015,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="44"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="72"/>
-      <c r="BC52" s="73"/>
-      <c r="BD52" s="71"/>
+      <c r="BB52" s="141"/>
+      <c r="BC52" s="142"/>
+      <c r="BD52" s="75"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="99"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="101"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="83"/>
+      <c r="A53" s="101"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="84"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5073,20 +5073,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="72"/>
-      <c r="BC53" s="73"/>
-      <c r="BD53" s="71"/>
+      <c r="BB53" s="141"/>
+      <c r="BC53" s="142"/>
+      <c r="BD53" s="75"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="102" t="s">
+      <c r="A54" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="103"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="79">
+      <c r="B54" s="129"/>
+      <c r="C54" s="130"/>
+      <c r="D54" s="122">
         <v>4.5</v>
       </c>
-      <c r="E54" s="84">
+      <c r="E54" s="123">
         <v>2</v>
       </c>
       <c r="F54" s="50"/>
@@ -5136,16 +5136,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="72"/>
-      <c r="BC54" s="73"/>
+      <c r="BB54" s="141"/>
+      <c r="BC54" s="142"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="92"/>
-      <c r="B55" s="93"/>
-      <c r="C55" s="94"/>
-      <c r="D55" s="66"/>
-      <c r="E55" s="68"/>
+      <c r="A55" s="91"/>
+      <c r="B55" s="92"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="117"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5194,16 +5194,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="72"/>
-      <c r="BC55" s="73"/>
+      <c r="BB55" s="141"/>
+      <c r="BC55" s="142"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="102"/>
-      <c r="B56" s="103"/>
-      <c r="C56" s="104"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="84"/>
+      <c r="A56" s="128"/>
+      <c r="B56" s="129"/>
+      <c r="C56" s="130"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="123"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5252,16 +5252,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="72"/>
-      <c r="BC56" s="73"/>
+      <c r="BB56" s="141"/>
+      <c r="BC56" s="142"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="92"/>
-      <c r="B57" s="93"/>
-      <c r="C57" s="94"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="68"/>
+      <c r="A57" s="91"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="93"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="117"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5310,16 +5310,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="72"/>
-      <c r="BC57" s="73"/>
+      <c r="BB57" s="141"/>
+      <c r="BC57" s="142"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="89"/>
-      <c r="B58" s="90"/>
-      <c r="C58" s="91"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="67"/>
+      <c r="A58" s="98"/>
+      <c r="B58" s="99"/>
+      <c r="C58" s="100"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="87"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5368,16 +5368,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="72"/>
-      <c r="BC58" s="73"/>
+      <c r="BB58" s="141"/>
+      <c r="BC58" s="142"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="101"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="83"/>
+      <c r="A59" s="101"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="103"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="84"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5426,74 +5426,96 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="74"/>
-      <c r="BC59" s="75"/>
+      <c r="BB59" s="143"/>
+      <c r="BC59" s="144"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="105" t="s">
+      <c r="A60" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="106"/>
-      <c r="C60" s="106"/>
-      <c r="D60" s="85">
+      <c r="B60" s="132"/>
+      <c r="C60" s="132"/>
+      <c r="D60" s="118">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="87">
+      <c r="E60" s="120">
         <f>SUM(E4:E59)</f>
         <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="107"/>
-      <c r="B61" s="108"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="86"/>
-      <c r="E61" s="88"/>
+      <c r="A61" s="133"/>
+      <c r="B61" s="134"/>
+      <c r="C61" s="134"/>
+      <c r="D61" s="119"/>
+      <c r="E61" s="121"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BD3:BD7"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="BD8:BD11"/>
+    <mergeCell ref="BD12:BD21"/>
+    <mergeCell ref="BD22:BD23"/>
+    <mergeCell ref="BB4:BC59"/>
+    <mergeCell ref="BD50:BD53"/>
+    <mergeCell ref="BD46:BD49"/>
+    <mergeCell ref="BD24:BD45"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
     <mergeCell ref="A20:C21"/>
     <mergeCell ref="A22:C23"/>
     <mergeCell ref="A24:C25"/>
@@ -5518,67 +5540,45 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="BD8:BD11"/>
-    <mergeCell ref="BD12:BD21"/>
-    <mergeCell ref="BD22:BD23"/>
-    <mergeCell ref="BB4:BC59"/>
-    <mergeCell ref="BD50:BD53"/>
-    <mergeCell ref="BD46:BD49"/>
-    <mergeCell ref="BD24:BD45"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BD3:BD7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fehler in der Darstellung vom Grid, Doku weitergeschrieben (Realisierung), Arbeitsjournal Zeiterfassung
</commit_message>
<xml_diff>
--- a/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
+++ b/Doku/PA_ProjektAnalyse_ZeitPlan_Alain_Hoch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueofficech-my.sharepoint.com/personal/a_hoch_blue-office_ch/Documents/IPA/boProjektAnalyse/Doku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="705" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C75B34E-D863-4B2C-B724-83C5B32905B6}"/>
+  <xr:revisionPtr revIDLastSave="710" documentId="8_{9C9B4D5D-1A59-475A-94EF-ED16E8ABAE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80B3D01D-C7C5-4404-9A85-9542F7AF83AC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF239887-3018-470C-857D-60A4FA8C1B03}"/>
   </bookViews>
@@ -1009,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1079,6 +1079,222 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1110,224 +1326,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1651,8 +1652,8 @@
   </sheetPr>
   <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AQ56" sqref="AQ56"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AP23" sqref="AP23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,171 +1665,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="109" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="110"/>
-      <c r="F1" s="111" t="s">
+      <c r="E1" s="127"/>
+      <c r="F1" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="76" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="76" t="s">
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="76" t="s">
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="136"/>
+      <c r="U1" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="76" t="s">
+      <c r="V1" s="135"/>
+      <c r="W1" s="135"/>
+      <c r="X1" s="135"/>
+      <c r="Y1" s="136"/>
+      <c r="Z1" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="76" t="s">
+      <c r="AA1" s="135"/>
+      <c r="AB1" s="135"/>
+      <c r="AC1" s="135"/>
+      <c r="AD1" s="136"/>
+      <c r="AE1" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="76" t="s">
+      <c r="AF1" s="135"/>
+      <c r="AG1" s="135"/>
+      <c r="AH1" s="135"/>
+      <c r="AI1" s="136"/>
+      <c r="AJ1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="76" t="s">
+      <c r="AK1" s="135"/>
+      <c r="AL1" s="135"/>
+      <c r="AM1" s="135"/>
+      <c r="AN1" s="136"/>
+      <c r="AO1" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="78"/>
-      <c r="AT1" s="76" t="s">
+      <c r="AP1" s="135"/>
+      <c r="AQ1" s="135"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
+      <c r="AT1" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="78"/>
-      <c r="AY1" s="76" t="s">
+      <c r="AU1" s="135"/>
+      <c r="AV1" s="135"/>
+      <c r="AW1" s="135"/>
+      <c r="AX1" s="136"/>
+      <c r="AY1" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="77"/>
-      <c r="BB1" s="77"/>
-      <c r="BC1" s="78"/>
-      <c r="BD1" s="75" t="s">
+      <c r="AZ1" s="135"/>
+      <c r="BA1" s="135"/>
+      <c r="BB1" s="135"/>
+      <c r="BC1" s="136"/>
+      <c r="BD1" s="71" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="114">
+      <c r="A2" s="124"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="131">
         <v>44957</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="79">
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="120">
         <v>44958</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="79">
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="120">
         <v>44959</v>
       </c>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="79">
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="120">
         <v>44960</v>
       </c>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="79">
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="120">
         <v>44964</v>
       </c>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="80"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="79">
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="122"/>
+      <c r="AE2" s="120">
         <v>44965</v>
       </c>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
-      <c r="AH2" s="80"/>
-      <c r="AI2" s="81"/>
-      <c r="AJ2" s="79">
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="121"/>
+      <c r="AH2" s="121"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="120">
         <v>44966</v>
       </c>
-      <c r="AK2" s="80"/>
-      <c r="AL2" s="80"/>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="81"/>
-      <c r="AO2" s="79">
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121"/>
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="120">
         <v>44967</v>
       </c>
-      <c r="AP2" s="80"/>
-      <c r="AQ2" s="80"/>
-      <c r="AR2" s="80"/>
-      <c r="AS2" s="81"/>
-      <c r="AT2" s="79">
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="120">
         <v>44971</v>
       </c>
-      <c r="AU2" s="80"/>
-      <c r="AV2" s="80"/>
-      <c r="AW2" s="80"/>
-      <c r="AX2" s="81"/>
-      <c r="AY2" s="79">
+      <c r="AU2" s="121"/>
+      <c r="AV2" s="121"/>
+      <c r="AW2" s="121"/>
+      <c r="AX2" s="122"/>
+      <c r="AY2" s="120">
         <v>44972</v>
       </c>
-      <c r="AZ2" s="80"/>
-      <c r="BA2" s="80"/>
-      <c r="BB2" s="80"/>
-      <c r="BC2" s="81"/>
-      <c r="BD2" s="75"/>
+      <c r="AZ2" s="121"/>
+      <c r="BA2" s="121"/>
+      <c r="BB2" s="121"/>
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="71"/>
     </row>
     <row r="3" spans="1:66" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,18 +1986,18 @@
       <c r="BC3" s="12">
         <v>17</v>
       </c>
-      <c r="BD3" s="82"/>
+      <c r="BD3" s="147"/>
     </row>
     <row r="4" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="94">
+      <c r="B4" s="116"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="69">
         <v>30</v>
       </c>
-      <c r="E4" s="96">
+      <c r="E4" s="80">
         <v>30</v>
       </c>
       <c r="F4" s="15"/>
@@ -2047,18 +2048,18 @@
       <c r="AY4" s="17"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
-      <c r="BB4" s="141" t="s">
+      <c r="BB4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="BC4" s="142"/>
-      <c r="BD4" s="82"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="147"/>
     </row>
     <row r="5" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="97"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2099,32 +2100,32 @@
       <c r="AQ5" s="30"/>
       <c r="AR5" s="30"/>
       <c r="AS5" s="4"/>
-      <c r="AT5" s="8"/>
-      <c r="AU5" s="9"/>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9"/>
-      <c r="AX5" s="4"/>
+      <c r="AT5" s="148"/>
+      <c r="AU5" s="30"/>
+      <c r="AV5" s="30"/>
+      <c r="AW5" s="30"/>
+      <c r="AX5" s="63"/>
       <c r="AY5" s="8"/>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9"/>
-      <c r="BB5" s="141"/>
-      <c r="BC5" s="142"/>
-      <c r="BD5" s="82"/>
-      <c r="BF5" s="65" t="s">
+      <c r="BB5" s="72"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="147"/>
+      <c r="BF5" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="69"/>
+      <c r="BG5" s="141"/>
     </row>
     <row r="6" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="98" t="s">
+      <c r="A6" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="99"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="85">
+      <c r="B6" s="90"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="65">
         <v>1</v>
       </c>
-      <c r="E6" s="104">
+      <c r="E6" s="118">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
@@ -2175,18 +2176,18 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="141"/>
-      <c r="BC6" s="142"/>
-      <c r="BD6" s="82"/>
-      <c r="BF6" s="66"/>
-      <c r="BG6" s="70"/>
+      <c r="BB6" s="72"/>
+      <c r="BC6" s="73"/>
+      <c r="BD6" s="147"/>
+      <c r="BF6" s="138"/>
+      <c r="BG6" s="142"/>
     </row>
     <row r="7" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="105"/>
+      <c r="A7" s="99"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="119"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -2235,24 +2236,24 @@
       <c r="AY7" s="10"/>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="141"/>
-      <c r="BC7" s="142"/>
-      <c r="BD7" s="82"/>
-      <c r="BF7" s="65" t="s">
+      <c r="BB7" s="72"/>
+      <c r="BC7" s="73"/>
+      <c r="BD7" s="147"/>
+      <c r="BF7" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="71"/>
+      <c r="BG7" s="143"/>
     </row>
     <row r="8" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="94">
+      <c r="B8" s="116"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="69">
         <v>1.5</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="70">
         <v>1</v>
       </c>
       <c r="F8" s="17"/>
@@ -2303,20 +2304,20 @@
       <c r="AY8" s="17"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="141"/>
-      <c r="BC8" s="142"/>
-      <c r="BD8" s="75" t="s">
+      <c r="BB8" s="72"/>
+      <c r="BC8" s="73"/>
+      <c r="BD8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="BF8" s="66"/>
-      <c r="BG8" s="72"/>
+      <c r="BF8" s="138"/>
+      <c r="BG8" s="144"/>
     </row>
     <row r="9" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="91"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="117"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="26"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2357,7 +2358,7 @@
       <c r="AQ9" s="9"/>
       <c r="AR9" s="9"/>
       <c r="AS9" s="4"/>
-      <c r="AT9" s="8"/>
+      <c r="AT9" s="36"/>
       <c r="AU9" s="9"/>
       <c r="AV9" s="9"/>
       <c r="AW9" s="9"/>
@@ -2365,24 +2366,24 @@
       <c r="AY9" s="8"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
-      <c r="BB9" s="141"/>
-      <c r="BC9" s="142"/>
-      <c r="BD9" s="75"/>
-      <c r="BF9" s="67" t="s">
+      <c r="BB9" s="72"/>
+      <c r="BC9" s="73"/>
+      <c r="BD9" s="71"/>
+      <c r="BF9" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="BG9" s="73"/>
+      <c r="BG9" s="145"/>
     </row>
     <row r="10" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="85">
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="65">
         <v>1.5</v>
       </c>
-      <c r="E10" s="87">
+      <c r="E10" s="67">
         <v>1.5</v>
       </c>
       <c r="F10" s="19"/>
@@ -2433,18 +2434,18 @@
       <c r="AY10" s="19"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
-      <c r="BB10" s="141"/>
-      <c r="BC10" s="142"/>
-      <c r="BD10" s="75"/>
-      <c r="BF10" s="68"/>
-      <c r="BG10" s="74"/>
+      <c r="BB10" s="72"/>
+      <c r="BC10" s="73"/>
+      <c r="BD10" s="71"/>
+      <c r="BF10" s="140"/>
+      <c r="BG10" s="146"/>
     </row>
     <row r="11" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="84"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="83"/>
       <c r="F11" s="27"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -2485,7 +2486,7 @@
       <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
       <c r="AS11" s="12"/>
-      <c r="AT11" s="10"/>
+      <c r="AT11" s="37"/>
       <c r="AU11" s="11"/>
       <c r="AV11" s="11"/>
       <c r="AW11" s="11"/>
@@ -2493,20 +2494,20 @@
       <c r="AY11" s="10"/>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="11"/>
-      <c r="BB11" s="141"/>
-      <c r="BC11" s="142"/>
-      <c r="BD11" s="75"/>
+      <c r="BB11" s="72"/>
+      <c r="BC11" s="73"/>
+      <c r="BD11" s="71"/>
     </row>
     <row r="12" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="94">
+      <c r="B12" s="116"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="69">
         <v>1</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="70">
         <v>1.5</v>
       </c>
       <c r="F12" s="19"/>
@@ -2557,9 +2558,9 @@
       <c r="AY12" s="5"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="141"/>
-      <c r="BC12" s="142"/>
-      <c r="BD12" s="75" t="s">
+      <c r="BB12" s="72"/>
+      <c r="BC12" s="73"/>
+      <c r="BD12" s="71" t="s">
         <v>16</v>
       </c>
       <c r="BF12" s="13"/>
@@ -2573,11 +2574,11 @@
       <c r="BN12" s="13"/>
     </row>
     <row r="13" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="91"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="117"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="9"/>
@@ -2626,9 +2627,9 @@
       <c r="AY13" s="8"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="141"/>
-      <c r="BC13" s="142"/>
-      <c r="BD13" s="75"/>
+      <c r="BB13" s="72"/>
+      <c r="BC13" s="73"/>
+      <c r="BD13" s="71"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
@@ -2640,15 +2641,15 @@
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="98" t="s">
+      <c r="A14" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="85">
+      <c r="B14" s="90"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="65">
         <v>2</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="67">
         <v>2</v>
       </c>
       <c r="F14" s="20"/>
@@ -2699,16 +2700,16 @@
       <c r="AY14" s="8"/>
       <c r="AZ14" s="9"/>
       <c r="BA14" s="9"/>
-      <c r="BB14" s="141"/>
-      <c r="BC14" s="142"/>
-      <c r="BD14" s="75"/>
+      <c r="BB14" s="72"/>
+      <c r="BC14" s="73"/>
+      <c r="BD14" s="71"/>
     </row>
     <row r="15" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="91"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="117"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="68"/>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2757,20 +2758,20 @@
       <c r="AY15" s="8"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="141"/>
-      <c r="BC15" s="142"/>
-      <c r="BD15" s="75"/>
+      <c r="BB15" s="72"/>
+      <c r="BC15" s="73"/>
+      <c r="BD15" s="71"/>
     </row>
     <row r="16" spans="1:66" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="85">
+      <c r="B16" s="90"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="65">
         <v>1</v>
       </c>
-      <c r="E16" s="87">
+      <c r="E16" s="67">
         <v>2</v>
       </c>
       <c r="F16" s="20"/>
@@ -2821,16 +2822,16 @@
       <c r="AY16" s="8"/>
       <c r="AZ16" s="9"/>
       <c r="BA16" s="9"/>
-      <c r="BB16" s="141"/>
-      <c r="BC16" s="142"/>
-      <c r="BD16" s="75"/>
+      <c r="BB16" s="72"/>
+      <c r="BC16" s="73"/>
+      <c r="BD16" s="71"/>
     </row>
     <row r="17" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="117"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="68"/>
       <c r="F17" s="20"/>
       <c r="G17" s="9"/>
       <c r="H17" s="30"/>
@@ -2879,23 +2880,23 @@
       <c r="AY17" s="8"/>
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
-      <c r="BB17" s="141"/>
-      <c r="BC17" s="142"/>
-      <c r="BD17" s="75"/>
+      <c r="BB17" s="72"/>
+      <c r="BC17" s="73"/>
+      <c r="BD17" s="71"/>
       <c r="BH17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="99"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="85">
+      <c r="B18" s="90"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="65">
         <v>2</v>
       </c>
-      <c r="E18" s="87">
+      <c r="E18" s="67">
         <v>2</v>
       </c>
       <c r="F18" s="20"/>
@@ -2946,16 +2947,16 @@
       <c r="AY18" s="8"/>
       <c r="AZ18" s="9"/>
       <c r="BA18" s="9"/>
-      <c r="BB18" s="141"/>
-      <c r="BC18" s="142"/>
-      <c r="BD18" s="75"/>
+      <c r="BB18" s="72"/>
+      <c r="BC18" s="73"/>
+      <c r="BD18" s="71"/>
     </row>
     <row r="19" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="91"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="117"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="68"/>
       <c r="F19" s="8"/>
       <c r="G19" s="23"/>
       <c r="H19" s="35"/>
@@ -3004,20 +3005,20 @@
       <c r="AY19" s="8"/>
       <c r="AZ19" s="9"/>
       <c r="BA19" s="9"/>
-      <c r="BB19" s="141"/>
-      <c r="BC19" s="142"/>
-      <c r="BD19" s="75"/>
+      <c r="BB19" s="72"/>
+      <c r="BC19" s="73"/>
+      <c r="BD19" s="71"/>
     </row>
     <row r="20" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="99"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="85">
+      <c r="B20" s="90"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="65">
         <v>1</v>
       </c>
-      <c r="E20" s="87">
+      <c r="E20" s="67">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
@@ -3068,16 +3069,16 @@
       <c r="AY20" s="8"/>
       <c r="AZ20" s="9"/>
       <c r="BA20" s="9"/>
-      <c r="BB20" s="141"/>
-      <c r="BC20" s="142"/>
-      <c r="BD20" s="75"/>
+      <c r="BB20" s="72"/>
+      <c r="BC20" s="73"/>
+      <c r="BD20" s="71"/>
     </row>
     <row r="21" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="101"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="84"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3126,20 +3127,20 @@
       <c r="AY21" s="10"/>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="11"/>
-      <c r="BB21" s="141"/>
-      <c r="BC21" s="142"/>
-      <c r="BD21" s="75"/>
+      <c r="BB21" s="72"/>
+      <c r="BC21" s="73"/>
+      <c r="BD21" s="71"/>
     </row>
     <row r="22" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="88" t="s">
+      <c r="A22" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="94">
+      <c r="B22" s="116"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="69">
         <v>0.5</v>
       </c>
-      <c r="E22" s="83">
+      <c r="E22" s="70">
         <v>0.5</v>
       </c>
       <c r="F22" s="5"/>
@@ -3190,18 +3191,18 @@
       <c r="AY22" s="5"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
-      <c r="BB22" s="141"/>
-      <c r="BC22" s="142"/>
-      <c r="BD22" s="75" t="s">
+      <c r="BB22" s="72"/>
+      <c r="BC22" s="73"/>
+      <c r="BD22" s="71" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="101"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="84"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="83"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3250,20 +3251,20 @@
       <c r="AY23" s="10"/>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="11"/>
-      <c r="BB23" s="141"/>
-      <c r="BC23" s="142"/>
-      <c r="BD23" s="75"/>
+      <c r="BB23" s="72"/>
+      <c r="BC23" s="73"/>
+      <c r="BD23" s="71"/>
     </row>
     <row r="24" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="94">
+      <c r="B24" s="116"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="69">
         <v>2</v>
       </c>
-      <c r="E24" s="83">
+      <c r="E24" s="70">
         <v>1</v>
       </c>
       <c r="F24" s="5"/>
@@ -3314,18 +3315,18 @@
       <c r="AY24" s="5"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
-      <c r="BB24" s="141"/>
-      <c r="BC24" s="142"/>
-      <c r="BD24" s="145" t="s">
+      <c r="BB24" s="72"/>
+      <c r="BC24" s="73"/>
+      <c r="BD24" s="76" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="91"/>
-      <c r="B25" s="92"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="117"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="68"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3374,20 +3375,20 @@
       <c r="AY25" s="8"/>
       <c r="AZ25" s="9"/>
       <c r="BA25" s="9"/>
-      <c r="BB25" s="141"/>
-      <c r="BC25" s="142"/>
-      <c r="BD25" s="146"/>
+      <c r="BB25" s="72"/>
+      <c r="BC25" s="73"/>
+      <c r="BD25" s="77"/>
     </row>
     <row r="26" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="85">
+      <c r="B26" s="90"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="65">
         <v>1</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="67">
         <v>0.5</v>
       </c>
       <c r="F26" s="8"/>
@@ -3438,16 +3439,16 @@
       <c r="AY26" s="8"/>
       <c r="AZ26" s="9"/>
       <c r="BA26" s="9"/>
-      <c r="BB26" s="141"/>
-      <c r="BC26" s="142"/>
-      <c r="BD26" s="146"/>
+      <c r="BB26" s="72"/>
+      <c r="BC26" s="73"/>
+      <c r="BD26" s="77"/>
     </row>
     <row r="27" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="91"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="117"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="68"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -3496,20 +3497,20 @@
       <c r="AY27" s="8"/>
       <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="141"/>
-      <c r="BC27" s="142"/>
-      <c r="BD27" s="146"/>
+      <c r="BB27" s="72"/>
+      <c r="BC27" s="73"/>
+      <c r="BD27" s="77"/>
     </row>
     <row r="28" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="99"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="85">
+      <c r="B28" s="90"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="65">
         <v>2</v>
       </c>
-      <c r="E28" s="87">
+      <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="8"/>
@@ -3560,16 +3561,16 @@
       <c r="AY28" s="8"/>
       <c r="AZ28" s="9"/>
       <c r="BA28" s="9"/>
-      <c r="BB28" s="141"/>
-      <c r="BC28" s="142"/>
-      <c r="BD28" s="146"/>
+      <c r="BB28" s="72"/>
+      <c r="BC28" s="73"/>
+      <c r="BD28" s="77"/>
     </row>
     <row r="29" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="91"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="117"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="93"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="68"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3618,20 +3619,20 @@
       <c r="AY29" s="8"/>
       <c r="AZ29" s="9"/>
       <c r="BA29" s="9"/>
-      <c r="BB29" s="141"/>
-      <c r="BC29" s="142"/>
-      <c r="BD29" s="146"/>
+      <c r="BB29" s="72"/>
+      <c r="BC29" s="73"/>
+      <c r="BD29" s="77"/>
     </row>
     <row r="30" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="99"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="85">
+      <c r="B30" s="90"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="65">
         <v>2</v>
       </c>
-      <c r="E30" s="87">
+      <c r="E30" s="67">
         <v>2</v>
       </c>
       <c r="F30" s="8"/>
@@ -3682,16 +3683,16 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="9"/>
       <c r="BA30" s="9"/>
-      <c r="BB30" s="141"/>
-      <c r="BC30" s="142"/>
-      <c r="BD30" s="146"/>
+      <c r="BB30" s="72"/>
+      <c r="BC30" s="73"/>
+      <c r="BD30" s="77"/>
     </row>
     <row r="31" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="117"/>
+      <c r="A31" s="92"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="68"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3740,20 +3741,20 @@
       <c r="AY31" s="8"/>
       <c r="AZ31" s="9"/>
       <c r="BA31" s="9"/>
-      <c r="BB31" s="141"/>
-      <c r="BC31" s="142"/>
-      <c r="BD31" s="146"/>
+      <c r="BB31" s="72"/>
+      <c r="BC31" s="73"/>
+      <c r="BD31" s="77"/>
     </row>
     <row r="32" spans="1:60" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="98" t="s">
+      <c r="A32" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="99"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="85">
+      <c r="B32" s="90"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="65">
         <v>4</v>
       </c>
-      <c r="E32" s="87">
+      <c r="E32" s="67">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3804,16 +3805,16 @@
       <c r="AY32" s="8"/>
       <c r="AZ32" s="9"/>
       <c r="BA32" s="9"/>
-      <c r="BB32" s="141"/>
-      <c r="BC32" s="142"/>
-      <c r="BD32" s="146"/>
+      <c r="BB32" s="72"/>
+      <c r="BC32" s="73"/>
+      <c r="BD32" s="77"/>
     </row>
     <row r="33" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="91"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="117"/>
+      <c r="A33" s="92"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3862,20 +3863,20 @@
       <c r="AY33" s="8"/>
       <c r="AZ33" s="9"/>
       <c r="BA33" s="9"/>
-      <c r="BB33" s="141"/>
-      <c r="BC33" s="142"/>
-      <c r="BD33" s="146"/>
+      <c r="BB33" s="72"/>
+      <c r="BC33" s="73"/>
+      <c r="BD33" s="77"/>
     </row>
     <row r="34" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135" t="s">
+      <c r="A34" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="136"/>
-      <c r="C34" s="137"/>
-      <c r="D34" s="85">
+      <c r="B34" s="110"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="65">
         <v>3</v>
       </c>
-      <c r="E34" s="87">
+      <c r="E34" s="67">
         <v>2.5</v>
       </c>
       <c r="F34" s="8"/>
@@ -3926,16 +3927,16 @@
       <c r="AY34" s="8"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
-      <c r="BB34" s="141"/>
-      <c r="BC34" s="142"/>
-      <c r="BD34" s="146"/>
+      <c r="BB34" s="72"/>
+      <c r="BC34" s="73"/>
+      <c r="BD34" s="77"/>
     </row>
     <row r="35" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="138"/>
-      <c r="B35" s="139"/>
-      <c r="C35" s="140"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="117"/>
+      <c r="A35" s="112"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="68"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3984,20 +3985,20 @@
       <c r="AY35" s="8"/>
       <c r="AZ35" s="9"/>
       <c r="BA35" s="9"/>
-      <c r="BB35" s="141"/>
-      <c r="BC35" s="142"/>
-      <c r="BD35" s="146"/>
+      <c r="BB35" s="72"/>
+      <c r="BC35" s="73"/>
+      <c r="BD35" s="77"/>
     </row>
     <row r="36" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="135" t="s">
+      <c r="A36" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="136"/>
-      <c r="C36" s="137"/>
-      <c r="D36" s="85">
+      <c r="B36" s="110"/>
+      <c r="C36" s="111"/>
+      <c r="D36" s="65">
         <v>4</v>
       </c>
-      <c r="E36" s="87">
+      <c r="E36" s="67">
         <v>4</v>
       </c>
       <c r="F36" s="8"/>
@@ -4047,16 +4048,16 @@
       <c r="AY36" s="8"/>
       <c r="AZ36" s="9"/>
       <c r="BA36" s="9"/>
-      <c r="BB36" s="141"/>
-      <c r="BC36" s="142"/>
-      <c r="BD36" s="146"/>
+      <c r="BB36" s="72"/>
+      <c r="BC36" s="73"/>
+      <c r="BD36" s="77"/>
     </row>
     <row r="37" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="138"/>
-      <c r="B37" s="139"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="117"/>
+      <c r="A37" s="112"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="114"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="68"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -4105,20 +4106,20 @@
       <c r="AY37" s="8"/>
       <c r="AZ37" s="9"/>
       <c r="BA37" s="9"/>
-      <c r="BB37" s="141"/>
-      <c r="BC37" s="142"/>
-      <c r="BD37" s="146"/>
+      <c r="BB37" s="72"/>
+      <c r="BC37" s="73"/>
+      <c r="BD37" s="77"/>
     </row>
     <row r="38" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="135" t="s">
+      <c r="A38" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="136"/>
-      <c r="C38" s="137"/>
-      <c r="D38" s="85">
+      <c r="B38" s="110"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="65">
         <v>1</v>
       </c>
-      <c r="E38" s="87">
+      <c r="E38" s="67">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
@@ -4167,16 +4168,16 @@
       <c r="AY38" s="8"/>
       <c r="AZ38" s="9"/>
       <c r="BA38" s="9"/>
-      <c r="BB38" s="141"/>
-      <c r="BC38" s="142"/>
-      <c r="BD38" s="146"/>
+      <c r="BB38" s="72"/>
+      <c r="BC38" s="73"/>
+      <c r="BD38" s="77"/>
     </row>
     <row r="39" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="138"/>
-      <c r="B39" s="139"/>
-      <c r="C39" s="140"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="117"/>
+      <c r="A39" s="112"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -4225,20 +4226,20 @@
       <c r="AY39" s="8"/>
       <c r="AZ39" s="9"/>
       <c r="BA39" s="9"/>
-      <c r="BB39" s="141"/>
-      <c r="BC39" s="142"/>
-      <c r="BD39" s="146"/>
+      <c r="BB39" s="72"/>
+      <c r="BC39" s="73"/>
+      <c r="BD39" s="77"/>
     </row>
     <row r="40" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="135" t="s">
+      <c r="A40" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="136"/>
-      <c r="C40" s="137"/>
-      <c r="D40" s="85">
+      <c r="B40" s="110"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="65">
         <v>1</v>
       </c>
-      <c r="E40" s="87">
+      <c r="E40" s="67">
         <v>1.5</v>
       </c>
       <c r="F40" s="8"/>
@@ -4290,16 +4291,16 @@
       <c r="AY40" s="8"/>
       <c r="AZ40" s="9"/>
       <c r="BA40" s="9"/>
-      <c r="BB40" s="141"/>
-      <c r="BC40" s="142"/>
-      <c r="BD40" s="146"/>
+      <c r="BB40" s="72"/>
+      <c r="BC40" s="73"/>
+      <c r="BD40" s="77"/>
     </row>
     <row r="41" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="138"/>
-      <c r="B41" s="139"/>
-      <c r="C41" s="140"/>
-      <c r="D41" s="95"/>
-      <c r="E41" s="117"/>
+      <c r="A41" s="112"/>
+      <c r="B41" s="113"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="68"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -4348,20 +4349,20 @@
       <c r="AY41" s="8"/>
       <c r="AZ41" s="9"/>
       <c r="BA41" s="9"/>
-      <c r="BB41" s="141"/>
-      <c r="BC41" s="142"/>
-      <c r="BD41" s="146"/>
+      <c r="BB41" s="72"/>
+      <c r="BC41" s="73"/>
+      <c r="BD41" s="77"/>
     </row>
     <row r="42" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="98" t="s">
+      <c r="A42" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="99"/>
-      <c r="C42" s="100"/>
-      <c r="D42" s="85">
+      <c r="B42" s="90"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="65">
         <v>2</v>
       </c>
-      <c r="E42" s="87">
+      <c r="E42" s="67">
         <v>2.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -4412,16 +4413,16 @@
       <c r="AY42" s="8"/>
       <c r="AZ42" s="9"/>
       <c r="BA42" s="9"/>
-      <c r="BB42" s="141"/>
-      <c r="BC42" s="142"/>
-      <c r="BD42" s="146"/>
+      <c r="BB42" s="72"/>
+      <c r="BC42" s="73"/>
+      <c r="BD42" s="77"/>
     </row>
     <row r="43" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="91"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="93"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="117"/>
+      <c r="A43" s="92"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="68"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -4470,20 +4471,20 @@
       <c r="AY43" s="8"/>
       <c r="AZ43" s="9"/>
       <c r="BA43" s="9"/>
-      <c r="BB43" s="141"/>
-      <c r="BC43" s="142"/>
-      <c r="BD43" s="146"/>
+      <c r="BB43" s="72"/>
+      <c r="BC43" s="73"/>
+      <c r="BD43" s="77"/>
     </row>
     <row r="44" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="99"/>
-      <c r="C44" s="100"/>
-      <c r="D44" s="85">
+      <c r="B44" s="90"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="65">
         <v>2</v>
       </c>
-      <c r="E44" s="87">
+      <c r="E44" s="67">
         <v>2</v>
       </c>
       <c r="F44" s="8"/>
@@ -4534,16 +4535,16 @@
       <c r="AY44" s="8"/>
       <c r="AZ44" s="9"/>
       <c r="BA44" s="9"/>
-      <c r="BB44" s="141"/>
-      <c r="BC44" s="142"/>
-      <c r="BD44" s="146"/>
+      <c r="BB44" s="72"/>
+      <c r="BC44" s="73"/>
+      <c r="BD44" s="77"/>
     </row>
     <row r="45" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="101"/>
-      <c r="B45" s="102"/>
-      <c r="C45" s="103"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="84"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="83"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4592,20 +4593,20 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="11"/>
-      <c r="BB45" s="141"/>
-      <c r="BC45" s="142"/>
-      <c r="BD45" s="147"/>
+      <c r="BB45" s="72"/>
+      <c r="BC45" s="73"/>
+      <c r="BD45" s="78"/>
     </row>
     <row r="46" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="128" t="s">
+      <c r="A46" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="129"/>
-      <c r="C46" s="130"/>
-      <c r="D46" s="122">
+      <c r="B46" s="103"/>
+      <c r="C46" s="104"/>
+      <c r="D46" s="79">
         <v>1</v>
       </c>
-      <c r="E46" s="96">
+      <c r="E46" s="80">
         <v>1.5</v>
       </c>
       <c r="F46" s="50"/>
@@ -4655,18 +4656,18 @@
       <c r="AY46" s="50"/>
       <c r="AZ46" s="23"/>
       <c r="BA46" s="23"/>
-      <c r="BB46" s="141"/>
-      <c r="BC46" s="142"/>
-      <c r="BD46" s="75" t="s">
+      <c r="BB46" s="72"/>
+      <c r="BC46" s="73"/>
+      <c r="BD46" s="71" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="91"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="95"/>
-      <c r="E47" s="97"/>
+      <c r="A47" s="92"/>
+      <c r="B47" s="93"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="81"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4715,20 +4716,20 @@
       <c r="AY47" s="8"/>
       <c r="AZ47" s="9"/>
       <c r="BA47" s="9"/>
-      <c r="BB47" s="141"/>
-      <c r="BC47" s="142"/>
-      <c r="BD47" s="75"/>
+      <c r="BB47" s="72"/>
+      <c r="BC47" s="73"/>
+      <c r="BD47" s="71"/>
     </row>
     <row r="48" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="99"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="85">
+      <c r="B48" s="90"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="65">
         <v>2</v>
       </c>
-      <c r="E48" s="87">
+      <c r="E48" s="67">
         <v>3.5</v>
       </c>
       <c r="F48" s="50"/>
@@ -4779,16 +4780,16 @@
       <c r="AY48" s="50"/>
       <c r="AZ48" s="23"/>
       <c r="BA48" s="23"/>
-      <c r="BB48" s="141"/>
-      <c r="BC48" s="142"/>
-      <c r="BD48" s="75"/>
+      <c r="BB48" s="72"/>
+      <c r="BC48" s="73"/>
+      <c r="BD48" s="71"/>
     </row>
     <row r="49" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="101"/>
-      <c r="B49" s="102"/>
-      <c r="C49" s="103"/>
-      <c r="D49" s="86"/>
-      <c r="E49" s="84"/>
+      <c r="A49" s="99"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="83"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4837,21 +4838,21 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="11"/>
-      <c r="BB49" s="141"/>
-      <c r="BC49" s="142"/>
-      <c r="BD49" s="75"/>
+      <c r="BB49" s="72"/>
+      <c r="BC49" s="73"/>
+      <c r="BD49" s="71"/>
     </row>
     <row r="50" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="124" t="s">
+      <c r="A50" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
-      <c r="D50" s="122">
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="79">
         <v>5</v>
       </c>
-      <c r="E50" s="123">
-        <v>4.5</v>
+      <c r="E50" s="84">
+        <v>5</v>
       </c>
       <c r="F50" s="50"/>
       <c r="G50" s="23"/>
@@ -4901,18 +4902,18 @@
       <c r="AY50" s="50"/>
       <c r="AZ50" s="23"/>
       <c r="BA50" s="54"/>
-      <c r="BB50" s="141"/>
-      <c r="BC50" s="142"/>
-      <c r="BD50" s="75" t="s">
+      <c r="BB50" s="72"/>
+      <c r="BC50" s="73"/>
+      <c r="BD50" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="126"/>
-      <c r="B51" s="127"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="95"/>
-      <c r="E51" s="117"/>
+      <c r="A51" s="97"/>
+      <c r="B51" s="98"/>
+      <c r="C51" s="98"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="68"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="48"/>
@@ -4961,20 +4962,20 @@
       <c r="AY51" s="8"/>
       <c r="AZ51" s="9"/>
       <c r="BA51" s="48"/>
-      <c r="BB51" s="141"/>
-      <c r="BC51" s="142"/>
-      <c r="BD51" s="75"/>
+      <c r="BB51" s="72"/>
+      <c r="BC51" s="73"/>
+      <c r="BD51" s="71"/>
     </row>
     <row r="52" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="99"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="85">
+      <c r="B52" s="90"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="65">
         <v>2</v>
       </c>
-      <c r="E52" s="87"/>
+      <c r="E52" s="67"/>
       <c r="F52" s="50"/>
       <c r="G52" s="23"/>
       <c r="H52" s="57"/>
@@ -5015,16 +5016,16 @@
       <c r="AY52" s="50"/>
       <c r="AZ52" s="44"/>
       <c r="BA52" s="23"/>
-      <c r="BB52" s="141"/>
-      <c r="BC52" s="142"/>
-      <c r="BD52" s="75"/>
+      <c r="BB52" s="72"/>
+      <c r="BC52" s="73"/>
+      <c r="BD52" s="71"/>
     </row>
     <row r="53" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="101"/>
-      <c r="B53" s="102"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="84"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="101"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="83"/>
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -5073,20 +5074,20 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="11"/>
-      <c r="BB53" s="141"/>
-      <c r="BC53" s="142"/>
-      <c r="BD53" s="75"/>
+      <c r="BB53" s="72"/>
+      <c r="BC53" s="73"/>
+      <c r="BD53" s="71"/>
     </row>
     <row r="54" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="128" t="s">
+      <c r="A54" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="129"/>
-      <c r="C54" s="130"/>
-      <c r="D54" s="122">
+      <c r="B54" s="103"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="79">
         <v>4.5</v>
       </c>
-      <c r="E54" s="123">
+      <c r="E54" s="84">
         <v>2</v>
       </c>
       <c r="F54" s="50"/>
@@ -5136,16 +5137,16 @@
       <c r="AY54" s="50"/>
       <c r="AZ54" s="23"/>
       <c r="BA54" s="51"/>
-      <c r="BB54" s="141"/>
-      <c r="BC54" s="142"/>
+      <c r="BB54" s="72"/>
+      <c r="BC54" s="73"/>
       <c r="BD54" s="61"/>
     </row>
     <row r="55" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="91"/>
-      <c r="B55" s="92"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="95"/>
-      <c r="E55" s="117"/>
+      <c r="A55" s="92"/>
+      <c r="B55" s="93"/>
+      <c r="C55" s="94"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -5194,16 +5195,16 @@
       <c r="AY55" s="8"/>
       <c r="AZ55" s="9"/>
       <c r="BA55" s="9"/>
-      <c r="BB55" s="141"/>
-      <c r="BC55" s="142"/>
+      <c r="BB55" s="72"/>
+      <c r="BC55" s="73"/>
       <c r="BD55" s="61"/>
     </row>
     <row r="56" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="128"/>
-      <c r="B56" s="129"/>
-      <c r="C56" s="130"/>
-      <c r="D56" s="122"/>
-      <c r="E56" s="123"/>
+      <c r="A56" s="102"/>
+      <c r="B56" s="103"/>
+      <c r="C56" s="104"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="84"/>
       <c r="F56" s="50"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
@@ -5252,16 +5253,16 @@
       <c r="AY56" s="50"/>
       <c r="AZ56" s="23"/>
       <c r="BA56" s="23"/>
-      <c r="BB56" s="141"/>
-      <c r="BC56" s="142"/>
+      <c r="BB56" s="72"/>
+      <c r="BC56" s="73"/>
       <c r="BD56" s="61"/>
     </row>
     <row r="57" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="91"/>
-      <c r="B57" s="92"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="95"/>
-      <c r="E57" s="117"/>
+      <c r="A57" s="92"/>
+      <c r="B57" s="93"/>
+      <c r="C57" s="94"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="68"/>
       <c r="F57" s="2"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -5310,16 +5311,16 @@
       <c r="AY57" s="2"/>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="141"/>
-      <c r="BC57" s="142"/>
+      <c r="BB57" s="72"/>
+      <c r="BC57" s="73"/>
       <c r="BD57" s="61"/>
     </row>
     <row r="58" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="98"/>
-      <c r="B58" s="99"/>
-      <c r="C58" s="100"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="87"/>
+      <c r="A58" s="89"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="91"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="67"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -5368,16 +5369,16 @@
       <c r="AY58" s="8"/>
       <c r="AZ58" s="9"/>
       <c r="BA58" s="9"/>
-      <c r="BB58" s="141"/>
-      <c r="BC58" s="142"/>
+      <c r="BB58" s="72"/>
+      <c r="BC58" s="73"/>
       <c r="BD58" s="61"/>
     </row>
     <row r="59" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="101"/>
-      <c r="B59" s="102"/>
-      <c r="C59" s="103"/>
-      <c r="D59" s="86"/>
-      <c r="E59" s="84"/>
+      <c r="A59" s="99"/>
+      <c r="B59" s="100"/>
+      <c r="C59" s="101"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="83"/>
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -5426,35 +5427,135 @@
       <c r="AY59" s="10"/>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="11"/>
-      <c r="BB59" s="143"/>
-      <c r="BC59" s="144"/>
+      <c r="BB59" s="74"/>
+      <c r="BC59" s="75"/>
       <c r="BD59" s="61"/>
     </row>
     <row r="60" spans="1:56" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="131" t="s">
+      <c r="A60" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="132"/>
-      <c r="C60" s="132"/>
-      <c r="D60" s="118">
+      <c r="B60" s="106"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="85">
         <f>SUM(D4:D59)</f>
         <v>80</v>
       </c>
-      <c r="E60" s="120">
+      <c r="E60" s="87">
         <f>SUM(E4:E59)</f>
-        <v>77</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="61" spans="1:56" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="133"/>
-      <c r="B61" s="134"/>
-      <c r="C61" s="134"/>
-      <c r="D61" s="119"/>
-      <c r="E61" s="121"/>
+      <c r="A61" s="107"/>
+      <c r="B61" s="108"/>
+      <c r="C61" s="108"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="88"/>
     </row>
     <row r="62" spans="1:56" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BD1:BD2"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AT2:AX2"/>
+    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="BD3:BD7"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="AO2:AS2"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AS1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="Z2:AD2"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A20:C21"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="A58:C59"/>
+    <mergeCell ref="A60:C61"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="A42:C43"/>
+    <mergeCell ref="A46:C47"/>
+    <mergeCell ref="A48:C49"/>
+    <mergeCell ref="A44:C45"/>
+    <mergeCell ref="A32:C33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="A36:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="D26:D27"/>
@@ -5479,106 +5580,6 @@
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="A54:C55"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="A58:C59"/>
-    <mergeCell ref="A60:C61"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A46:C47"/>
-    <mergeCell ref="A48:C49"/>
-    <mergeCell ref="A44:C45"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="A36:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A20:C21"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="AO2:AS2"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BF7:BF8"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BG7:BG8"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BD1:BD2"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="AT2:AX2"/>
-    <mergeCell ref="AY2:BC2"/>
-    <mergeCell ref="BD3:BD7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="3" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>